<commit_message>
Removed two fuses, as per the final version
</commit_message>
<xml_diff>
--- a/AQN-BOM.xlsx
+++ b/AQN-BOM.xlsx
@@ -711,9 +711,6 @@
     <t>D4, D5, D6, D8, D9, D13, D14, D22</t>
   </si>
   <si>
-    <t>F2, F5, F6, F9, F10, F15, F16, F19, F20, F26, F27, F28, F29, F40, F41, F42, F43, F46, F47, F48, F49, F50, F51, F54, F55, F56, F57, F59, F60, F62, F74, F75, F76, F78, F79, F82, F83</t>
-  </si>
-  <si>
     <t>I2C_1, I2C_2, I2C_3, I2C_4, I2C_6, I2C_7, I2C_8, I2C_9, I_UART_HUB_1, LOPY_I2C, LOPY_UART0, LOPY_UART1, PI_RS_485, PI_UART, PI_UART_HUB_2, PI_UART_HUB_3</t>
   </si>
   <si>
@@ -754,6 +751,9 @@
   </si>
   <si>
     <t>USB1</t>
+  </si>
+  <si>
+    <t>F2, F5, F6, F9, F10, F15, F16, F19, F20, F26, F27, F28, F29, F40, F41, F42, F43, F46, F47, F48, F49, F50, F51, F54, F55, F56, F57, F59, F60, F62, F76, F78, F79, F82, F83</t>
   </si>
 </sst>
 </file>
@@ -1604,7 +1604,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1699,19 +1699,19 @@
         <v>0.01</v>
       </c>
       <c r="M2" s="7">
-        <f>L2*$K$67</f>
+        <f t="shared" ref="M2:M14" si="0">L2*$K$67</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N2" s="8">
-        <f t="shared" ref="N2:N30" si="0">PRODUCT(M2,C2)</f>
+        <f t="shared" ref="N2:N30" si="1">PRODUCT(M2,C2)</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="O2">
-        <f>ROUNDUP(ROUNDUP((C2*$K$65*(1+$K$66)),0)/K2,0)*K2</f>
+        <f t="shared" ref="O2:O30" si="2">ROUNDUP(ROUNDUP((C2*$K$65*(1+$K$66)),0)/K2,0)*K2</f>
         <v>6</v>
       </c>
       <c r="P2" s="8">
-        <f t="shared" ref="P2:P30" si="1">O2*M2</f>
+        <f t="shared" ref="P2:P30" si="3">O2*M2</f>
         <v>4.6200000000000005E-2</v>
       </c>
     </row>
@@ -1726,7 +1726,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D63" si="2">LEN(A3)-LEN(SUBSTITUTE(A3,",",""))+1</f>
+        <f t="shared" ref="D3:D63" si="4">LEN(A3)-LEN(SUBSTITUTE(A3,",",""))+1</f>
         <v>2</v>
       </c>
       <c r="E3" t="s">
@@ -1742,19 +1742,19 @@
         <v>0.01</v>
       </c>
       <c r="M3" s="7">
-        <f>L3*$K$67</f>
+        <f t="shared" si="0"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N3" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.54E-2</v>
       </c>
       <c r="O3">
-        <f>ROUNDUP(ROUNDUP((C3*$K$65*(1+$K$66)),0)/K3,0)*K3</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="P3" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.4699999999999998E-2</v>
       </c>
     </row>
@@ -1769,7 +1769,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="E4" t="s">
@@ -1785,19 +1785,19 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="M4" s="7">
-        <f>L4*$K$67</f>
+        <f t="shared" si="0"/>
         <v>3.1570000000000001E-2</v>
       </c>
       <c r="N4" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.12628</v>
       </c>
       <c r="O4">
-        <f>ROUNDUP(ROUNDUP((C4*$K$65*(1+$K$66)),0)/K4,0)*K4</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="P4" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.66297000000000006</v>
       </c>
     </row>
@@ -1812,7 +1812,7 @@
         <v>25</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
       <c r="E5" t="s">
@@ -1828,19 +1828,19 @@
         <v>0.01</v>
       </c>
       <c r="M5" s="7">
-        <f>L5*$K$67</f>
+        <f t="shared" si="0"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N5" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1925</v>
       </c>
       <c r="O5">
-        <f>ROUNDUP(ROUNDUP((C5*$K$65*(1+$K$66)),0)/K5,0)*K5</f>
+        <f t="shared" si="2"/>
         <v>126</v>
       </c>
       <c r="P5" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.97020000000000006</v>
       </c>
     </row>
@@ -1855,7 +1855,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E6" t="s">
@@ -1871,19 +1871,19 @@
         <v>0.01</v>
       </c>
       <c r="M6" s="7">
-        <f>L6*$K$67</f>
-        <v>7.7000000000000002E-3</v>
-      </c>
-      <c r="N6" s="8">
         <f t="shared" si="0"/>
         <v>7.7000000000000002E-3</v>
       </c>
+      <c r="N6" s="8">
+        <f t="shared" si="1"/>
+        <v>7.7000000000000002E-3</v>
+      </c>
       <c r="O6">
-        <f>ROUNDUP(ROUNDUP((C6*$K$65*(1+$K$66)),0)/K6,0)*K6</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="P6" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.6200000000000005E-2</v>
       </c>
     </row>
@@ -1898,7 +1898,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="E7" t="s">
@@ -1914,19 +1914,19 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="M7" s="7">
-        <f>L7*$K$67</f>
+        <f t="shared" si="0"/>
         <v>3.696E-2</v>
       </c>
       <c r="N7" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.392E-2</v>
       </c>
       <c r="O7">
-        <f>ROUNDUP(ROUNDUP((C7*$K$65*(1+$K$66)),0)/K7,0)*K7</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="P7" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.40655999999999998</v>
       </c>
     </row>
@@ -1941,7 +1941,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E8" t="s">
@@ -1957,19 +1957,19 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="M8" s="7">
-        <f>L8*$K$67</f>
-        <v>1.155E-2</v>
-      </c>
-      <c r="N8" s="8">
         <f t="shared" si="0"/>
         <v>1.155E-2</v>
       </c>
+      <c r="N8" s="8">
+        <f t="shared" si="1"/>
+        <v>1.155E-2</v>
+      </c>
       <c r="O8">
-        <f>ROUNDUP(ROUNDUP((C8*$K$65*(1+$K$66)),0)/K8,0)*K8</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="P8" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.93E-2</v>
       </c>
     </row>
@@ -1984,7 +1984,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="E9" t="s">
@@ -2000,19 +2000,19 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="M9" s="7">
-        <f>L9*$K$67</f>
+        <f t="shared" si="0"/>
         <v>3.1570000000000001E-2</v>
       </c>
       <c r="N9" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.12628</v>
       </c>
       <c r="O9">
-        <f>ROUNDUP(ROUNDUP((C9*$K$65*(1+$K$66)),0)/K9,0)*K9</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="P9" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.66297000000000006</v>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E10" t="s">
@@ -2043,19 +2043,19 @@
         <v>0.104</v>
       </c>
       <c r="M10" s="7">
-        <f>L10*$K$67</f>
-        <v>8.0079999999999998E-2</v>
-      </c>
-      <c r="N10" s="8">
         <f t="shared" si="0"/>
         <v>8.0079999999999998E-2</v>
       </c>
+      <c r="N10" s="8">
+        <f t="shared" si="1"/>
+        <v>8.0079999999999998E-2</v>
+      </c>
       <c r="O10">
-        <f>ROUNDUP(ROUNDUP((C10*$K$65*(1+$K$66)),0)/K10,0)*K10</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="P10" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.48048000000000002</v>
       </c>
     </row>
@@ -2070,7 +2070,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E11" t="s">
@@ -2086,19 +2086,19 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="M11" s="7">
-        <f>L11*$K$67</f>
-        <v>3.696E-2</v>
-      </c>
-      <c r="N11" s="8">
         <f t="shared" si="0"/>
         <v>3.696E-2</v>
       </c>
+      <c r="N11" s="8">
+        <f t="shared" si="1"/>
+        <v>3.696E-2</v>
+      </c>
       <c r="O11">
-        <f>ROUNDUP(ROUNDUP((C11*$K$65*(1+$K$66)),0)/K11,0)*K11</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="P11" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.22176000000000001</v>
       </c>
     </row>
@@ -2113,7 +2113,7 @@
         <v>5</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="E12" t="s">
@@ -2129,19 +2129,19 @@
         <v>1.4E-2</v>
       </c>
       <c r="M12" s="7">
-        <f>L12*$K$67</f>
+        <f t="shared" si="0"/>
         <v>1.078E-2</v>
       </c>
       <c r="N12" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.3899999999999997E-2</v>
       </c>
       <c r="O12">
-        <f>ROUNDUP(ROUNDUP((C12*$K$65*(1+$K$66)),0)/K12,0)*K12</f>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="P12" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.28027999999999997</v>
       </c>
     </row>
@@ -2156,7 +2156,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="E13" t="s">
@@ -2172,19 +2172,19 @@
         <v>1.4E-2</v>
       </c>
       <c r="M13" s="7">
-        <f>L13*$K$67</f>
+        <f t="shared" si="0"/>
         <v>1.078E-2</v>
       </c>
       <c r="N13" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.3119999999999999E-2</v>
       </c>
       <c r="O13">
-        <f>ROUNDUP(ROUNDUP((C13*$K$65*(1+$K$66)),0)/K13,0)*K13</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="P13" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.22638</v>
       </c>
     </row>
@@ -2199,7 +2199,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="E14" t="s">
@@ -2215,19 +2215,19 @@
         <v>1.4E-2</v>
       </c>
       <c r="M14" s="7">
-        <f>L14*$K$67</f>
+        <f t="shared" si="0"/>
         <v>1.078E-2</v>
       </c>
       <c r="N14" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.6239999999999997E-2</v>
       </c>
       <c r="O14">
-        <f>ROUNDUP(ROUNDUP((C14*$K$65*(1+$K$66)),0)/K14,0)*K14</f>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="P14" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.44197999999999998</v>
       </c>
     </row>
@@ -2239,7 +2239,7 @@
         <v>4</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
@@ -2259,15 +2259,15 @@
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="N15" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.20799999999999999</v>
       </c>
       <c r="O15">
-        <f>ROUNDUP(ROUNDUP((C15*$K$65*(1+$K$66)),0)/K15,0)*K15</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="P15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.0919999999999999</v>
       </c>
     </row>
@@ -2280,7 +2280,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G16">
@@ -2297,31 +2297,31 @@
         <v>7.5459999999999999E-2</v>
       </c>
       <c r="N16" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.5459999999999999E-2</v>
       </c>
       <c r="O16">
-        <f>ROUNDUP(ROUNDUP((C16*$K$65*(1+$K$66)),0)/K16,0)*K16</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="P16" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.45276</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>105</v>
       </c>
       <c r="C17">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="2"/>
-        <v>37</v>
+        <f t="shared" si="4"/>
+        <v>35</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>104</v>
@@ -2337,16 +2337,16 @@
         <v>3.619E-2</v>
       </c>
       <c r="N17" s="8">
-        <f t="shared" si="0"/>
-        <v>1.3390299999999999</v>
+        <f t="shared" si="1"/>
+        <v>1.2666500000000001</v>
       </c>
       <c r="O17">
-        <f>ROUNDUP(ROUNDUP((C17*$K$65*(1+$K$66)),0)/K17,0)*K17</f>
-        <v>186</v>
+        <f t="shared" si="2"/>
+        <v>176</v>
       </c>
       <c r="P17" s="8">
-        <f t="shared" si="1"/>
-        <v>6.7313400000000003</v>
+        <f t="shared" si="3"/>
+        <v>6.36944</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -2358,7 +2358,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="I18" t="s">
@@ -2369,28 +2369,28 @@
         <v>0</v>
       </c>
       <c r="N18" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O18" t="e">
-        <f>ROUNDUP(ROUNDUP((C18*$K$65*(1+$K$66)),0)/K18,0)*K18</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P18" s="8" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19">
         <v>16</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="F19" s="3" t="s">
@@ -2407,15 +2407,15 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="N19" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.6560000000000001</v>
       </c>
       <c r="O19">
-        <f>ROUNDUP(ROUNDUP((C19*$K$65*(1+$K$66)),0)/K19,0)*K19</f>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="P19" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>14.110000000000001</v>
       </c>
     </row>
@@ -2430,7 +2430,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E20" t="s">
@@ -2450,15 +2450,15 @@
         <v>7.0069999999999993E-2</v>
       </c>
       <c r="N20" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.0069999999999993E-2</v>
       </c>
       <c r="O20">
-        <f>ROUNDUP(ROUNDUP((C20*$K$65*(1+$K$66)),0)/K20,0)*K20</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="P20" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.42041999999999996</v>
       </c>
     </row>
@@ -2473,7 +2473,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E21" t="s">
@@ -2490,15 +2490,15 @@
         <v>8.3930000000000005E-2</v>
       </c>
       <c r="N21" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.3930000000000005E-2</v>
       </c>
       <c r="O21">
-        <f>ROUNDUP(ROUNDUP((C21*$K$65*(1+$K$66)),0)/K21,0)*K21</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="P21" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.50358000000000003</v>
       </c>
     </row>
@@ -2513,7 +2513,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="E22" t="s">
@@ -2533,15 +2533,15 @@
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N22" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.54E-2</v>
       </c>
       <c r="O22">
-        <f>ROUNDUP(ROUNDUP((C22*$K$65*(1+$K$66)),0)/K22,0)*K22</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="P22" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.4699999999999998E-2</v>
       </c>
     </row>
@@ -2556,7 +2556,7 @@
         <v>6</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="E23" t="s">
@@ -2576,21 +2576,21 @@
         <v>1.9250000000000003E-2</v>
       </c>
       <c r="N23" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.11550000000000002</v>
       </c>
       <c r="O23">
-        <f>ROUNDUP(ROUNDUP((C23*$K$65*(1+$K$66)),0)/K23,0)*K23</f>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="P23" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.59675000000000011</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>64</v>
@@ -2599,7 +2599,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="E24" t="s">
@@ -2619,15 +2619,15 @@
         <v>1.155E-2</v>
       </c>
       <c r="N24" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.465E-2</v>
       </c>
       <c r="O24">
-        <f>ROUNDUP(ROUNDUP((C24*$K$65*(1+$K$66)),0)/K24,0)*K24</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="P24" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.18479999999999999</v>
       </c>
     </row>
@@ -2639,7 +2639,7 @@
         <v>2</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F25" s="3" t="s">
@@ -2659,28 +2659,28 @@
         <v>1.41</v>
       </c>
       <c r="N25" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.82</v>
       </c>
       <c r="O25">
-        <f>ROUNDUP(ROUNDUP((C25*$K$65*(1+$K$66)),0)/K25,0)*K25</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="P25" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>15.51</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26">
         <v>9</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="F26" s="3" t="s">
@@ -2697,15 +2697,15 @@
         <v>0.23599999999999999</v>
       </c>
       <c r="N26" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.1239999999999997</v>
       </c>
       <c r="O26">
-        <f>ROUNDUP(ROUNDUP((C26*$K$65*(1+$K$66)),0)/K26,0)*K26</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="P26" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11.799999999999999</v>
       </c>
     </row>
@@ -2718,7 +2718,7 @@
         <v>1</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F27" s="3" t="s">
@@ -2740,15 +2740,15 @@
         <v>32.509399999999999</v>
       </c>
       <c r="N27" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32.509399999999999</v>
       </c>
       <c r="O27">
-        <f>ROUNDUP(ROUNDUP((C27*$K$65*(1+$K$66)),0)/K27,0)*K27</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="P27" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>195.0564</v>
       </c>
     </row>
@@ -2763,7 +2763,7 @@
         <v>1</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G28" s="3">
@@ -2779,15 +2779,15 @@
         <v>0.27900000000000003</v>
       </c>
       <c r="N28" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.27900000000000003</v>
       </c>
       <c r="O28">
-        <f>ROUNDUP(ROUNDUP((C28*$K$65*(1+$K$66)),0)/K28,0)*K28</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="P28" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.79</v>
       </c>
       <c r="S28">
@@ -2806,7 +2806,7 @@
         <v>2</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="E29" t="s">
@@ -2826,15 +2826,15 @@
         <v>0.10472000000000001</v>
       </c>
       <c r="N29" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.20944000000000002</v>
       </c>
       <c r="O29">
-        <f>ROUNDUP(ROUNDUP((C29*$K$65*(1+$K$66)),0)/K29,0)*K29</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="P29" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.1519200000000001</v>
       </c>
     </row>
@@ -2849,7 +2849,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="E30" t="s">
@@ -2869,15 +2869,15 @@
         <v>2.5410000000000002E-2</v>
       </c>
       <c r="N30" s="8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5410000000000002E-2</v>
       </c>
       <c r="O30">
-        <f>ROUNDUP(ROUNDUP((C30*$K$65*(1+$K$66)),0)/K30,0)*K30</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="P30" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.15246000000000001</v>
       </c>
     </row>
@@ -2886,13 +2886,13 @@
         <v>203</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E31" t="s">
@@ -2909,13 +2909,13 @@
         <v>211</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="E32" t="s">
@@ -2929,7 +2929,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>62</v>
@@ -2938,7 +2938,7 @@
         <v>10</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="E33" t="s">
@@ -2954,19 +2954,19 @@
         <v>0.01</v>
       </c>
       <c r="M33" s="7">
-        <f>L33*$K$67</f>
+        <f t="shared" ref="M33:M42" si="5">L33*$K$67</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N33" s="8">
-        <f t="shared" ref="N33:N42" si="3">PRODUCT(M33,C33)</f>
+        <f t="shared" ref="N33:N42" si="6">PRODUCT(M33,C33)</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="O33">
-        <f>ROUNDUP(ROUNDUP((C33*$K$65*(1+$K$66)),0)/K33,0)*K33</f>
+        <f t="shared" ref="O33:O42" si="7">ROUNDUP(ROUNDUP((C33*$K$65*(1+$K$66)),0)/K33,0)*K33</f>
         <v>51</v>
       </c>
       <c r="P33" s="8">
-        <f t="shared" ref="P33:P42" si="4">O33*M33</f>
+        <f t="shared" ref="P33:P42" si="8">O33*M33</f>
         <v>0.39269999999999999</v>
       </c>
     </row>
@@ -2981,7 +2981,7 @@
         <v>6</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="E34" t="s">
@@ -2997,25 +2997,25 @@
         <v>0.01</v>
       </c>
       <c r="M34" s="7">
-        <f>L34*$K$67</f>
+        <f t="shared" si="5"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N34" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4.6200000000000005E-2</v>
       </c>
       <c r="O34">
-        <f>ROUNDUP(ROUNDUP((C34*$K$65*(1+$K$66)),0)/K34,0)*K34</f>
+        <f t="shared" si="7"/>
         <v>31</v>
       </c>
       <c r="P34" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.2387</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>5</v>
@@ -3024,7 +3024,7 @@
         <v>5</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="E35" t="s">
@@ -3040,19 +3040,19 @@
         <v>0.01</v>
       </c>
       <c r="M35" s="7">
-        <f>L35*$K$67</f>
+        <f t="shared" si="5"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N35" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3.85E-2</v>
       </c>
       <c r="O35">
-        <f>ROUNDUP(ROUNDUP((C35*$K$65*(1+$K$66)),0)/K35,0)*K35</f>
+        <f t="shared" si="7"/>
         <v>26</v>
       </c>
       <c r="P35" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.20020000000000002</v>
       </c>
     </row>
@@ -3067,7 +3067,7 @@
         <v>1</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E36" t="s">
@@ -3083,19 +3083,19 @@
         <v>0.01</v>
       </c>
       <c r="M36" s="7">
-        <f>L36*$K$67</f>
+        <f t="shared" si="5"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N36" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="O36">
-        <f>ROUNDUP(ROUNDUP((C36*$K$65*(1+$K$66)),0)/K36,0)*K36</f>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="P36" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4.6200000000000005E-2</v>
       </c>
     </row>
@@ -3110,7 +3110,7 @@
         <v>1</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E37" t="s">
@@ -3126,19 +3126,19 @@
         <v>0.01</v>
       </c>
       <c r="M37" s="7">
-        <f>L37*$K$67</f>
+        <f t="shared" si="5"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N37" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="O37">
-        <f>ROUNDUP(ROUNDUP((C37*$K$65*(1+$K$66)),0)/K37,0)*K37</f>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="P37" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4.6200000000000005E-2</v>
       </c>
     </row>
@@ -3153,7 +3153,7 @@
         <v>2</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="E38" t="s">
@@ -3169,19 +3169,19 @@
         <v>0.01</v>
       </c>
       <c r="M38" s="7">
-        <f>L38*$K$67</f>
+        <f t="shared" si="5"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N38" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.54E-2</v>
       </c>
       <c r="O38">
-        <f>ROUNDUP(ROUNDUP((C38*$K$65*(1+$K$66)),0)/K38,0)*K38</f>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="P38" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8.4699999999999998E-2</v>
       </c>
     </row>
@@ -3196,7 +3196,7 @@
         <v>2</v>
       </c>
       <c r="D39" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="E39" t="s">
@@ -3212,19 +3212,19 @@
         <v>0.01</v>
       </c>
       <c r="M39" s="7">
-        <f>L39*$K$67</f>
+        <f t="shared" si="5"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N39" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>1.54E-2</v>
       </c>
       <c r="O39">
-        <f>ROUNDUP(ROUNDUP((C39*$K$65*(1+$K$66)),0)/K39,0)*K39</f>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="P39" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8.4699999999999998E-2</v>
       </c>
     </row>
@@ -3239,7 +3239,7 @@
         <v>3</v>
       </c>
       <c r="D40" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="E40" t="s">
@@ -3255,25 +3255,25 @@
         <v>0.01</v>
       </c>
       <c r="M40" s="7">
-        <f>L40*$K$67</f>
+        <f t="shared" si="5"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N40" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.3100000000000002E-2</v>
       </c>
       <c r="O40">
-        <f>ROUNDUP(ROUNDUP((C40*$K$65*(1+$K$66)),0)/K40,0)*K40</f>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
       <c r="P40" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.1232</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>41</v>
@@ -3282,7 +3282,7 @@
         <v>3</v>
       </c>
       <c r="D41" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="E41" t="s">
@@ -3298,19 +3298,19 @@
         <v>0.01</v>
       </c>
       <c r="M41" s="7">
-        <f>L41*$K$67</f>
+        <f t="shared" si="5"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N41" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.3100000000000002E-2</v>
       </c>
       <c r="O41">
-        <f>ROUNDUP(ROUNDUP((C41*$K$65*(1+$K$66)),0)/K41,0)*K41</f>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
       <c r="P41" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.1232</v>
       </c>
     </row>
@@ -3325,7 +3325,7 @@
         <v>3</v>
       </c>
       <c r="D42" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="E42" t="s">
@@ -3341,19 +3341,19 @@
         <v>0.01</v>
       </c>
       <c r="M42" s="7">
-        <f>L42*$K$67</f>
+        <f t="shared" si="5"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N42" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>2.3100000000000002E-2</v>
       </c>
       <c r="O42">
-        <f>ROUNDUP(ROUNDUP((C42*$K$65*(1+$K$66)),0)/K42,0)*K42</f>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
       <c r="P42" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.1232</v>
       </c>
     </row>
@@ -3366,14 +3366,14 @@
         <v>1</v>
       </c>
       <c r="D43" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E43" t="s">
         <v>222</v>
       </c>
       <c r="F43" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G43">
         <v>9238379</v>
@@ -3389,10 +3389,10 @@
         <v>214</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D44" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J44" s="1"/>
@@ -3409,7 +3409,7 @@
         <v>1</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F45" s="3" t="s">
@@ -3429,30 +3429,30 @@
         <v>5.39</v>
       </c>
       <c r="N45" s="8">
-        <f t="shared" ref="N45:N64" si="5">PRODUCT(M45,C45)</f>
+        <f t="shared" ref="N45:N64" si="9">PRODUCT(M45,C45)</f>
         <v>5.39</v>
       </c>
       <c r="O45">
-        <f t="shared" ref="O45:O64" si="6">ROUNDUP(ROUNDUP((C45*$K$65*(1+$K$66)),0)/K45,0)*K45</f>
+        <f t="shared" ref="O45:O64" si="10">ROUNDUP(ROUNDUP((C45*$K$65*(1+$K$66)),0)/K45,0)*K45</f>
         <v>6</v>
       </c>
       <c r="P45" s="8">
-        <f t="shared" ref="P45:P64" si="7">O45*M45</f>
+        <f t="shared" ref="P45:P64" si="11">O45*M45</f>
         <v>32.339999999999996</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="C46">
         <v>4</v>
       </c>
       <c r="D46" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="J46" s="1"/>
@@ -3464,15 +3464,15 @@
         <v>0</v>
       </c>
       <c r="N46" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>21</v>
       </c>
       <c r="P46" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3485,7 +3485,7 @@
         <v>17</v>
       </c>
       <c r="D47" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="I47" t="s">
@@ -3496,15 +3496,15 @@
         <v>0</v>
       </c>
       <c r="N47" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O47" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P47" s="8" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3519,7 +3519,7 @@
         <v>2</v>
       </c>
       <c r="D48" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="F48" s="3" t="s">
@@ -3539,15 +3539,15 @@
         <v>3.41</v>
       </c>
       <c r="N48" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>6.82</v>
       </c>
       <c r="O48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>11</v>
       </c>
       <c r="P48" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>37.510000000000005</v>
       </c>
     </row>
@@ -3562,7 +3562,7 @@
         <v>1</v>
       </c>
       <c r="D49" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F49" s="3" t="s">
@@ -3579,15 +3579,15 @@
         <v>0.36199999999999999</v>
       </c>
       <c r="N49" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.36199999999999999</v>
       </c>
       <c r="O49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="P49" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.62</v>
       </c>
     </row>
@@ -3602,7 +3602,7 @@
         <v>1</v>
       </c>
       <c r="D50" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F50" s="3" t="s">
@@ -3619,15 +3619,15 @@
         <v>2.85</v>
       </c>
       <c r="N50" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2.85</v>
       </c>
       <c r="O50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="P50" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>17.100000000000001</v>
       </c>
     </row>
@@ -3642,7 +3642,7 @@
         <v>1</v>
       </c>
       <c r="D51" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F51" s="3" t="s">
@@ -3657,15 +3657,15 @@
         <v>2.09</v>
       </c>
       <c r="N51" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2.09</v>
       </c>
       <c r="O51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="P51" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>12.54</v>
       </c>
     </row>
@@ -3680,7 +3680,7 @@
         <v>1</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F52" s="3" t="s">
@@ -3702,15 +3702,15 @@
         <v>0.37191000000000002</v>
       </c>
       <c r="N52" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.37191000000000002</v>
       </c>
       <c r="O52">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="P52" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.7191000000000001</v>
       </c>
     </row>
@@ -3723,7 +3723,7 @@
         <v>1</v>
       </c>
       <c r="D53" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E53" t="s">
@@ -3748,15 +3748,15 @@
         <v>7.6614999999999993</v>
       </c>
       <c r="N53" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7.6614999999999993</v>
       </c>
       <c r="O53">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="P53" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>45.968999999999994</v>
       </c>
     </row>
@@ -3771,7 +3771,7 @@
         <v>1</v>
       </c>
       <c r="D54" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F54" s="3" t="s">
@@ -3791,15 +3791,15 @@
         <v>1</v>
       </c>
       <c r="N54" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="P54" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
     </row>
@@ -3814,7 +3814,7 @@
         <v>1</v>
       </c>
       <c r="D55" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F55" s="3" t="s">
@@ -3833,15 +3833,15 @@
         <v>0.28599999999999998</v>
       </c>
       <c r="N55" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.28599999999999998</v>
       </c>
       <c r="O55">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="P55" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.7159999999999997</v>
       </c>
     </row>
@@ -3856,7 +3856,7 @@
         <v>1</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E56" t="s">
@@ -3878,15 +3878,15 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N56" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="O56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="P56" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.44999999999999996</v>
       </c>
     </row>
@@ -3901,7 +3901,7 @@
         <v>1</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F57" s="3" t="s">
@@ -3921,15 +3921,15 @@
         <v>1.46</v>
       </c>
       <c r="N57" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.46</v>
       </c>
       <c r="O57">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="P57" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>8.76</v>
       </c>
     </row>
@@ -3944,7 +3944,7 @@
         <v>1</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E58" t="s">
@@ -3967,15 +3967,15 @@
         <v>0.873</v>
       </c>
       <c r="N58" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.873</v>
       </c>
       <c r="O58">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="P58" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>5.2379999999999995</v>
       </c>
     </row>
@@ -3987,7 +3987,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F59" s="3" t="s">
@@ -4005,15 +4005,15 @@
         <v>26.3</v>
       </c>
       <c r="N59" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>26.3</v>
       </c>
       <c r="O59">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="P59" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>157.80000000000001</v>
       </c>
     </row>
@@ -4028,7 +4028,7 @@
         <v>1</v>
       </c>
       <c r="D60" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F60" s="3" t="s">
@@ -4047,21 +4047,21 @@
         <v>1.5</v>
       </c>
       <c r="N60" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.5</v>
       </c>
       <c r="O60">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="P60" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>84</v>
@@ -4070,7 +4070,7 @@
         <v>4</v>
       </c>
       <c r="D61" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="E61" t="s">
@@ -4090,15 +4090,15 @@
         <v>2.4100999999999999</v>
       </c>
       <c r="N61" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9.6403999999999996</v>
       </c>
       <c r="O61">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>21</v>
       </c>
       <c r="P61" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>50.612099999999998</v>
       </c>
     </row>
@@ -4113,7 +4113,7 @@
         <v>1</v>
       </c>
       <c r="D62" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F62" s="4" t="s">
@@ -4132,21 +4132,21 @@
         <v>0.68700000000000006</v>
       </c>
       <c r="N62" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.68700000000000006</v>
       </c>
       <c r="O62">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="P62" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4.1219999999999999</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>117</v>
@@ -4155,7 +4155,7 @@
         <v>1</v>
       </c>
       <c r="D63" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J63" s="1" t="s">
@@ -4172,15 +4172,15 @@
         <v>9.0090000000000003E-2</v>
       </c>
       <c r="N63" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9.0090000000000003E-2</v>
       </c>
       <c r="O63">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="P63" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.54054000000000002</v>
       </c>
     </row>
@@ -4195,7 +4195,7 @@
         <v>1</v>
       </c>
       <c r="D64" s="1">
-        <f t="shared" ref="D64" si="8">LEN(A64)-LEN(SUBSTITUTE(A64,",",""))+1</f>
+        <f t="shared" ref="D64" si="12">LEN(A64)-LEN(SUBSTITUTE(A64,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="J64" s="1" t="s">
@@ -4212,15 +4212,15 @@
         <v>0.15400000000000003</v>
       </c>
       <c r="N64" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.15400000000000003</v>
       </c>
       <c r="O64">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="P64" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.92400000000000015</v>
       </c>
     </row>
@@ -4236,7 +4236,7 @@
       </c>
       <c r="N65" s="8">
         <f>SUM(N2:N62)</f>
-        <v>111.04093</v>
+        <v>110.96854999999999</v>
       </c>
       <c r="O65" s="6" t="s">
         <v>163</v>

</xml_diff>

<commit_message>
Added missing pricing information
</commit_message>
<xml_diff>
--- a/AQN-BOM.xlsx
+++ b/AQN-BOM.xlsx
@@ -444,9 +444,6 @@
     <t>DHT22 temp/humidity sensor - maybe you have this?</t>
   </si>
   <si>
-    <t>Cannot find better sources - Ask Steven</t>
-  </si>
-  <si>
     <t>http://www.amazon.co.uk/LM2596-Step-down-Adjustable-Supply-Module/dp/B008RE3YOA</t>
   </si>
   <si>
@@ -754,6 +751,9 @@
   </si>
   <si>
     <t>F2, F5, F6, F9, F10, F15, F16, F19, F20, F26, F27, F28, F29, F40, F41, F42, F43, F46, F47, F48, F49, F50, F51, F54, F55, F56, F57, F59, F60, F62, F76, F78, F79, F82, F83</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1253,10 +1253,9 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1"/>
@@ -1601,15 +1600,15 @@
   <dimension ref="A1:S84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="P47" sqref="P47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="99.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="41" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -1617,8 +1616,8 @@
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="26" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10" style="5" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="5" customWidth="1"/>
+    <col min="12" max="12" width="10" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="4" customWidth="1"/>
     <col min="14" max="14" width="9.42578125" customWidth="1"/>
     <col min="15" max="15" width="14.140625" customWidth="1"/>
     <col min="16" max="16" width="17" customWidth="1"/>
@@ -1636,7 +1635,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -1645,10 +1644,10 @@
         <v>121</v>
       </c>
       <c r="G1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H1" t="s">
         <v>164</v>
-      </c>
-      <c r="H1" t="s">
-        <v>165</v>
       </c>
       <c r="I1" t="s">
         <v>122</v>
@@ -1657,25 +1656,25 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="L1" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="N1" t="s">
         <v>142</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="N1" t="s">
-        <v>143</v>
-      </c>
       <c r="O1" t="s">
+        <v>159</v>
+      </c>
+      <c r="P1" t="s">
         <v>160</v>
       </c>
-      <c r="P1" t="s">
-        <v>161</v>
-      </c>
       <c r="Q1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -1692,17 +1691,17 @@
         <f>LEN(A2)-LEN(SUBSTITUTE(A2,",",""))+1</f>
         <v>1</v>
       </c>
-      <c r="K2" s="9">
-        <v>1</v>
-      </c>
-      <c r="L2" s="5">
+      <c r="K2" s="8">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4">
         <v>0.01</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="6">
         <f t="shared" ref="M2:M14" si="0">L2*$K$67</f>
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="7">
         <f t="shared" ref="N2:N30" si="1">PRODUCT(M2,C2)</f>
         <v>7.7000000000000002E-3</v>
       </c>
@@ -1710,7 +1709,7 @@
         <f t="shared" ref="O2:O30" si="2">ROUNDUP(ROUNDUP((C2*$K$65*(1+$K$66)),0)/K2,0)*K2</f>
         <v>6</v>
       </c>
-      <c r="P2" s="8">
+      <c r="P2" s="7">
         <f t="shared" ref="P2:P30" si="3">O2*M2</f>
         <v>4.6200000000000005E-2</v>
       </c>
@@ -1735,17 +1734,17 @@
       <c r="J3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="9">
-        <v>1</v>
-      </c>
-      <c r="L3" s="5">
+      <c r="K3" s="8">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4">
         <v>0.01</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="6">
         <f t="shared" si="0"/>
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="7">
         <f t="shared" si="1"/>
         <v>1.54E-2</v>
       </c>
@@ -1753,14 +1752,14 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="P3" s="8">
+      <c r="P3" s="7">
         <f t="shared" si="3"/>
         <v>8.4699999999999998E-2</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>66</v>
@@ -1773,22 +1772,22 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="K4" s="9">
-        <v>1</v>
-      </c>
-      <c r="L4" s="5">
+      <c r="K4" s="8">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="6">
         <f t="shared" si="0"/>
         <v>3.1570000000000001E-2</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="7">
         <f t="shared" si="1"/>
         <v>0.12628</v>
       </c>
@@ -1796,14 +1795,14 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="P4" s="8">
+      <c r="P4" s="7">
         <f t="shared" si="3"/>
         <v>0.66297000000000006</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
@@ -1816,22 +1815,22 @@
         <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="9">
-        <v>1</v>
-      </c>
-      <c r="L5" s="5">
+      <c r="K5" s="8">
+        <v>1</v>
+      </c>
+      <c r="L5" s="4">
         <v>0.01</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="6">
         <f t="shared" si="0"/>
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="7">
         <f t="shared" si="1"/>
         <v>0.1925</v>
       </c>
@@ -1839,7 +1838,7 @@
         <f t="shared" si="2"/>
         <v>126</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5" s="7">
         <f t="shared" si="3"/>
         <v>0.97020000000000006</v>
       </c>
@@ -1859,22 +1858,22 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="9">
-        <v>1</v>
-      </c>
-      <c r="L6" s="5">
+      <c r="K6" s="8">
+        <v>1</v>
+      </c>
+      <c r="L6" s="4">
         <v>0.01</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="6">
         <f t="shared" si="0"/>
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="7">
         <f t="shared" si="1"/>
         <v>7.7000000000000002E-3</v>
       </c>
@@ -1882,7 +1881,7 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6" s="7">
         <f t="shared" si="3"/>
         <v>4.6200000000000005E-2</v>
       </c>
@@ -1902,22 +1901,22 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="9">
-        <v>1</v>
-      </c>
-      <c r="L7" s="5">
+      <c r="K7" s="8">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="6">
         <f t="shared" si="0"/>
         <v>3.696E-2</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="7">
         <f t="shared" si="1"/>
         <v>7.392E-2</v>
       </c>
@@ -1925,7 +1924,7 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="P7" s="8">
+      <c r="P7" s="7">
         <f t="shared" si="3"/>
         <v>0.40655999999999998</v>
       </c>
@@ -1945,22 +1944,22 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="9">
-        <v>1</v>
-      </c>
-      <c r="L8" s="5">
+      <c r="K8" s="8">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="6">
         <f t="shared" si="0"/>
         <v>1.155E-2</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="7">
         <f t="shared" si="1"/>
         <v>1.155E-2</v>
       </c>
@@ -1968,7 +1967,7 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="P8" s="8">
+      <c r="P8" s="7">
         <f t="shared" si="3"/>
         <v>6.93E-2</v>
       </c>
@@ -1988,22 +1987,22 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K9" s="9">
-        <v>1</v>
-      </c>
-      <c r="L9" s="5">
+      <c r="K9" s="8">
+        <v>1</v>
+      </c>
+      <c r="L9" s="4">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="6">
         <f t="shared" si="0"/>
         <v>3.1570000000000001E-2</v>
       </c>
-      <c r="N9" s="8">
+      <c r="N9" s="7">
         <f t="shared" si="1"/>
         <v>0.12628</v>
       </c>
@@ -2011,7 +2010,7 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="P9" s="8">
+      <c r="P9" s="7">
         <f t="shared" si="3"/>
         <v>0.66297000000000006</v>
       </c>
@@ -2031,22 +2030,22 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="9">
-        <v>1</v>
-      </c>
-      <c r="L10" s="5">
+      <c r="K10" s="8">
+        <v>1</v>
+      </c>
+      <c r="L10" s="4">
         <v>0.104</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="6">
         <f t="shared" si="0"/>
         <v>8.0079999999999998E-2</v>
       </c>
-      <c r="N10" s="8">
+      <c r="N10" s="7">
         <f t="shared" si="1"/>
         <v>8.0079999999999998E-2</v>
       </c>
@@ -2054,7 +2053,7 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="P10" s="8">
+      <c r="P10" s="7">
         <f t="shared" si="3"/>
         <v>0.48048000000000002</v>
       </c>
@@ -2074,22 +2073,22 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="K11" s="9">
-        <v>1</v>
-      </c>
-      <c r="L11" s="5">
+      <c r="K11" s="8">
+        <v>1</v>
+      </c>
+      <c r="L11" s="4">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="6">
         <f t="shared" si="0"/>
         <v>3.696E-2</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="7">
         <f t="shared" si="1"/>
         <v>3.696E-2</v>
       </c>
@@ -2097,14 +2096,14 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="P11" s="8">
+      <c r="P11" s="7">
         <f t="shared" si="3"/>
         <v>0.22176000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>70</v>
@@ -2117,22 +2116,22 @@
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="K12" s="9">
-        <v>1</v>
-      </c>
-      <c r="L12" s="5">
+      <c r="K12" s="8">
+        <v>1</v>
+      </c>
+      <c r="L12" s="4">
         <v>1.4E-2</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="6">
         <f t="shared" si="0"/>
         <v>1.078E-2</v>
       </c>
-      <c r="N12" s="8">
+      <c r="N12" s="7">
         <f t="shared" si="1"/>
         <v>5.3899999999999997E-2</v>
       </c>
@@ -2140,14 +2139,14 @@
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="P12" s="8">
+      <c r="P12" s="7">
         <f t="shared" si="3"/>
         <v>0.28027999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>86</v>
@@ -2160,22 +2159,22 @@
         <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K13" s="9">
-        <v>1</v>
-      </c>
-      <c r="L13" s="5">
+      <c r="K13" s="8">
+        <v>1</v>
+      </c>
+      <c r="L13" s="4">
         <v>1.4E-2</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="6">
         <f t="shared" si="0"/>
         <v>1.078E-2</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N13" s="7">
         <f t="shared" si="1"/>
         <v>4.3119999999999999E-2</v>
       </c>
@@ -2183,14 +2182,14 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="P13" s="8">
+      <c r="P13" s="7">
         <f t="shared" si="3"/>
         <v>0.22638</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>101</v>
@@ -2203,22 +2202,22 @@
         <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K14" s="9">
-        <v>1</v>
-      </c>
-      <c r="L14" s="5">
+      <c r="K14" s="8">
+        <v>1</v>
+      </c>
+      <c r="L14" s="4">
         <v>1.4E-2</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="6">
         <f t="shared" si="0"/>
         <v>1.078E-2</v>
       </c>
-      <c r="N14" s="8">
+      <c r="N14" s="7">
         <f t="shared" si="1"/>
         <v>8.6239999999999997E-2</v>
       </c>
@@ -2226,14 +2225,14 @@
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="P14" s="8">
+      <c r="P14" s="7">
         <f t="shared" si="3"/>
         <v>0.44197999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -2242,23 +2241,23 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>156</v>
+      <c r="F15" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="G15">
         <v>2356152</v>
       </c>
-      <c r="H15" s="3"/>
+      <c r="H15" s="2"/>
       <c r="J15" s="1">
         <v>61300111121</v>
       </c>
-      <c r="K15" s="10">
-        <v>1</v>
-      </c>
-      <c r="M15" s="7">
+      <c r="K15" s="9">
+        <v>1</v>
+      </c>
+      <c r="M15" s="6">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="N15" s="8">
+      <c r="N15" s="7">
         <f t="shared" si="1"/>
         <v>0.20799999999999999</v>
       </c>
@@ -2266,7 +2265,7 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="P15" s="8">
+      <c r="P15" s="7">
         <f t="shared" si="3"/>
         <v>1.0919999999999999</v>
       </c>
@@ -2286,17 +2285,17 @@
       <c r="G16">
         <v>1822224</v>
       </c>
-      <c r="K16" s="9">
-        <v>1</v>
-      </c>
-      <c r="L16" s="5">
+      <c r="K16" s="8">
+        <v>1</v>
+      </c>
+      <c r="L16" s="4">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="M16" s="7">
+      <c r="M16" s="6">
         <f>L16*$K$67</f>
         <v>7.5459999999999999E-2</v>
       </c>
-      <c r="N16" s="8">
+      <c r="N16" s="7">
         <f t="shared" si="1"/>
         <v>7.5459999999999999E-2</v>
       </c>
@@ -2304,14 +2303,14 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="P16" s="8">
+      <c r="P16" s="7">
         <f t="shared" si="3"/>
         <v>0.45276</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>105</v>
@@ -2326,17 +2325,17 @@
       <c r="J17" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K17" s="9">
-        <v>1</v>
-      </c>
-      <c r="L17" s="5">
+      <c r="K17" s="8">
+        <v>1</v>
+      </c>
+      <c r="L17" s="4">
         <v>4.7E-2</v>
       </c>
-      <c r="M17" s="7">
+      <c r="M17" s="6">
         <f>L17*$K$67</f>
         <v>3.619E-2</v>
       </c>
-      <c r="N17" s="8">
+      <c r="N17" s="7">
         <f t="shared" si="1"/>
         <v>1.2666500000000001</v>
       </c>
@@ -2344,7 +2343,7 @@
         <f t="shared" si="2"/>
         <v>176</v>
       </c>
-      <c r="P17" s="8">
+      <c r="P17" s="7">
         <f t="shared" si="3"/>
         <v>6.36944</v>
       </c>
@@ -2364,26 +2363,16 @@
       <c r="I18" t="s">
         <v>136</v>
       </c>
-      <c r="K18" s="10"/>
-      <c r="M18" s="7">
-        <v>0</v>
-      </c>
-      <c r="N18" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O18" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P18" s="8" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+      <c r="K18" s="9"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="7"/>
+      <c r="P18" s="7" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19">
@@ -2393,20 +2382,20 @@
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="G19" s="3"/>
+      <c r="G19" s="2"/>
       <c r="H19" t="s">
-        <v>166</v>
-      </c>
-      <c r="K19" s="10">
+        <v>165</v>
+      </c>
+      <c r="K19" s="9">
         <v>5</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="6">
         <v>0.16600000000000001</v>
       </c>
-      <c r="N19" s="8">
+      <c r="N19" s="7">
         <f t="shared" si="1"/>
         <v>2.6560000000000001</v>
       </c>
@@ -2414,7 +2403,7 @@
         <f t="shared" si="2"/>
         <v>85</v>
       </c>
-      <c r="P19" s="8">
+      <c r="P19" s="7">
         <f t="shared" si="3"/>
         <v>14.110000000000001</v>
       </c>
@@ -2434,22 +2423,22 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K20" s="9">
-        <v>1</v>
-      </c>
-      <c r="L20" s="5">
+      <c r="K20" s="8">
+        <v>1</v>
+      </c>
+      <c r="L20" s="4">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="M20" s="7">
+      <c r="M20" s="6">
         <f>L20*$K$67</f>
         <v>7.0069999999999993E-2</v>
       </c>
-      <c r="N20" s="8">
+      <c r="N20" s="7">
         <f t="shared" si="1"/>
         <v>7.0069999999999993E-2</v>
       </c>
@@ -2457,7 +2446,7 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="P20" s="8">
+      <c r="P20" s="7">
         <f t="shared" si="3"/>
         <v>0.42041999999999996</v>
       </c>
@@ -2477,19 +2466,19 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>198</v>
-      </c>
-      <c r="K21" s="9">
-        <v>1</v>
-      </c>
-      <c r="L21" s="5">
+        <v>197</v>
+      </c>
+      <c r="K21" s="8">
+        <v>1</v>
+      </c>
+      <c r="L21" s="4">
         <v>0.109</v>
       </c>
-      <c r="M21" s="7">
+      <c r="M21" s="6">
         <f>L21*$K$67</f>
         <v>8.3930000000000005E-2</v>
       </c>
-      <c r="N21" s="8">
+      <c r="N21" s="7">
         <f t="shared" si="1"/>
         <v>8.3930000000000005E-2</v>
       </c>
@@ -2497,7 +2486,7 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="P21" s="8">
+      <c r="P21" s="7">
         <f t="shared" si="3"/>
         <v>0.50358000000000003</v>
       </c>
@@ -2517,22 +2506,22 @@
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K22" s="9">
-        <v>1</v>
-      </c>
-      <c r="L22" s="5">
+      <c r="K22" s="8">
+        <v>1</v>
+      </c>
+      <c r="L22" s="4">
         <v>0.01</v>
       </c>
-      <c r="M22" s="7">
+      <c r="M22" s="6">
         <f>L22*$K$67</f>
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="N22" s="8">
+      <c r="N22" s="7">
         <f t="shared" si="1"/>
         <v>1.54E-2</v>
       </c>
@@ -2540,7 +2529,7 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="P22" s="8">
+      <c r="P22" s="7">
         <f t="shared" si="3"/>
         <v>8.4699999999999998E-2</v>
       </c>
@@ -2560,22 +2549,22 @@
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K23" s="9">
-        <v>1</v>
-      </c>
-      <c r="L23" s="5">
+      <c r="K23" s="8">
+        <v>1</v>
+      </c>
+      <c r="L23" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="M23" s="7">
+      <c r="M23" s="6">
         <f>L23*$K$67</f>
         <v>1.9250000000000003E-2</v>
       </c>
-      <c r="N23" s="8">
+      <c r="N23" s="7">
         <f t="shared" si="1"/>
         <v>0.11550000000000002</v>
       </c>
@@ -2583,14 +2572,14 @@
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="P23" s="8">
+      <c r="P23" s="7">
         <f t="shared" si="3"/>
         <v>0.59675000000000011</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>64</v>
@@ -2603,22 +2592,22 @@
         <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K24" s="9">
-        <v>1</v>
-      </c>
-      <c r="L24" s="5">
+      <c r="K24" s="8">
+        <v>1</v>
+      </c>
+      <c r="L24" s="4">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M24" s="7">
+      <c r="M24" s="6">
         <f>L24*$K$67</f>
         <v>1.155E-2</v>
       </c>
-      <c r="N24" s="8">
+      <c r="N24" s="7">
         <f t="shared" si="1"/>
         <v>3.465E-2</v>
       </c>
@@ -2626,14 +2615,14 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="P24" s="8">
+      <c r="P24" s="7">
         <f t="shared" si="3"/>
         <v>0.18479999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -2642,23 +2631,23 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>153</v>
+      <c r="F25" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="G25">
         <v>1667519</v>
       </c>
-      <c r="H25" s="3"/>
+      <c r="H25" s="2"/>
       <c r="J25" t="s">
-        <v>151</v>
-      </c>
-      <c r="K25" s="10">
-        <v>1</v>
-      </c>
-      <c r="M25" s="7">
+        <v>150</v>
+      </c>
+      <c r="K25" s="9">
+        <v>1</v>
+      </c>
+      <c r="M25" s="6">
         <v>1.41</v>
       </c>
-      <c r="N25" s="8">
+      <c r="N25" s="7">
         <f t="shared" si="1"/>
         <v>2.82</v>
       </c>
@@ -2666,14 +2655,14 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="P25" s="8">
+      <c r="P25" s="7">
         <f t="shared" si="3"/>
         <v>15.51</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26">
@@ -2683,20 +2672,20 @@
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G26" s="3"/>
+      <c r="G26" s="2"/>
       <c r="H26" t="s">
-        <v>167</v>
-      </c>
-      <c r="K26" s="10">
+        <v>166</v>
+      </c>
+      <c r="K26" s="9">
         <v>5</v>
       </c>
-      <c r="M26" s="7">
+      <c r="M26" s="6">
         <v>0.23599999999999999</v>
       </c>
-      <c r="N26" s="8">
+      <c r="N26" s="7">
         <f t="shared" si="1"/>
         <v>2.1239999999999997</v>
       </c>
@@ -2704,7 +2693,7 @@
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="P26" s="8">
+      <c r="P26" s="7">
         <f t="shared" si="3"/>
         <v>11.799999999999999</v>
       </c>
@@ -2721,25 +2710,25 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="F27" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
       <c r="I27" t="s">
         <v>124</v>
       </c>
-      <c r="K27" s="9">
-        <v>1</v>
-      </c>
-      <c r="L27" s="5">
+      <c r="K27" s="8">
+        <v>1</v>
+      </c>
+      <c r="L27" s="4">
         <v>42.22</v>
       </c>
-      <c r="M27" s="7">
+      <c r="M27" s="6">
         <f>L27*$K$67</f>
         <v>32.509399999999999</v>
       </c>
-      <c r="N27" s="8">
+      <c r="N27" s="7">
         <f t="shared" si="1"/>
         <v>32.509399999999999</v>
       </c>
@@ -2747,7 +2736,7 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="P27" s="8">
+      <c r="P27" s="7">
         <f t="shared" si="3"/>
         <v>195.0564</v>
       </c>
@@ -2757,7 +2746,7 @@
         <v>60</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2766,19 +2755,19 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28" s="2">
         <v>2449396</v>
       </c>
-      <c r="J28" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="K28" s="10">
+      <c r="J28" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="K28" s="9">
         <v>5</v>
       </c>
-      <c r="M28" s="7">
+      <c r="M28" s="6">
         <v>0.27900000000000003</v>
       </c>
-      <c r="N28" s="8">
+      <c r="N28" s="7">
         <f t="shared" si="1"/>
         <v>0.27900000000000003</v>
       </c>
@@ -2786,7 +2775,7 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="P28" s="8">
+      <c r="P28" s="7">
         <f t="shared" si="3"/>
         <v>2.79</v>
       </c>
@@ -2810,22 +2799,22 @@
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K29" s="9">
-        <v>1</v>
-      </c>
-      <c r="L29" s="5">
+      <c r="K29" s="8">
+        <v>1</v>
+      </c>
+      <c r="L29" s="4">
         <v>0.13600000000000001</v>
       </c>
-      <c r="M29" s="7">
+      <c r="M29" s="6">
         <f>L29*$K$67</f>
         <v>0.10472000000000001</v>
       </c>
-      <c r="N29" s="8">
+      <c r="N29" s="7">
         <f t="shared" si="1"/>
         <v>0.20944000000000002</v>
       </c>
@@ -2833,14 +2822,14 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="P29" s="8">
+      <c r="P29" s="7">
         <f t="shared" si="3"/>
         <v>1.1519200000000001</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>75</v>
@@ -2853,22 +2842,22 @@
         <v>4</v>
       </c>
       <c r="E30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K30" s="9">
-        <v>1</v>
-      </c>
-      <c r="L30" s="5">
+      <c r="K30" s="8">
+        <v>1</v>
+      </c>
+      <c r="L30" s="4">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="M30" s="7">
+      <c r="M30" s="6">
         <f>L30*$K$67</f>
         <v>2.5410000000000002E-2</v>
       </c>
-      <c r="N30" s="8">
+      <c r="N30" s="7">
         <f t="shared" si="1"/>
         <v>2.5410000000000002E-2</v>
       </c>
@@ -2876,40 +2865,58 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="P30" s="8">
+      <c r="P30" s="7">
         <f t="shared" si="3"/>
         <v>0.15246000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
         <v>203</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E31" t="s">
-        <v>204</v>
-      </c>
       <c r="J31" s="1"/>
-      <c r="K31" s="9"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="8"/>
-      <c r="P31" s="8"/>
+      <c r="K31" s="8">
+        <v>1</v>
+      </c>
+      <c r="L31" s="4">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="M31" s="6">
+        <f t="shared" ref="M31:M32" si="5">L31*$K$67</f>
+        <v>2.5410000000000002E-2</v>
+      </c>
+      <c r="N31" s="7">
+        <f t="shared" ref="N31:N32" si="6">PRODUCT(M31,C31)</f>
+        <v>2.5410000000000002E-2</v>
+      </c>
+      <c r="O31">
+        <f t="shared" ref="O31:O32" si="7">ROUNDUP(ROUNDUP((C31*$K$65*(1+$K$66)),0)/K31,0)*K31</f>
+        <v>6</v>
+      </c>
+      <c r="P31" s="7">
+        <f t="shared" ref="P31:P32" si="8">O31*M31</f>
+        <v>0.15246000000000001</v>
+      </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -2919,17 +2926,35 @@
         <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J32" s="1"/>
-      <c r="K32" s="9"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="8"/>
-      <c r="P32" s="8"/>
+      <c r="K32" s="8">
+        <v>1</v>
+      </c>
+      <c r="L32" s="4">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="M32" s="6">
+        <f t="shared" si="5"/>
+        <v>8.4700000000000001E-3</v>
+      </c>
+      <c r="N32" s="7">
+        <f t="shared" si="6"/>
+        <v>1.694E-2</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="P32" s="7">
+        <f t="shared" si="8"/>
+        <v>9.3170000000000003E-2</v>
+      </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>62</v>
@@ -2947,32 +2972,32 @@
       <c r="J33" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K33" s="9">
-        <v>1</v>
-      </c>
-      <c r="L33" s="5">
+      <c r="K33" s="8">
+        <v>1</v>
+      </c>
+      <c r="L33" s="4">
         <v>0.01</v>
       </c>
-      <c r="M33" s="7">
-        <f t="shared" ref="M33:M42" si="5">L33*$K$67</f>
+      <c r="M33" s="6">
+        <f t="shared" ref="M33:M44" si="9">L33*$K$67</f>
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="N33" s="8">
-        <f t="shared" ref="N33:N42" si="6">PRODUCT(M33,C33)</f>
+      <c r="N33" s="7">
+        <f t="shared" ref="N33:N42" si="10">PRODUCT(M33,C33)</f>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="O33">
-        <f t="shared" ref="O33:O42" si="7">ROUNDUP(ROUNDUP((C33*$K$65*(1+$K$66)),0)/K33,0)*K33</f>
+        <f t="shared" ref="O33:O43" si="11">ROUNDUP(ROUNDUP((C33*$K$65*(1+$K$66)),0)/K33,0)*K33</f>
         <v>51</v>
       </c>
-      <c r="P33" s="8">
-        <f t="shared" ref="P33:P42" si="8">O33*M33</f>
+      <c r="P33" s="7">
+        <f t="shared" ref="P33:P42" si="12">O33*M33</f>
         <v>0.39269999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>14</v>
@@ -2985,37 +3010,37 @@
         <v>6</v>
       </c>
       <c r="E34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K34" s="9">
-        <v>1</v>
-      </c>
-      <c r="L34" s="5">
+      <c r="K34" s="8">
+        <v>1</v>
+      </c>
+      <c r="L34" s="4">
         <v>0.01</v>
       </c>
-      <c r="M34" s="7">
-        <f t="shared" si="5"/>
+      <c r="M34" s="6">
+        <f t="shared" si="9"/>
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="N34" s="8">
-        <f t="shared" si="6"/>
+      <c r="N34" s="7">
+        <f t="shared" si="10"/>
         <v>4.6200000000000005E-2</v>
       </c>
       <c r="O34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>31</v>
       </c>
-      <c r="P34" s="8">
-        <f t="shared" si="8"/>
+      <c r="P34" s="7">
+        <f t="shared" si="12"/>
         <v>0.2387</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>5</v>
@@ -3033,26 +3058,26 @@
       <c r="J35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K35" s="9">
-        <v>1</v>
-      </c>
-      <c r="L35" s="5">
+      <c r="K35" s="8">
+        <v>1</v>
+      </c>
+      <c r="L35" s="4">
         <v>0.01</v>
       </c>
-      <c r="M35" s="7">
-        <f t="shared" si="5"/>
+      <c r="M35" s="6">
+        <f t="shared" si="9"/>
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="N35" s="8">
-        <f t="shared" si="6"/>
+      <c r="N35" s="7">
+        <f t="shared" si="10"/>
         <v>3.85E-2</v>
       </c>
       <c r="O35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>26</v>
       </c>
-      <c r="P35" s="8">
-        <f t="shared" si="8"/>
+      <c r="P35" s="7">
+        <f t="shared" si="12"/>
         <v>0.20020000000000002</v>
       </c>
     </row>
@@ -3071,31 +3096,31 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K36" s="9">
-        <v>1</v>
-      </c>
-      <c r="L36" s="5">
+      <c r="K36" s="8">
+        <v>1</v>
+      </c>
+      <c r="L36" s="4">
         <v>0.01</v>
       </c>
-      <c r="M36" s="7">
-        <f t="shared" si="5"/>
+      <c r="M36" s="6">
+        <f t="shared" si="9"/>
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="N36" s="8">
-        <f t="shared" si="6"/>
+      <c r="N36" s="7">
+        <f t="shared" si="10"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="O36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
-      <c r="P36" s="8">
-        <f t="shared" si="8"/>
+      <c r="P36" s="7">
+        <f t="shared" si="12"/>
         <v>4.6200000000000005E-2</v>
       </c>
     </row>
@@ -3114,31 +3139,31 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K37" s="9">
-        <v>1</v>
-      </c>
-      <c r="L37" s="5">
+      <c r="K37" s="8">
+        <v>1</v>
+      </c>
+      <c r="L37" s="4">
         <v>0.01</v>
       </c>
-      <c r="M37" s="7">
-        <f t="shared" si="5"/>
+      <c r="M37" s="6">
+        <f t="shared" si="9"/>
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="N37" s="8">
-        <f t="shared" si="6"/>
+      <c r="N37" s="7">
+        <f t="shared" si="10"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="O37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
-      <c r="P37" s="8">
-        <f t="shared" si="8"/>
+      <c r="P37" s="7">
+        <f t="shared" si="12"/>
         <v>4.6200000000000005E-2</v>
       </c>
     </row>
@@ -3157,37 +3182,37 @@
         <v>2</v>
       </c>
       <c r="E38" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K38" s="9">
-        <v>1</v>
-      </c>
-      <c r="L38" s="5">
+      <c r="K38" s="8">
+        <v>1</v>
+      </c>
+      <c r="L38" s="4">
         <v>0.01</v>
       </c>
-      <c r="M38" s="7">
-        <f t="shared" si="5"/>
+      <c r="M38" s="6">
+        <f t="shared" si="9"/>
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="N38" s="8">
-        <f t="shared" si="6"/>
+      <c r="N38" s="7">
+        <f t="shared" si="10"/>
         <v>1.54E-2</v>
       </c>
       <c r="O38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
-      <c r="P38" s="8">
-        <f t="shared" si="8"/>
+      <c r="P38" s="7">
+        <f t="shared" si="12"/>
         <v>8.4699999999999998E-2</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>7</v>
@@ -3200,31 +3225,31 @@
         <v>4</v>
       </c>
       <c r="E39" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K39" s="9">
-        <v>1</v>
-      </c>
-      <c r="L39" s="5">
+      <c r="K39" s="8">
+        <v>1</v>
+      </c>
+      <c r="L39" s="4">
         <v>0.01</v>
       </c>
-      <c r="M39" s="7">
-        <f t="shared" si="5"/>
+      <c r="M39" s="6">
+        <f t="shared" si="9"/>
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="N39" s="8">
-        <f t="shared" si="6"/>
+      <c r="N39" s="7">
+        <f t="shared" si="10"/>
         <v>1.54E-2</v>
       </c>
       <c r="O39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
-      <c r="P39" s="8">
-        <f t="shared" si="8"/>
+      <c r="P39" s="7">
+        <f t="shared" si="12"/>
         <v>8.4699999999999998E-2</v>
       </c>
     </row>
@@ -3248,32 +3273,32 @@
       <c r="J40" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K40" s="9">
-        <v>1</v>
-      </c>
-      <c r="L40" s="5">
+      <c r="K40" s="8">
+        <v>1</v>
+      </c>
+      <c r="L40" s="4">
         <v>0.01</v>
       </c>
-      <c r="M40" s="7">
-        <f t="shared" si="5"/>
+      <c r="M40" s="6">
+        <f t="shared" si="9"/>
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="N40" s="8">
-        <f t="shared" si="6"/>
+      <c r="N40" s="7">
+        <f t="shared" si="10"/>
         <v>2.3100000000000002E-2</v>
       </c>
       <c r="O40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="P40" s="8">
-        <f t="shared" si="8"/>
+      <c r="P40" s="7">
+        <f t="shared" si="12"/>
         <v>0.1232</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>41</v>
@@ -3286,37 +3311,37 @@
         <v>3</v>
       </c>
       <c r="E41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K41" s="9">
-        <v>1</v>
-      </c>
-      <c r="L41" s="5">
+      <c r="K41" s="8">
+        <v>1</v>
+      </c>
+      <c r="L41" s="4">
         <v>0.01</v>
       </c>
-      <c r="M41" s="7">
-        <f t="shared" si="5"/>
+      <c r="M41" s="6">
+        <f t="shared" si="9"/>
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="N41" s="8">
-        <f t="shared" si="6"/>
+      <c r="N41" s="7">
+        <f t="shared" si="10"/>
         <v>2.3100000000000002E-2</v>
       </c>
       <c r="O41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="P41" s="8">
-        <f t="shared" si="8"/>
+      <c r="P41" s="7">
+        <f t="shared" si="12"/>
         <v>0.1232</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>10</v>
@@ -3334,32 +3359,32 @@
       <c r="J42" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K42" s="9">
-        <v>1</v>
-      </c>
-      <c r="L42" s="5">
+      <c r="K42" s="8">
+        <v>1</v>
+      </c>
+      <c r="L42" s="4">
         <v>0.01</v>
       </c>
-      <c r="M42" s="7">
-        <f t="shared" si="5"/>
+      <c r="M42" s="6">
+        <f t="shared" si="9"/>
         <v>7.7000000000000002E-3</v>
       </c>
-      <c r="N42" s="8">
-        <f t="shared" si="6"/>
+      <c r="N42" s="7">
+        <f t="shared" si="10"/>
         <v>2.3100000000000002E-2</v>
       </c>
       <c r="O42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
-      <c r="P42" s="8">
-        <f t="shared" si="8"/>
+      <c r="P42" s="7">
+        <f t="shared" si="12"/>
         <v>0.1232</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43">
@@ -3370,40 +3395,75 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G43">
         <v>9238379</v>
       </c>
       <c r="J43" s="1"/>
-      <c r="K43" s="9"/>
-      <c r="M43" s="7"/>
-      <c r="N43" s="8"/>
-      <c r="P43" s="8"/>
+      <c r="K43" s="8">
+        <v>10</v>
+      </c>
+      <c r="M43" s="6">
+        <v>1.35E-2</v>
+      </c>
+      <c r="N43" s="7">
+        <f t="shared" ref="N43:N44" si="13">PRODUCT(M43,C43)</f>
+        <v>1.35E-2</v>
+      </c>
+      <c r="O43">
+        <f t="shared" ref="O43:O44" si="14">ROUNDUP(ROUNDUP((C43*$K$65*(1+$K$66)),0)/K43,0)*K43</f>
+        <v>10</v>
+      </c>
+      <c r="P43" s="7">
+        <f t="shared" ref="P43:P44" si="15">O43*M43</f>
+        <v>0.13500000000000001</v>
+      </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
       </c>
       <c r="D44" s="1">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J44" s="1"/>
-      <c r="K44" s="9"/>
-      <c r="M44" s="7"/>
-      <c r="N44" s="8"/>
-      <c r="P44" s="8"/>
+      <c r="K44" s="8">
+        <v>1</v>
+      </c>
+      <c r="L44" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="M44" s="6">
+        <f>L44*$K$67</f>
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="N44" s="7">
+        <f>PRODUCT(M44,C44)</f>
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="O44">
+        <f>ROUNDUP(ROUNDUP((C44*$K$65*(1+$K$66)),0)/K44,0)*K44</f>
+        <v>6</v>
+      </c>
+      <c r="P44" s="7">
+        <f t="shared" ref="P44" si="16">O44*M44</f>
+        <v>4.6200000000000005E-2</v>
+      </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -3412,41 +3472,41 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>150</v>
+      <c r="F45" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="G45">
         <v>2308433</v>
       </c>
-      <c r="H45" s="3"/>
+      <c r="H45" s="2"/>
       <c r="J45" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K45">
         <v>1</v>
       </c>
-      <c r="M45" s="7">
+      <c r="M45" s="6">
         <v>5.39</v>
       </c>
-      <c r="N45" s="8">
-        <f t="shared" ref="N45:N64" si="9">PRODUCT(M45,C45)</f>
+      <c r="N45" s="7">
+        <f t="shared" ref="N45:N64" si="17">PRODUCT(M45,C45)</f>
         <v>5.39</v>
       </c>
       <c r="O45">
-        <f t="shared" ref="O45:O64" si="10">ROUNDUP(ROUNDUP((C45*$K$65*(1+$K$66)),0)/K45,0)*K45</f>
+        <f t="shared" ref="O45:O64" si="18">ROUNDUP(ROUNDUP((C45*$K$65*(1+$K$66)),0)/K45,0)*K45</f>
         <v>6</v>
       </c>
-      <c r="P45" s="8">
-        <f t="shared" ref="P45:P64" si="11">O45*M45</f>
+      <c r="P45" s="7">
+        <f t="shared" ref="P45:P64" si="19">O45*M45</f>
         <v>32.339999999999996</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="C46">
         <v>4</v>
@@ -3456,24 +3516,23 @@
         <v>4</v>
       </c>
       <c r="J46" s="1"/>
-      <c r="K46" s="9">
-        <v>1</v>
-      </c>
-      <c r="M46" s="7">
-        <f>L46*$K$67</f>
-        <v>0</v>
-      </c>
-      <c r="N46" s="8">
-        <f t="shared" si="9"/>
-        <v>0</v>
+      <c r="K46" s="8">
+        <v>1</v>
+      </c>
+      <c r="M46" s="6">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="N46" s="7">
+        <f t="shared" si="17"/>
+        <v>0.40799999999999997</v>
       </c>
       <c r="O46">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>21</v>
       </c>
-      <c r="P46" s="8">
-        <f t="shared" si="11"/>
-        <v>0</v>
+      <c r="P46" s="7">
+        <f t="shared" si="19"/>
+        <v>2.1419999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -3491,21 +3550,23 @@
       <c r="I47" t="s">
         <v>123</v>
       </c>
-      <c r="K47" s="10"/>
-      <c r="M47" s="7">
+      <c r="K47" s="9">
+        <v>1</v>
+      </c>
+      <c r="M47" s="6">
         <v>0</v>
       </c>
-      <c r="N47" s="8">
-        <f t="shared" si="9"/>
+      <c r="N47" s="7">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="O47" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P47" s="8" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+      <c r="O47">
+        <f t="shared" si="18"/>
+        <v>86</v>
+      </c>
+      <c r="P47" s="7">
+        <f t="shared" si="19"/>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -3513,7 +3574,7 @@
         <v>94</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C48">
         <v>2</v>
@@ -3522,32 +3583,32 @@
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="F48" s="2" t="s">
         <v>133</v>
       </c>
       <c r="G48">
         <v>1630424</v>
       </c>
-      <c r="H48" s="3"/>
+      <c r="H48" s="2"/>
       <c r="J48" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K48" s="10">
-        <v>1</v>
-      </c>
-      <c r="M48" s="7">
+      <c r="K48" s="9">
+        <v>1</v>
+      </c>
+      <c r="M48" s="6">
         <v>3.41</v>
       </c>
-      <c r="N48" s="8">
-        <f t="shared" si="9"/>
+      <c r="N48" s="7">
+        <f t="shared" si="17"/>
         <v>6.82</v>
       </c>
       <c r="O48">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
-      <c r="P48" s="8">
-        <f t="shared" si="11"/>
+      <c r="P48" s="7">
+        <f t="shared" si="19"/>
         <v>37.510000000000005</v>
       </c>
     </row>
@@ -3556,7 +3617,7 @@
         <v>78</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -3565,29 +3626,29 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="F49" s="2" t="s">
         <v>125</v>
       </c>
       <c r="G49">
         <v>2101366</v>
       </c>
-      <c r="H49" s="3"/>
-      <c r="K49" s="10">
+      <c r="H49" s="2"/>
+      <c r="K49" s="9">
         <v>10</v>
       </c>
-      <c r="M49" s="7">
+      <c r="M49" s="6">
         <v>0.36199999999999999</v>
       </c>
-      <c r="N49" s="8">
-        <f t="shared" si="9"/>
+      <c r="N49" s="7">
+        <f t="shared" si="17"/>
         <v>0.36199999999999999</v>
       </c>
       <c r="O49">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>10</v>
       </c>
-      <c r="P49" s="8">
-        <f t="shared" si="11"/>
+      <c r="P49" s="7">
+        <f t="shared" si="19"/>
         <v>3.62</v>
       </c>
     </row>
@@ -3596,7 +3657,7 @@
         <v>97</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -3605,29 +3666,29 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="F50" s="2" t="s">
         <v>135</v>
       </c>
       <c r="G50">
         <v>2510021</v>
       </c>
-      <c r="H50" s="3"/>
-      <c r="K50" s="10">
-        <v>1</v>
-      </c>
-      <c r="M50" s="7">
+      <c r="H50" s="2"/>
+      <c r="K50" s="9">
+        <v>1</v>
+      </c>
+      <c r="M50" s="6">
         <v>2.85</v>
       </c>
-      <c r="N50" s="8">
-        <f t="shared" si="9"/>
+      <c r="N50" s="7">
+        <f t="shared" si="17"/>
         <v>2.85</v>
       </c>
       <c r="O50">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="P50" s="8">
-        <f t="shared" si="11"/>
+      <c r="P50" s="7">
+        <f t="shared" si="19"/>
         <v>17.100000000000001</v>
       </c>
     </row>
@@ -3636,7 +3697,7 @@
         <v>82</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -3645,27 +3706,27 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F51" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="K51" s="10">
-        <v>1</v>
-      </c>
-      <c r="M51" s="7">
+      <c r="F51" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="K51" s="9">
+        <v>1</v>
+      </c>
+      <c r="M51" s="6">
         <v>2.09</v>
       </c>
-      <c r="N51" s="8">
-        <f t="shared" si="9"/>
+      <c r="N51" s="7">
+        <f t="shared" si="17"/>
         <v>2.09</v>
       </c>
       <c r="O51">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="P51" s="8">
-        <f t="shared" si="11"/>
+      <c r="P51" s="7">
+        <f t="shared" si="19"/>
         <v>12.54</v>
       </c>
     </row>
@@ -3674,7 +3735,7 @@
         <v>83</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -3683,34 +3744,31 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F52" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="K52" s="10">
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="K52" s="9">
         <v>10</v>
       </c>
-      <c r="L52" s="5">
+      <c r="L52" s="4">
         <v>0.48299999999999998</v>
       </c>
-      <c r="M52" s="7">
+      <c r="M52" s="6">
         <f>PRODUCT(0.77, L52)</f>
         <v>0.37191000000000002</v>
       </c>
-      <c r="N52" s="8">
-        <f t="shared" si="9"/>
+      <c r="N52" s="7">
+        <f t="shared" si="17"/>
         <v>0.37191000000000002</v>
       </c>
       <c r="O52">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>10</v>
       </c>
-      <c r="P52" s="8">
-        <f t="shared" si="11"/>
+      <c r="P52" s="7">
+        <f t="shared" si="19"/>
         <v>3.7191000000000001</v>
       </c>
     </row>
@@ -3727,36 +3785,36 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>191</v>
-      </c>
-      <c r="F53" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
       <c r="I53" t="s">
         <v>139</v>
       </c>
-      <c r="K53" s="10">
-        <v>1</v>
-      </c>
-      <c r="L53" s="5">
+      <c r="K53" s="9">
+        <v>1</v>
+      </c>
+      <c r="L53" s="4">
         <v>9.9499999999999993</v>
       </c>
-      <c r="M53" s="7">
+      <c r="M53" s="6">
         <f>PRODUCT(0.77, L53)</f>
         <v>7.6614999999999993</v>
       </c>
-      <c r="N53" s="8">
-        <f t="shared" si="9"/>
+      <c r="N53" s="7">
+        <f t="shared" si="17"/>
         <v>7.6614999999999993</v>
       </c>
       <c r="O53">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="P53" s="8">
-        <f t="shared" si="11"/>
+      <c r="P53" s="7">
+        <f t="shared" si="19"/>
         <v>45.968999999999994</v>
       </c>
     </row>
@@ -3765,7 +3823,7 @@
         <v>92</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -3774,32 +3832,32 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="F54" s="2" t="s">
         <v>132</v>
       </c>
       <c r="G54">
         <v>1332087</v>
       </c>
-      <c r="H54" s="3"/>
+      <c r="H54" s="2"/>
       <c r="J54" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K54" s="10">
-        <v>1</v>
-      </c>
-      <c r="M54" s="7">
-        <v>1</v>
-      </c>
-      <c r="N54" s="8">
-        <f t="shared" si="9"/>
+      <c r="K54" s="9">
+        <v>1</v>
+      </c>
+      <c r="M54" s="6">
+        <v>1</v>
+      </c>
+      <c r="N54" s="7">
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="O54">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="P54" s="8">
-        <f t="shared" si="11"/>
+      <c r="P54" s="7">
+        <f t="shared" si="19"/>
         <v>6</v>
       </c>
     </row>
@@ -3808,7 +3866,7 @@
         <v>69</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -3817,8 +3875,8 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F55" s="3" t="s">
-        <v>146</v>
+      <c r="F55" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="G55">
         <v>1085308</v>
@@ -3826,22 +3884,22 @@
       <c r="J55" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K55" s="10">
-        <v>1</v>
-      </c>
-      <c r="M55" s="7">
+      <c r="K55" s="9">
+        <v>1</v>
+      </c>
+      <c r="M55" s="6">
         <v>0.28599999999999998</v>
       </c>
-      <c r="N55" s="8">
-        <f t="shared" si="9"/>
+      <c r="N55" s="7">
+        <f t="shared" si="17"/>
         <v>0.28599999999999998</v>
       </c>
       <c r="O55">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="P55" s="8">
-        <f t="shared" si="11"/>
+      <c r="P55" s="7">
+        <f t="shared" si="19"/>
         <v>1.7159999999999997</v>
       </c>
     </row>
@@ -3850,7 +3908,7 @@
         <v>77</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -3860,10 +3918,10 @@
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>208</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>147</v>
+        <v>207</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="G56">
         <v>1466595</v>
@@ -3871,22 +3929,22 @@
       <c r="J56" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="K56" s="10">
+      <c r="K56" s="9">
         <v>5</v>
       </c>
-      <c r="M56" s="7">
+      <c r="M56" s="6">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="N56" s="8">
-        <f t="shared" si="9"/>
+      <c r="N56" s="7">
+        <f t="shared" si="17"/>
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="O56">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>10</v>
       </c>
-      <c r="P56" s="8">
-        <f t="shared" si="11"/>
+      <c r="P56" s="7">
+        <f t="shared" si="19"/>
         <v>0.44999999999999996</v>
       </c>
     </row>
@@ -3895,7 +3953,7 @@
         <v>107</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -3904,32 +3962,32 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="F57" s="2" t="s">
         <v>137</v>
       </c>
       <c r="G57">
         <v>9387129</v>
       </c>
-      <c r="H57" s="3"/>
+      <c r="H57" s="2"/>
       <c r="J57" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="K57" s="10">
-        <v>1</v>
-      </c>
-      <c r="M57" s="7">
+      <c r="K57" s="9">
+        <v>1</v>
+      </c>
+      <c r="M57" s="6">
         <v>1.46</v>
       </c>
-      <c r="N57" s="8">
-        <f t="shared" si="9"/>
+      <c r="N57" s="7">
+        <f t="shared" si="17"/>
         <v>1.46</v>
       </c>
       <c r="O57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="P57" s="8">
-        <f t="shared" si="11"/>
+      <c r="P57" s="7">
+        <f t="shared" si="19"/>
         <v>8.76</v>
       </c>
     </row>
@@ -3938,7 +3996,7 @@
         <v>96</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -3948,34 +4006,34 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>192</v>
-      </c>
-      <c r="F58" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>134</v>
       </c>
       <c r="G58">
         <v>2103565</v>
       </c>
-      <c r="H58" s="3"/>
+      <c r="H58" s="2"/>
       <c r="J58" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K58" s="10">
-        <v>1</v>
-      </c>
-      <c r="M58" s="7">
+      <c r="K58" s="9">
+        <v>1</v>
+      </c>
+      <c r="M58" s="6">
         <v>0.873</v>
       </c>
-      <c r="N58" s="8">
-        <f t="shared" si="9"/>
+      <c r="N58" s="7">
+        <f t="shared" si="17"/>
         <v>0.873</v>
       </c>
       <c r="O58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="P58" s="8">
-        <f t="shared" si="11"/>
+      <c r="P58" s="7">
+        <f t="shared" si="19"/>
         <v>5.2379999999999995</v>
       </c>
     </row>
@@ -3990,30 +4048,30 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F59" s="3" t="s">
+      <c r="F59" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
       <c r="I59" t="s">
         <v>129</v>
       </c>
-      <c r="K59" s="10">
-        <v>1</v>
-      </c>
-      <c r="M59" s="7">
+      <c r="K59" s="9">
+        <v>1</v>
+      </c>
+      <c r="M59" s="6">
         <v>26.3</v>
       </c>
-      <c r="N59" s="8">
-        <f t="shared" si="9"/>
+      <c r="N59" s="7">
+        <f t="shared" si="17"/>
         <v>26.3</v>
       </c>
       <c r="O59">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="P59" s="8">
-        <f t="shared" si="11"/>
+      <c r="P59" s="7">
+        <f t="shared" si="19"/>
         <v>157.80000000000001</v>
       </c>
     </row>
@@ -4022,7 +4080,7 @@
         <v>90</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -4031,7 +4089,7 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="F60" s="2" t="s">
         <v>131</v>
       </c>
       <c r="G60">
@@ -4040,28 +4098,28 @@
       <c r="J60" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="K60" s="10">
-        <v>1</v>
-      </c>
-      <c r="M60" s="7">
+      <c r="K60" s="9">
+        <v>1</v>
+      </c>
+      <c r="M60" s="6">
         <v>1.5</v>
       </c>
-      <c r="N60" s="8">
-        <f t="shared" si="9"/>
+      <c r="N60" s="7">
+        <f t="shared" si="17"/>
         <v>1.5</v>
       </c>
       <c r="O60">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="P60" s="8">
-        <f t="shared" si="11"/>
+      <c r="P60" s="7">
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>84</v>
@@ -4074,31 +4132,31 @@
         <v>4</v>
       </c>
       <c r="E61" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="K61" s="9">
-        <v>1</v>
-      </c>
-      <c r="L61" s="5">
+      <c r="K61" s="8">
+        <v>1</v>
+      </c>
+      <c r="L61" s="4">
         <v>3.13</v>
       </c>
-      <c r="M61" s="7">
+      <c r="M61" s="6">
         <f>L61*$K$67</f>
         <v>2.4100999999999999</v>
       </c>
-      <c r="N61" s="8">
-        <f t="shared" si="9"/>
+      <c r="N61" s="7">
+        <f t="shared" si="17"/>
         <v>9.6403999999999996</v>
       </c>
       <c r="O61">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>21</v>
       </c>
-      <c r="P61" s="8">
-        <f t="shared" si="11"/>
+      <c r="P61" s="7">
+        <f t="shared" si="19"/>
         <v>50.612099999999998</v>
       </c>
     </row>
@@ -4107,7 +4165,7 @@
         <v>72</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -4116,37 +4174,37 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F62" s="4" t="s">
+      <c r="F62" s="3" t="s">
         <v>73</v>
       </c>
       <c r="G62">
         <v>2373743</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="K62" s="10">
-        <v>1</v>
-      </c>
-      <c r="M62" s="7">
+        <v>186</v>
+      </c>
+      <c r="K62" s="9">
+        <v>1</v>
+      </c>
+      <c r="M62" s="6">
         <v>0.68700000000000006</v>
       </c>
-      <c r="N62" s="8">
-        <f t="shared" si="9"/>
+      <c r="N62" s="7">
+        <f t="shared" si="17"/>
         <v>0.68700000000000006</v>
       </c>
       <c r="O62">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="P62" s="8">
-        <f t="shared" si="11"/>
+      <c r="P62" s="7">
+        <f t="shared" si="19"/>
         <v>4.1219999999999999</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>117</v>
@@ -4161,26 +4219,26 @@
       <c r="J63" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="K63" s="9">
-        <v>1</v>
-      </c>
-      <c r="L63" s="5">
+      <c r="K63" s="8">
+        <v>1</v>
+      </c>
+      <c r="L63" s="4">
         <v>0.11700000000000001</v>
       </c>
-      <c r="M63" s="7">
+      <c r="M63" s="6">
         <f>L63*$K$67</f>
         <v>9.0090000000000003E-2</v>
       </c>
-      <c r="N63" s="8">
-        <f t="shared" si="9"/>
+      <c r="N63" s="7">
+        <f t="shared" si="17"/>
         <v>9.0090000000000003E-2</v>
       </c>
       <c r="O63">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="P63" s="8">
-        <f t="shared" si="11"/>
+      <c r="P63" s="7">
+        <f t="shared" si="19"/>
         <v>0.54054000000000002</v>
       </c>
     </row>
@@ -4195,80 +4253,80 @@
         <v>1</v>
       </c>
       <c r="D64" s="1">
-        <f t="shared" ref="D64" si="12">LEN(A64)-LEN(SUBSTITUTE(A64,",",""))+1</f>
+        <f t="shared" ref="D64" si="20">LEN(A64)-LEN(SUBSTITUTE(A64,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K64" s="9">
-        <v>1</v>
-      </c>
-      <c r="L64" s="5">
+      <c r="K64" s="8">
+        <v>1</v>
+      </c>
+      <c r="L64" s="4">
         <v>0.2</v>
       </c>
-      <c r="M64" s="7">
+      <c r="M64" s="6">
         <f>L64*$K$67</f>
         <v>0.15400000000000003</v>
       </c>
-      <c r="N64" s="8">
-        <f t="shared" si="9"/>
+      <c r="N64" s="7">
+        <f t="shared" si="17"/>
         <v>0.15400000000000003</v>
       </c>
       <c r="O64">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
-      <c r="P64" s="8">
-        <f t="shared" si="11"/>
+      <c r="P64" s="7">
+        <f t="shared" si="19"/>
         <v>0.92400000000000015</v>
       </c>
     </row>
     <row r="65" spans="7:18" x14ac:dyDescent="0.25">
-      <c r="J65" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="K65" s="12">
+      <c r="J65" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="K65" s="11">
         <v>5</v>
       </c>
-      <c r="M65" s="6" t="s">
+      <c r="M65" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="N65" s="7">
+        <f>SUM(N2:N62)</f>
+        <v>111.4401</v>
+      </c>
+      <c r="O65" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="N65" s="8">
-        <f>SUM(N2:N62)</f>
-        <v>110.96854999999999</v>
-      </c>
-      <c r="O65" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="P65" s="8" t="e">
+      <c r="P65" s="7">
         <f>SUM(P2:P64)</f>
-        <v>#DIV/0!</v>
+        <v>656.86777999999993</v>
       </c>
     </row>
     <row r="66" spans="7:18" x14ac:dyDescent="0.25">
-      <c r="J66" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="K66" s="14">
+      <c r="J66" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="K66" s="13">
         <v>1E-3</v>
       </c>
-      <c r="O66" s="6"/>
-      <c r="P66" s="8"/>
+      <c r="O66" s="5"/>
+      <c r="P66" s="7"/>
     </row>
     <row r="67" spans="7:18" x14ac:dyDescent="0.25">
       <c r="J67" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K67">
         <v>0.77</v>
       </c>
       <c r="R67" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="71" spans="7:18" x14ac:dyDescent="0.25">
-      <c r="G71" s="3">
+      <c r="G71" s="2">
         <v>2449396</v>
       </c>
       <c r="H71">

</xml_diff>

<commit_message>
Added final few parts
</commit_message>
<xml_diff>
--- a/AQN-BOM.xlsx
+++ b/AQN-BOM.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="246">
   <si>
     <t>Qty</t>
   </si>
@@ -81,18 +81,6 @@
     <t>CC0603KRX7R9BB103</t>
   </si>
   <si>
-    <t>10pf</t>
-  </si>
-  <si>
-    <t>C1, C3</t>
-  </si>
-  <si>
-    <t>302010097</t>
-  </si>
-  <si>
-    <t>CC0603JRNPO9BN100</t>
-  </si>
-  <si>
     <t>C32</t>
   </si>
   <si>
@@ -204,9 +192,6 @@
     <t>F1</t>
   </si>
   <si>
-    <t>Q1</t>
-  </si>
-  <si>
     <t>330R</t>
   </si>
   <si>
@@ -309,9 +294,6 @@
     <t>U$1, U$2</t>
   </si>
   <si>
-    <t>MCP79412-I/SN</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -384,9 +366,6 @@
     <t>320170002</t>
   </si>
   <si>
-    <t>Designator</t>
-  </si>
-  <si>
     <t>Source (if not Seeed)</t>
   </si>
   <si>
@@ -426,9 +405,6 @@
     <t>http://uk.farnell.com/microchip/mcp3424-e-sl/adc-18bit-quad-channel-14soic/dp/1630424</t>
   </si>
   <si>
-    <t>http://uk.farnell.com/microchip/mcp79412-i-sn/rtcc-i2c-1k-ee-64b-sram-8soic/dp/2103565</t>
-  </si>
-  <si>
     <t>http://uk.farnell.com/microchip/mic29300-5-0wu/ldo-volt-reg-3a-5v-to-263-3/dp/2510021</t>
   </si>
   <si>
@@ -528,15 +504,9 @@
     <t>Spares</t>
   </si>
   <si>
-    <t xml:space="preserve">LFXTAL016178 </t>
-  </si>
-  <si>
     <t>Exchange rate</t>
   </si>
   <si>
-    <t>Crystal</t>
-  </si>
-  <si>
     <t>eeprom</t>
   </si>
   <si>
@@ -597,9 +567,6 @@
     <t>dht22</t>
   </si>
   <si>
-    <t>mcp79412</t>
-  </si>
-  <si>
     <t>330R 1500mA</t>
   </si>
   <si>
@@ -754,6 +721,45 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>DS3231SN</t>
+  </si>
+  <si>
+    <t>DS3231SN#</t>
+  </si>
+  <si>
+    <t>http://onecall.farnell.com/maxim-integrated-products/ds3231sn/rtc-tcxo-crystal-3-3v-16soic/dp/2518948</t>
+  </si>
+  <si>
+    <t>.Designator</t>
+  </si>
+  <si>
+    <t>J12</t>
+  </si>
+  <si>
+    <t>JP1, JP2</t>
+  </si>
+  <si>
+    <t>320030017</t>
+  </si>
+  <si>
+    <t>F185-1104A1BSYA1</t>
+  </si>
+  <si>
+    <t>4p-2.54</t>
+  </si>
+  <si>
+    <t>JUMPER</t>
+  </si>
+  <si>
+    <t>http://onecall.farnell.com/harwin/m20-9990246/0-1-pin-header-2-way/dp/CN09983</t>
+  </si>
+  <si>
+    <t>CN09983</t>
+  </si>
+  <si>
+    <t>M20-9990246</t>
   </si>
 </sst>
 </file>
@@ -1597,19 +1603,20 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S84"/>
+  <dimension ref="A1:R150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P47" sqref="P47"/>
+      <selection pane="bottomRight" activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="41" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" customWidth="1"/>
@@ -1626,7 +1633,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>120</v>
+        <v>236</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1635,54 +1642,54 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="G1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="H1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="I1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="N1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="O1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="P1" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="Q1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1698,41 +1705,41 @@
         <v>0.01</v>
       </c>
       <c r="M2" s="6">
-        <f t="shared" ref="M2:M14" si="0">L2*$K$67</f>
+        <f>L2*$K$67</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N2" s="7">
-        <f t="shared" ref="N2:N30" si="1">PRODUCT(M2,C2)</f>
+        <f>PRODUCT(M2,C2)</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:O30" si="2">ROUNDUP(ROUNDUP((C2*$K$65*(1+$K$66)),0)/K2,0)*K2</f>
+        <f>ROUNDUP(ROUNDUP((C2*$K$65*(1+$K$66)),0)/K2,0)*K2</f>
         <v>6</v>
       </c>
       <c r="P2" s="7">
-        <f t="shared" ref="P2:P30" si="3">O2*M2</f>
+        <f>O2*M2</f>
         <v>4.6200000000000005E-2</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>213</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D63" si="4">LEN(A3)-LEN(SUBSTITUTE(A3,",",""))+1</f>
-        <v>2</v>
+        <f>LEN(A3)-LEN(SUBSTITUTE(A3,",",""))+1</f>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>172</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K3" s="8">
         <v>1</v>
@@ -1741,385 +1748,385 @@
         <v>0.01</v>
       </c>
       <c r="M3" s="6">
-        <f t="shared" si="0"/>
+        <f>L3*$K$67</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N3" s="7">
-        <f t="shared" si="1"/>
-        <v>1.54E-2</v>
+        <f>PRODUCT(M3,C3)</f>
+        <v>0.1925</v>
       </c>
       <c r="O3">
-        <f t="shared" si="2"/>
-        <v>11</v>
+        <f>ROUNDUP(ROUNDUP((C3*$K$65*(1+$K$66)),0)/K3,0)*K3</f>
+        <v>126</v>
       </c>
       <c r="P3" s="7">
-        <f t="shared" si="3"/>
-        <v>8.4699999999999998E-2</v>
+        <f>O3*M3</f>
+        <v>0.97020000000000006</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>223</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f>LEN(A4)-LEN(SUBSTITUTE(A4,",",""))+1</f>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="K4" s="8">
         <v>1</v>
       </c>
       <c r="L4" s="4">
-        <v>4.1000000000000002E-2</v>
+        <v>0.01</v>
       </c>
       <c r="M4" s="6">
-        <f t="shared" si="0"/>
-        <v>3.1570000000000001E-2</v>
+        <f>L4*$K$67</f>
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="N4" s="7">
-        <f t="shared" si="1"/>
-        <v>0.12628</v>
+        <f>PRODUCT(M4,C4)</f>
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="O4">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f>ROUNDUP(ROUNDUP((C4*$K$65*(1+$K$66)),0)/K4,0)*K4</f>
+        <v>6</v>
       </c>
       <c r="P4" s="7">
-        <f t="shared" si="3"/>
-        <v>0.66297000000000006</v>
+        <f>O4*M4</f>
+        <v>4.6200000000000005E-2</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>224</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C5">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="4"/>
-        <v>25</v>
+        <f>LEN(A5)-LEN(SUBSTITUTE(A5,",",""))+1</f>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="K5" s="8">
         <v>1</v>
       </c>
       <c r="L5" s="4">
-        <v>0.01</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="M5" s="6">
-        <f t="shared" si="0"/>
-        <v>7.7000000000000002E-3</v>
+        <f>L5*$K$67</f>
+        <v>3.696E-2</v>
       </c>
       <c r="N5" s="7">
-        <f t="shared" si="1"/>
-        <v>0.1925</v>
+        <f>PRODUCT(M5,C5)</f>
+        <v>7.392E-2</v>
       </c>
       <c r="O5">
-        <f t="shared" si="2"/>
-        <v>126</v>
+        <f>ROUNDUP(ROUNDUP((C5*$K$65*(1+$K$66)),0)/K5,0)*K5</f>
+        <v>11</v>
       </c>
       <c r="P5" s="7">
-        <f t="shared" si="3"/>
-        <v>0.97020000000000006</v>
+        <f>O5*M5</f>
+        <v>0.40655999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>212</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f>LEN(A6)-LEN(SUBSTITUTE(A6,",",""))+1</f>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>215</v>
+        <v>182</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="K6" s="8">
         <v>1</v>
       </c>
       <c r="L6" s="4">
-        <v>0.01</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="M6" s="6">
-        <f t="shared" si="0"/>
-        <v>7.7000000000000002E-3</v>
+        <f>L6*$K$67</f>
+        <v>3.1570000000000001E-2</v>
       </c>
       <c r="N6" s="7">
-        <f t="shared" si="1"/>
-        <v>7.7000000000000002E-3</v>
+        <f>PRODUCT(M6,C6)</f>
+        <v>0.12628</v>
       </c>
       <c r="O6">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f>ROUNDUP(ROUNDUP((C6*$K$65*(1+$K$66)),0)/K6,0)*K6</f>
+        <v>21</v>
       </c>
       <c r="P6" s="7">
-        <f t="shared" si="3"/>
-        <v>4.6200000000000005E-2</v>
+        <f>O6*M6</f>
+        <v>0.66297000000000006</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="4"/>
-        <v>2</v>
+        <f>LEN(A7)-LEN(SUBSTITUTE(A7,",",""))+1</f>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="K7" s="8">
         <v>1</v>
       </c>
       <c r="L7" s="4">
-        <v>4.8000000000000001E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="M7" s="6">
-        <f t="shared" si="0"/>
-        <v>3.696E-2</v>
+        <f>L7*$K$67</f>
+        <v>1.155E-2</v>
       </c>
       <c r="N7" s="7">
-        <f t="shared" si="1"/>
-        <v>7.392E-2</v>
+        <f>PRODUCT(M7,C7)</f>
+        <v>1.155E-2</v>
       </c>
       <c r="O7">
-        <f t="shared" si="2"/>
-        <v>11</v>
+        <f>ROUNDUP(ROUNDUP((C7*$K$65*(1+$K$66)),0)/K7,0)*K7</f>
+        <v>6</v>
       </c>
       <c r="P7" s="7">
-        <f t="shared" si="3"/>
-        <v>0.40655999999999998</v>
+        <f>O7*M7</f>
+        <v>6.93E-2</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <f>LEN(A8)-LEN(SUBSTITUTE(A8,",",""))+1</f>
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>197</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>217</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="K8" s="8">
         <v>1</v>
       </c>
       <c r="L8" s="4">
-        <v>1.4999999999999999E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="M8" s="6">
-        <f t="shared" si="0"/>
-        <v>1.155E-2</v>
+        <f>L8*$K$67</f>
+        <v>3.1570000000000001E-2</v>
       </c>
       <c r="N8" s="7">
-        <f t="shared" si="1"/>
-        <v>1.155E-2</v>
+        <f>PRODUCT(M8,C8)</f>
+        <v>0.12628</v>
       </c>
       <c r="O8">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f>ROUNDUP(ROUNDUP((C8*$K$65*(1+$K$66)),0)/K8,0)*K8</f>
+        <v>21</v>
       </c>
       <c r="P8" s="7">
-        <f t="shared" si="3"/>
-        <v>6.93E-2</v>
+        <f>O8*M8</f>
+        <v>0.66297000000000006</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f>LEN(A9)-LEN(SUBSTITUTE(A9,",",""))+1</f>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="K9" s="8">
         <v>1</v>
       </c>
       <c r="L9" s="4">
-        <v>4.1000000000000002E-2</v>
+        <v>0.104</v>
       </c>
       <c r="M9" s="6">
-        <f t="shared" si="0"/>
-        <v>3.1570000000000001E-2</v>
+        <f>L9*$K$67</f>
+        <v>8.0079999999999998E-2</v>
       </c>
       <c r="N9" s="7">
-        <f t="shared" si="1"/>
-        <v>0.12628</v>
+        <f>PRODUCT(M9,C9)</f>
+        <v>8.0079999999999998E-2</v>
       </c>
       <c r="O9">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f>ROUNDUP(ROUNDUP((C9*$K$65*(1+$K$66)),0)/K9,0)*K9</f>
+        <v>6</v>
       </c>
       <c r="P9" s="7">
-        <f t="shared" si="3"/>
-        <v>0.66297000000000006</v>
+        <f>O9*M9</f>
+        <v>0.48048000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A10)-LEN(SUBSTITUTE(A10,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>52</v>
+        <v>109</v>
       </c>
       <c r="K10" s="8">
         <v>1</v>
       </c>
       <c r="L10" s="4">
-        <v>0.104</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="M10" s="6">
-        <f t="shared" si="0"/>
-        <v>8.0079999999999998E-2</v>
+        <f>L10*$K$67</f>
+        <v>3.696E-2</v>
       </c>
       <c r="N10" s="7">
-        <f t="shared" si="1"/>
-        <v>8.0079999999999998E-2</v>
+        <f>PRODUCT(M10,C10)</f>
+        <v>3.696E-2</v>
       </c>
       <c r="O10">
-        <f t="shared" si="2"/>
+        <f>ROUNDUP(ROUNDUP((C10*$K$65*(1+$K$66)),0)/K10,0)*K10</f>
         <v>6</v>
       </c>
       <c r="P10" s="7">
-        <f t="shared" si="3"/>
-        <v>0.48048000000000002</v>
+        <f>O10*M10</f>
+        <v>0.22176000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>113</v>
+        <v>215</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f>LEN(A11)-LEN(SUBSTITUTE(A11,",",""))+1</f>
+        <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>216</v>
+        <v>185</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
       <c r="K11" s="8">
         <v>1</v>
       </c>
       <c r="L11" s="4">
-        <v>4.8000000000000001E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="M11" s="6">
-        <f t="shared" si="0"/>
-        <v>3.696E-2</v>
+        <f>L11*$K$67</f>
+        <v>1.078E-2</v>
       </c>
       <c r="N11" s="7">
-        <f t="shared" si="1"/>
-        <v>3.696E-2</v>
+        <f>PRODUCT(M11,C11)</f>
+        <v>4.3119999999999999E-2</v>
       </c>
       <c r="O11">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f>ROUNDUP(ROUNDUP((C11*$K$65*(1+$K$66)),0)/K11,0)*K11</f>
+        <v>21</v>
       </c>
       <c r="P11" s="7">
-        <f t="shared" si="3"/>
-        <v>0.22176000000000001</v>
+        <f>O11*M11</f>
+        <v>0.22638</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f>LEN(A12)-LEN(SUBSTITUTE(A12,",",""))+1</f>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="K12" s="8">
         <v>1</v>
@@ -2128,41 +2135,41 @@
         <v>1.4E-2</v>
       </c>
       <c r="M12" s="6">
-        <f t="shared" si="0"/>
+        <f>L12*$K$67</f>
         <v>1.078E-2</v>
       </c>
       <c r="N12" s="7">
-        <f t="shared" si="1"/>
-        <v>5.3899999999999997E-2</v>
+        <f>PRODUCT(M12,C12)</f>
+        <v>8.6239999999999997E-2</v>
       </c>
       <c r="O12">
-        <f t="shared" si="2"/>
-        <v>26</v>
+        <f>ROUNDUP(ROUNDUP((C12*$K$65*(1+$K$66)),0)/K12,0)*K12</f>
+        <v>41</v>
       </c>
       <c r="P12" s="7">
-        <f t="shared" si="3"/>
-        <v>0.28027999999999997</v>
+        <f>O12*M12</f>
+        <v>0.44197999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f>LEN(A13)-LEN(SUBSTITUTE(A13,",",""))+1</f>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="K13" s="8">
         <v>1</v>
@@ -2171,302 +2178,302 @@
         <v>1.4E-2</v>
       </c>
       <c r="M13" s="6">
-        <f t="shared" si="0"/>
+        <f>L13*$K$67</f>
         <v>1.078E-2</v>
       </c>
       <c r="N13" s="7">
-        <f t="shared" si="1"/>
-        <v>4.3119999999999999E-2</v>
+        <f>PRODUCT(M13,C13)</f>
+        <v>5.3899999999999997E-2</v>
       </c>
       <c r="O13">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f>ROUNDUP(ROUNDUP((C13*$K$65*(1+$K$66)),0)/K13,0)*K13</f>
+        <v>26</v>
       </c>
       <c r="P13" s="7">
-        <f t="shared" si="3"/>
-        <v>0.22638</v>
+        <f>O13*M13</f>
+        <v>0.28027999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="C14">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="4"/>
-        <v>8</v>
-      </c>
-      <c r="E14" t="s">
-        <v>214</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="K14" s="8">
-        <v>1</v>
-      </c>
-      <c r="L14" s="4">
-        <v>1.4E-2</v>
+        <f>LEN(A14)-LEN(SUBSTITUTE(A14,",",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G14">
+        <v>2356152</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="J14" s="1">
+        <v>61300111121</v>
+      </c>
+      <c r="K14" s="9">
+        <v>1</v>
       </c>
       <c r="M14" s="6">
-        <f t="shared" si="0"/>
-        <v>1.078E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="N14" s="7">
-        <f t="shared" si="1"/>
-        <v>8.6239999999999997E-2</v>
+        <f>PRODUCT(M14,C14)</f>
+        <v>0.20799999999999999</v>
       </c>
       <c r="O14">
-        <f t="shared" si="2"/>
-        <v>41</v>
+        <f>ROUNDUP(ROUNDUP((C14*$K$65*(1+$K$66)),0)/K14,0)*K14</f>
+        <v>21</v>
       </c>
       <c r="P14" s="7">
-        <f t="shared" si="3"/>
-        <v>0.44197999999999998</v>
+        <f>O14*M14</f>
+        <v>1.0919999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>154</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B15" s="1"/>
       <c r="C15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>155</v>
+        <f>LEN(A15)-LEN(SUBSTITUTE(A15,",",""))+1</f>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>2356152</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="J15" s="1">
-        <v>61300111121</v>
-      </c>
-      <c r="K15" s="9">
-        <v>1</v>
+        <v>1822224</v>
+      </c>
+      <c r="K15" s="8">
+        <v>1</v>
+      </c>
+      <c r="L15" s="4">
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="M15" s="6">
-        <v>5.1999999999999998E-2</v>
+        <f>L15*$K$67</f>
+        <v>7.5459999999999999E-2</v>
       </c>
       <c r="N15" s="7">
-        <f t="shared" si="1"/>
-        <v>0.20799999999999999</v>
+        <f>PRODUCT(M15,C15)</f>
+        <v>7.5459999999999999E-2</v>
       </c>
       <c r="O15">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f>ROUNDUP(ROUNDUP((C15*$K$65*(1+$K$66)),0)/K15,0)*K15</f>
+        <v>6</v>
       </c>
       <c r="P15" s="7">
-        <f t="shared" si="3"/>
-        <v>1.0919999999999999</v>
+        <f>O15*M15</f>
+        <v>0.45276</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="1"/>
+        <v>231</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="C16">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>1822224</v>
+        <f>LEN(A16)-LEN(SUBSTITUTE(A16,",",""))+1</f>
+        <v>35</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="K16" s="8">
         <v>1</v>
       </c>
       <c r="L16" s="4">
-        <v>9.8000000000000004E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="M16" s="6">
         <f>L16*$K$67</f>
-        <v>7.5459999999999999E-2</v>
+        <v>3.619E-2</v>
       </c>
       <c r="N16" s="7">
-        <f t="shared" si="1"/>
-        <v>7.5459999999999999E-2</v>
+        <f>PRODUCT(M16,C16)</f>
+        <v>1.2666500000000001</v>
       </c>
       <c r="O16">
-        <f t="shared" si="2"/>
+        <f>ROUNDUP(ROUNDUP((C16*$K$65*(1+$K$66)),0)/K16,0)*K16</f>
+        <v>176</v>
+      </c>
+      <c r="P16" s="7">
+        <f>O16*M16</f>
+        <v>6.36944</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17">
         <v>6</v>
       </c>
-      <c r="P16" s="7">
-        <f t="shared" si="3"/>
-        <v>0.45276</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C17">
-        <v>35</v>
-      </c>
       <c r="D17" s="1">
-        <f t="shared" si="4"/>
-        <v>35</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="K17" s="8">
-        <v>1</v>
-      </c>
-      <c r="L17" s="4">
-        <v>4.7E-2</v>
-      </c>
-      <c r="M17" s="6">
-        <f>L17*$K$67</f>
-        <v>3.619E-2</v>
-      </c>
-      <c r="N17" s="7">
-        <f t="shared" si="1"/>
-        <v>1.2666500000000001</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="2"/>
-        <v>176</v>
-      </c>
-      <c r="P17" s="7">
-        <f t="shared" si="3"/>
-        <v>6.36944</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+        <f>LEN(A17)-LEN(SUBSTITUTE(A17,",",""))+1</f>
+        <v>6</v>
+      </c>
+      <c r="I17" t="s">
+        <v>128</v>
+      </c>
+      <c r="K17" s="9"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="7"/>
+      <c r="P17" s="7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>100</v>
+        <v>217</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18">
+        <v>16</v>
+      </c>
+      <c r="D18" s="1">
+        <f>LEN(A18)-LEN(SUBSTITUTE(A18,",",""))+1</f>
+        <v>16</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" t="s">
+        <v>157</v>
+      </c>
+      <c r="K18" s="9">
+        <v>5</v>
+      </c>
+      <c r="M18" s="6">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="N18" s="7">
+        <f>PRODUCT(M18,C18)</f>
+        <v>2.6560000000000001</v>
+      </c>
+      <c r="O18">
+        <f>ROUNDUP(ROUNDUP((C18*$K$65*(1+$K$66)),0)/K18,0)*K18</f>
+        <v>85</v>
+      </c>
+      <c r="P18" s="7">
+        <f>O18*M18</f>
+        <v>14.110000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <f>LEN(A19)-LEN(SUBSTITUTE(A19,",",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>194</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K19" s="8">
+        <v>1</v>
+      </c>
+      <c r="L19" s="4">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="M19" s="6">
+        <f>L19*$K$67</f>
+        <v>7.0069999999999993E-2</v>
+      </c>
+      <c r="N19" s="7">
+        <f>PRODUCT(M19,C19)</f>
+        <v>7.0069999999999993E-2</v>
+      </c>
+      <c r="O19">
+        <f>ROUNDUP(ROUNDUP((C19*$K$65*(1+$K$66)),0)/K19,0)*K19</f>
         <v>6</v>
       </c>
-      <c r="D18" s="1">
-        <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="I18" t="s">
-        <v>136</v>
-      </c>
-      <c r="K18" s="9"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="7"/>
-      <c r="P18" s="7" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19">
-        <v>16</v>
-      </c>
-      <c r="D19" s="1">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" t="s">
-        <v>165</v>
-      </c>
-      <c r="K19" s="9">
-        <v>5</v>
-      </c>
-      <c r="M19" s="6">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="N19" s="7">
-        <f t="shared" si="1"/>
-        <v>2.6560000000000001</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="2"/>
-        <v>85</v>
-      </c>
       <c r="P19" s="7">
-        <f t="shared" si="3"/>
-        <v>14.110000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>80</v>
+        <f>O19*M19</f>
+        <v>0.42041999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>237</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>81</v>
+        <v>239</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>205</v>
+        <f>LEN(A20)-LEN(SUBSTITUTE(A20,",",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>241</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>79</v>
+        <v>240</v>
       </c>
       <c r="K20" s="8">
         <v>1</v>
       </c>
       <c r="L20" s="4">
-        <v>9.0999999999999998E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="M20" s="6">
         <f>L20*$K$67</f>
-        <v>7.0069999999999993E-2</v>
+        <v>1.617E-2</v>
       </c>
       <c r="N20" s="7">
-        <f t="shared" si="1"/>
-        <v>7.0069999999999993E-2</v>
+        <f>PRODUCT(M20,C20)</f>
+        <v>1.617E-2</v>
       </c>
       <c r="O20">
-        <f t="shared" si="2"/>
+        <f>ROUNDUP(ROUNDUP((C20*$K$65*(1+$K$66)),0)/K20,0)*K20</f>
         <v>6</v>
       </c>
       <c r="P20" s="7">
-        <f t="shared" si="3"/>
-        <v>0.42041999999999996</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+        <f>O20*M20</f>
+        <v>9.7019999999999995E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A21)-LEN(SUBSTITUTE(A21,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="K21" s="8">
         <v>1</v>
@@ -2479,37 +2486,37 @@
         <v>8.3930000000000005E-2</v>
       </c>
       <c r="N21" s="7">
-        <f t="shared" si="1"/>
+        <f>PRODUCT(M21,C21)</f>
         <v>8.3930000000000005E-2</v>
       </c>
       <c r="O21">
-        <f t="shared" si="2"/>
+        <f>ROUNDUP(ROUNDUP((C21*$K$65*(1+$K$66)),0)/K21,0)*K21</f>
         <v>6</v>
       </c>
       <c r="P21" s="7">
-        <f t="shared" si="3"/>
+        <f>O21*M21</f>
         <v>0.50358000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A22)-LEN(SUBSTITUTE(A22,",",""))+1</f>
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="K22" s="8">
         <v>1</v>
@@ -2522,37 +2529,37 @@
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N22" s="7">
-        <f t="shared" si="1"/>
+        <f>PRODUCT(M22,C22)</f>
         <v>1.54E-2</v>
       </c>
       <c r="O22">
-        <f t="shared" si="2"/>
+        <f>ROUNDUP(ROUNDUP((C22*$K$65*(1+$K$66)),0)/K22,0)*K22</f>
         <v>11</v>
       </c>
       <c r="P22" s="7">
-        <f t="shared" si="3"/>
+        <f>O22*M22</f>
         <v>8.4699999999999998E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C23">
         <v>6</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A23)-LEN(SUBSTITUTE(A23,",",""))+1</f>
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K23" s="8">
         <v>1</v>
@@ -2565,244 +2572,244 @@
         <v>1.9250000000000003E-2</v>
       </c>
       <c r="N23" s="7">
-        <f t="shared" si="1"/>
+        <f>PRODUCT(M23,C23)</f>
         <v>0.11550000000000002</v>
       </c>
       <c r="O23">
-        <f t="shared" si="2"/>
+        <f>ROUNDUP(ROUNDUP((C23*$K$65*(1+$K$66)),0)/K23,0)*K23</f>
         <v>31</v>
       </c>
       <c r="P23" s="7">
-        <f t="shared" si="3"/>
+        <f>O23*M23</f>
         <v>0.59675000000000011</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>229</v>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>238</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>64</v>
+        <v>242</v>
       </c>
       <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <f>LEN(A24)-LEN(SUBSTITUTE(A24,",",""))+1</f>
+        <v>2</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G24" t="s">
+        <v>244</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="K24" s="8">
+        <v>10</v>
+      </c>
+      <c r="M24" s="6">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="N24" s="7">
+        <f>PRODUCT(M24,C24)</f>
+        <v>0.13</v>
+      </c>
+      <c r="O24">
+        <f>ROUNDUP(ROUNDUP((C24*$K$65*(1+$K$66)),0)/K24,0)*K24</f>
+        <v>20</v>
+      </c>
+      <c r="P24" s="7">
+        <f>O24*M24</f>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25">
         <v>3</v>
       </c>
-      <c r="D24" s="1">
-        <f t="shared" si="4"/>
+      <c r="D25" s="1">
+        <f>LEN(A25)-LEN(SUBSTITUTE(A25,",",""))+1</f>
         <v>3</v>
       </c>
-      <c r="E24" t="s">
-        <v>192</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K24" s="8">
-        <v>1</v>
-      </c>
-      <c r="L24" s="4">
+      <c r="E25" t="s">
+        <v>181</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K25" s="8">
+        <v>1</v>
+      </c>
+      <c r="L25" s="4">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M24" s="6">
-        <f>L24*$K$67</f>
+      <c r="M25" s="6">
+        <f>L25*$K$67</f>
         <v>1.155E-2</v>
       </c>
-      <c r="N24" s="7">
-        <f t="shared" si="1"/>
+      <c r="N25" s="7">
+        <f>PRODUCT(M25,C25)</f>
         <v>3.465E-2</v>
       </c>
-      <c r="O24">
-        <f t="shared" si="2"/>
+      <c r="O25">
+        <f>ROUNDUP(ROUNDUP((C25*$K$65*(1+$K$66)),0)/K25,0)*K25</f>
         <v>16</v>
       </c>
-      <c r="P24" s="7">
-        <f t="shared" si="3"/>
+      <c r="P25" s="7">
+        <f>O25*M25</f>
         <v>0.18479999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C26">
         <v>2</v>
       </c>
-      <c r="D25" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G25">
+      <c r="D26" s="1">
+        <f>LEN(A26)-LEN(SUBSTITUTE(A26,",",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G26">
         <v>1667519</v>
       </c>
-      <c r="H25" s="2"/>
-      <c r="J25" t="s">
-        <v>150</v>
-      </c>
-      <c r="K25" s="9">
-        <v>1</v>
-      </c>
-      <c r="M25" s="6">
+      <c r="H26" s="2"/>
+      <c r="J26" t="s">
+        <v>142</v>
+      </c>
+      <c r="K26" s="9">
+        <v>1</v>
+      </c>
+      <c r="M26" s="6">
         <v>1.41</v>
       </c>
-      <c r="N25" s="7">
-        <f t="shared" si="1"/>
+      <c r="N26" s="7">
+        <f>PRODUCT(M26,C26)</f>
         <v>2.82</v>
       </c>
-      <c r="O25">
-        <f t="shared" si="2"/>
+      <c r="O26">
+        <f>ROUNDUP(ROUNDUP((C26*$K$65*(1+$K$66)),0)/K26,0)*K26</f>
         <v>11</v>
       </c>
-      <c r="P25" s="7">
-        <f t="shared" si="3"/>
+      <c r="P26" s="7">
+        <f>O26*M26</f>
         <v>15.51</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="C26">
-        <v>9</v>
-      </c>
-      <c r="D26" s="1">
-        <f t="shared" si="4"/>
-        <v>9</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G26" s="2"/>
-      <c r="H26" t="s">
-        <v>166</v>
-      </c>
-      <c r="K26" s="9">
-        <v>5</v>
-      </c>
-      <c r="M26" s="6">
-        <v>0.23599999999999999</v>
-      </c>
-      <c r="N26" s="7">
-        <f t="shared" si="1"/>
-        <v>2.1239999999999997</v>
-      </c>
-      <c r="O26">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-      <c r="P26" s="7">
-        <f t="shared" si="3"/>
-        <v>11.799999999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>103</v>
+        <v>219</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f>LEN(A27)-LEN(SUBSTITUTE(A27,",",""))+1</f>
+        <v>9</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" t="s">
-        <v>124</v>
-      </c>
-      <c r="K27" s="8">
-        <v>1</v>
-      </c>
-      <c r="L27" s="4">
+      <c r="H27" t="s">
+        <v>158</v>
+      </c>
+      <c r="K27" s="9">
+        <v>5</v>
+      </c>
+      <c r="M27" s="6">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="N27" s="7">
+        <f>PRODUCT(M27,C27)</f>
+        <v>2.1239999999999997</v>
+      </c>
+      <c r="O27">
+        <f>ROUNDUP(ROUNDUP((C27*$K$65*(1+$K$66)),0)/K27,0)*K27</f>
+        <v>50</v>
+      </c>
+      <c r="P27" s="7">
+        <f>O27*M27</f>
+        <v>11.799999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1">
+        <f>LEN(A28)-LEN(SUBSTITUTE(A28,",",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" t="s">
+        <v>117</v>
+      </c>
+      <c r="K28" s="8">
+        <v>1</v>
+      </c>
+      <c r="L28" s="4">
         <v>42.22</v>
       </c>
-      <c r="M27" s="6">
-        <f>L27*$K$67</f>
+      <c r="M28" s="6">
+        <f>L28*$K$67</f>
         <v>32.509399999999999</v>
       </c>
-      <c r="N27" s="7">
-        <f t="shared" si="1"/>
+      <c r="N28" s="7">
+        <f>PRODUCT(M28,C28)</f>
         <v>32.509399999999999</v>
       </c>
-      <c r="O27">
-        <f t="shared" si="2"/>
+      <c r="O28">
+        <f>ROUNDUP(ROUNDUP((C28*$K$65*(1+$K$66)),0)/K28,0)*K28</f>
         <v>6</v>
       </c>
-      <c r="P27" s="7">
-        <f t="shared" si="3"/>
+      <c r="P28" s="7">
+        <f>O28*M28</f>
         <v>195.0564</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="G28" s="2">
-        <v>2449396</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="K28" s="9">
-        <v>5</v>
-      </c>
-      <c r="M28" s="6">
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="N28" s="7">
-        <f t="shared" si="1"/>
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="O28">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="P28" s="7">
-        <f t="shared" si="3"/>
-        <v>2.79</v>
-      </c>
-      <c r="S28">
-        <f>ROUNDUP(C28*K52*(1+K53),0)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A29)-LEN(SUBSTITUTE(A29,",",""))+1</f>
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="K29" s="8">
         <v>1</v>
@@ -2815,37 +2822,37 @@
         <v>0.10472000000000001</v>
       </c>
       <c r="N29" s="7">
-        <f t="shared" si="1"/>
+        <f>PRODUCT(M29,C29)</f>
         <v>0.20944000000000002</v>
       </c>
       <c r="O29">
-        <f t="shared" si="2"/>
+        <f>ROUNDUP(ROUNDUP((C29*$K$65*(1+$K$66)),0)/K29,0)*K29</f>
         <v>11</v>
       </c>
       <c r="P29" s="7">
-        <f t="shared" si="3"/>
+        <f>O29*M29</f>
         <v>1.1519200000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A30)-LEN(SUBSTITUTE(A30,",",""))+1</f>
         <v>4</v>
       </c>
       <c r="E30" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="K30" s="8">
         <v>1</v>
@@ -2858,34 +2865,34 @@
         <v>2.5410000000000002E-2</v>
       </c>
       <c r="N30" s="7">
-        <f t="shared" si="1"/>
+        <f>PRODUCT(M30,C30)</f>
         <v>2.5410000000000002E-2</v>
       </c>
       <c r="O30">
-        <f t="shared" si="2"/>
+        <f>ROUNDUP(ROUNDUP((C30*$K$65*(1+$K$66)),0)/K30,0)*K30</f>
         <v>6</v>
       </c>
       <c r="P30" s="7">
-        <f t="shared" si="3"/>
+        <f>O30*M30</f>
         <v>0.15246000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A31)-LEN(SUBSTITUTE(A31,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="8">
@@ -2895,38 +2902,38 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="M31" s="6">
-        <f t="shared" ref="M31:M32" si="5">L31*$K$67</f>
+        <f>L31*$K$67</f>
         <v>2.5410000000000002E-2</v>
       </c>
       <c r="N31" s="7">
-        <f t="shared" ref="N31:N32" si="6">PRODUCT(M31,C31)</f>
+        <f>PRODUCT(M31,C31)</f>
         <v>2.5410000000000002E-2</v>
       </c>
       <c r="O31">
-        <f t="shared" ref="O31:O32" si="7">ROUNDUP(ROUNDUP((C31*$K$65*(1+$K$66)),0)/K31,0)*K31</f>
+        <f>ROUNDUP(ROUNDUP((C31*$K$65*(1+$K$66)),0)/K31,0)*K31</f>
         <v>6</v>
       </c>
       <c r="P31" s="7">
-        <f t="shared" ref="P31:P32" si="8">O31*M31</f>
+        <f>O31*M31</f>
         <v>0.15246000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A32)-LEN(SUBSTITUTE(A32,",",""))+1</f>
         <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="8">
@@ -2936,41 +2943,41 @@
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="M32" s="6">
-        <f t="shared" si="5"/>
+        <f>L32*$K$67</f>
         <v>8.4700000000000001E-3</v>
       </c>
       <c r="N32" s="7">
-        <f t="shared" si="6"/>
+        <f>PRODUCT(M32,C32)</f>
         <v>1.694E-2</v>
       </c>
       <c r="O32">
-        <f t="shared" si="7"/>
+        <f>ROUNDUP(ROUNDUP((C32*$K$65*(1+$K$66)),0)/K32,0)*K32</f>
         <v>11</v>
       </c>
       <c r="P32" s="7">
-        <f t="shared" si="8"/>
+        <f>O32*M32</f>
         <v>9.3170000000000003E-2</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="C33">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="4"/>
-        <v>10</v>
+        <f>LEN(A33)-LEN(SUBSTITUTE(A33,",",""))+1</f>
+        <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>61</v>
+        <v>173</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="K33" s="8">
         <v>1</v>
@@ -2979,41 +2986,41 @@
         <v>0.01</v>
       </c>
       <c r="M33" s="6">
-        <f t="shared" ref="M33:M44" si="9">L33*$K$67</f>
+        <f>L33*$K$67</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N33" s="7">
-        <f t="shared" ref="N33:N42" si="10">PRODUCT(M33,C33)</f>
-        <v>7.6999999999999999E-2</v>
+        <f>PRODUCT(M33,C33)</f>
+        <v>4.6200000000000005E-2</v>
       </c>
       <c r="O33">
-        <f t="shared" ref="O33:O43" si="11">ROUNDUP(ROUNDUP((C33*$K$65*(1+$K$66)),0)/K33,0)*K33</f>
-        <v>51</v>
+        <f>ROUNDUP(ROUNDUP((C33*$K$65*(1+$K$66)),0)/K33,0)*K33</f>
+        <v>31</v>
       </c>
       <c r="P33" s="7">
-        <f t="shared" ref="P33:P42" si="12">O33*M33</f>
-        <v>0.39269999999999999</v>
+        <f>O33*M33</f>
+        <v>0.2387</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>212</v>
+        <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C34">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="4"/>
-        <v>6</v>
+        <f>LEN(A34)-LEN(SUBSTITUTE(A34,",",""))+1</f>
+        <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="K34" s="8">
         <v>1</v>
@@ -3022,84 +3029,82 @@
         <v>0.01</v>
       </c>
       <c r="M34" s="6">
-        <f t="shared" si="9"/>
+        <f>L34*$K$67</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N34" s="7">
-        <f t="shared" si="10"/>
+        <f>PRODUCT(M34,C34)</f>
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="O34">
+        <f>ROUNDUP(ROUNDUP((C34*$K$65*(1+$K$66)),0)/K34,0)*K34</f>
+        <v>6</v>
+      </c>
+      <c r="P34" s="7">
+        <f>O34*M34</f>
         <v>4.6200000000000005E-2</v>
-      </c>
-      <c r="O34">
-        <f t="shared" si="11"/>
-        <v>31</v>
-      </c>
-      <c r="P34" s="7">
-        <f t="shared" si="12"/>
-        <v>0.2387</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="B35" s="1"/>
       <c r="C35">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="4"/>
-        <v>5</v>
+        <f>LEN(A35)-LEN(SUBSTITUTE(A35,",",""))+1</f>
+        <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>4</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="F35" t="s">
+        <v>225</v>
+      </c>
+      <c r="G35">
+        <v>9238379</v>
+      </c>
+      <c r="J35" s="1"/>
       <c r="K35" s="8">
-        <v>1</v>
-      </c>
-      <c r="L35" s="4">
-        <v>0.01</v>
+        <v>10</v>
       </c>
       <c r="M35" s="6">
-        <f t="shared" si="9"/>
-        <v>7.7000000000000002E-3</v>
+        <v>1.35E-2</v>
       </c>
       <c r="N35" s="7">
-        <f t="shared" si="10"/>
-        <v>3.85E-2</v>
+        <f>PRODUCT(M35,C35)</f>
+        <v>1.35E-2</v>
       </c>
       <c r="O35">
-        <f t="shared" si="11"/>
-        <v>26</v>
+        <f>ROUNDUP(ROUNDUP((C35*$K$65*(1+$K$66)),0)/K35,0)*K35</f>
+        <v>10</v>
       </c>
       <c r="P35" s="7">
-        <f t="shared" si="12"/>
-        <v>0.20020000000000002</v>
+        <f>O35*M35</f>
+        <v>0.13500000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C36">
         <v>1</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A36)-LEN(SUBSTITUTE(A36,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K36" s="8">
         <v>1</v>
@@ -3108,41 +3113,41 @@
         <v>0.01</v>
       </c>
       <c r="M36" s="6">
-        <f t="shared" si="9"/>
+        <f>L36*$K$67</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N36" s="7">
-        <f t="shared" si="10"/>
+        <f>PRODUCT(M36,C36)</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="O36">
-        <f t="shared" si="11"/>
+        <f>ROUNDUP(ROUNDUP((C36*$K$65*(1+$K$66)),0)/K36,0)*K36</f>
         <v>6</v>
       </c>
       <c r="P36" s="7">
-        <f t="shared" si="12"/>
+        <f>O36*M36</f>
         <v>4.6200000000000005E-2</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f>LEN(A37)-LEN(SUBSTITUTE(A37,",",""))+1</f>
+        <v>2</v>
       </c>
       <c r="E37" t="s">
-        <v>218</v>
+        <v>178</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="K37" s="8">
         <v>1</v>
@@ -3151,41 +3156,41 @@
         <v>0.01</v>
       </c>
       <c r="M37" s="6">
-        <f t="shared" si="9"/>
+        <f>L37*$K$67</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N37" s="7">
-        <f t="shared" si="10"/>
-        <v>7.7000000000000002E-3</v>
+        <f>PRODUCT(M37,C37)</f>
+        <v>1.54E-2</v>
       </c>
       <c r="O37">
-        <f t="shared" si="11"/>
-        <v>6</v>
+        <f>ROUNDUP(ROUNDUP((C37*$K$65*(1+$K$66)),0)/K37,0)*K37</f>
+        <v>11</v>
       </c>
       <c r="P37" s="7">
-        <f t="shared" si="12"/>
-        <v>4.6200000000000005E-2</v>
+        <f>O37*M37</f>
+        <v>8.4699999999999998E-2</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>56</v>
+        <v>193</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="C38">
         <v>2</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" si="4"/>
-        <v>2</v>
+        <f>LEN(A38)-LEN(SUBSTITUTE(A38,",",""))+1</f>
+        <v>4</v>
       </c>
       <c r="E38" t="s">
         <v>188</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="K38" s="8">
         <v>1</v>
@@ -3194,41 +3199,41 @@
         <v>0.01</v>
       </c>
       <c r="M38" s="6">
-        <f t="shared" si="9"/>
+        <f>L38*$K$67</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N38" s="7">
-        <f t="shared" si="10"/>
+        <f>PRODUCT(M38,C38)</f>
         <v>1.54E-2</v>
       </c>
       <c r="O38">
-        <f t="shared" si="11"/>
+        <f>ROUNDUP(ROUNDUP((C38*$K$65*(1+$K$66)),0)/K38,0)*K38</f>
         <v>11</v>
       </c>
       <c r="P38" s="7">
-        <f t="shared" si="12"/>
+        <f>O38*M38</f>
         <v>8.4699999999999998E-2</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>204</v>
+        <v>43</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D39" s="1">
-        <f t="shared" si="4"/>
-        <v>4</v>
+        <f>LEN(A39)-LEN(SUBSTITUTE(A39,",",""))+1</f>
+        <v>3</v>
       </c>
       <c r="E39" t="s">
-        <v>199</v>
+        <v>42</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="K39" s="8">
         <v>1</v>
@@ -3237,42 +3242,37 @@
         <v>0.01</v>
       </c>
       <c r="M39" s="6">
-        <f t="shared" si="9"/>
+        <f>L39*$K$67</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N39" s="7">
-        <f t="shared" si="10"/>
-        <v>1.54E-2</v>
+        <f>PRODUCT(M39,C39)</f>
+        <v>2.3100000000000002E-2</v>
       </c>
       <c r="O39">
-        <f t="shared" si="11"/>
-        <v>11</v>
+        <f>ROUNDUP(ROUNDUP((C39*$K$65*(1+$K$66)),0)/K39,0)*K39</f>
+        <v>16</v>
       </c>
       <c r="P39" s="7">
-        <f t="shared" si="12"/>
-        <v>8.4699999999999998E-2</v>
+        <f>O39*M39</f>
+        <v>0.1232</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>47</v>
+        <v>202</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>48</v>
+        <v>226</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D40" s="1">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="E40" t="s">
-        <v>46</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>49</v>
-      </c>
+        <f>LEN(A40)-LEN(SUBSTITUTE(A40,",",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="J40" s="1"/>
       <c r="K40" s="8">
         <v>1</v>
       </c>
@@ -3280,41 +3280,41 @@
         <v>0.01</v>
       </c>
       <c r="M40" s="6">
-        <f t="shared" si="9"/>
+        <f>L40*$K$67</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N40" s="7">
-        <f t="shared" si="10"/>
-        <v>2.3100000000000002E-2</v>
+        <f>PRODUCT(M40,C40)</f>
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="O40">
-        <f t="shared" si="11"/>
-        <v>16</v>
+        <f>ROUNDUP(ROUNDUP((C40*$K$65*(1+$K$66)),0)/K40,0)*K40</f>
+        <v>6</v>
       </c>
       <c r="P40" s="7">
-        <f t="shared" si="12"/>
-        <v>0.1232</v>
+        <f>O40*M40</f>
+        <v>4.6200000000000005E-2</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C41">
         <v>3</v>
       </c>
       <c r="D41" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A41)-LEN(SUBSTITUTE(A41,",",""))+1</f>
         <v>3</v>
       </c>
       <c r="E41" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K41" s="8">
         <v>1</v>
@@ -3323,41 +3323,41 @@
         <v>0.01</v>
       </c>
       <c r="M41" s="6">
-        <f t="shared" si="9"/>
+        <f>L41*$K$67</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N41" s="7">
-        <f t="shared" si="10"/>
+        <f>PRODUCT(M41,C41)</f>
         <v>2.3100000000000002E-2</v>
       </c>
       <c r="O41">
-        <f t="shared" si="11"/>
+        <f>ROUNDUP(ROUNDUP((C41*$K$65*(1+$K$66)),0)/K41,0)*K41</f>
         <v>16</v>
       </c>
       <c r="P41" s="7">
-        <f t="shared" si="12"/>
+        <f>O41*M41</f>
         <v>0.1232</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42">
         <v>10</v>
       </c>
-      <c r="C42">
-        <v>3</v>
-      </c>
       <c r="D42" s="1">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <f>LEN(A42)-LEN(SUBSTITUTE(A42,",",""))+1</f>
+        <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="K42" s="8">
         <v>1</v>
@@ -3366,78 +3366,85 @@
         <v>0.01</v>
       </c>
       <c r="M42" s="6">
-        <f t="shared" si="9"/>
+        <f>L42*$K$67</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N42" s="7">
-        <f t="shared" si="10"/>
-        <v>2.3100000000000002E-2</v>
+        <f>PRODUCT(M42,C42)</f>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="O42">
-        <f t="shared" si="11"/>
-        <v>16</v>
+        <f>ROUNDUP(ROUNDUP((C42*$K$65*(1+$K$66)),0)/K42,0)*K42</f>
+        <v>51</v>
       </c>
       <c r="P42" s="7">
-        <f t="shared" si="12"/>
-        <v>0.1232</v>
+        <f>O42*M42</f>
+        <v>0.39269999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B43" s="1"/>
+        <v>223</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C43">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D43" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
+        <f>LEN(A43)-LEN(SUBSTITUTE(A43,",",""))+1</f>
+        <v>5</v>
       </c>
       <c r="E43" t="s">
-        <v>221</v>
-      </c>
-      <c r="F43" t="s">
-        <v>236</v>
-      </c>
-      <c r="G43">
-        <v>9238379</v>
-      </c>
-      <c r="J43" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="K43" s="8">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="L43" s="4">
+        <v>0.01</v>
       </c>
       <c r="M43" s="6">
-        <v>1.35E-2</v>
+        <f>L43*$K$67</f>
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="N43" s="7">
-        <f t="shared" ref="N43:N44" si="13">PRODUCT(M43,C43)</f>
-        <v>1.35E-2</v>
+        <f>PRODUCT(M43,C43)</f>
+        <v>3.85E-2</v>
       </c>
       <c r="O43">
-        <f t="shared" ref="O43:O44" si="14">ROUNDUP(ROUNDUP((C43*$K$65*(1+$K$66)),0)/K43,0)*K43</f>
-        <v>10</v>
+        <f>ROUNDUP(ROUNDUP((C43*$K$65*(1+$K$66)),0)/K43,0)*K43</f>
+        <v>26</v>
       </c>
       <c r="P43" s="7">
-        <f t="shared" ref="P43:P44" si="15">O43*M43</f>
-        <v>0.13500000000000001</v>
+        <f>O43*M43</f>
+        <v>0.20020000000000002</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>237</v>
+        <v>10</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D44" s="1">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J44" s="1"/>
+        <f>LEN(A44)-LEN(SUBSTITUTE(A44,",",""))+1</f>
+        <v>3</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="K44" s="8">
         <v>1</v>
       </c>
@@ -3450,37 +3457,37 @@
       </c>
       <c r="N44" s="7">
         <f>PRODUCT(M44,C44)</f>
-        <v>7.7000000000000002E-3</v>
+        <v>2.3100000000000002E-2</v>
       </c>
       <c r="O44">
         <f>ROUNDUP(ROUNDUP((C44*$K$65*(1+$K$66)),0)/K44,0)*K44</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="P44" s="7">
-        <f t="shared" ref="P44" si="16">O44*M44</f>
-        <v>4.6200000000000005E-2</v>
+        <f>O44*M44</f>
+        <v>0.1232</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A45)-LEN(SUBSTITUTE(A45,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="G45">
         <v>2308433</v>
       </c>
       <c r="H45" s="2"/>
       <c r="J45" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="K45">
         <v>1</v>
@@ -3489,30 +3496,30 @@
         <v>5.39</v>
       </c>
       <c r="N45" s="7">
-        <f t="shared" ref="N45:N64" si="17">PRODUCT(M45,C45)</f>
+        <f>PRODUCT(M45,C45)</f>
         <v>5.39</v>
       </c>
       <c r="O45">
-        <f t="shared" ref="O45:O64" si="18">ROUNDUP(ROUNDUP((C45*$K$65*(1+$K$66)),0)/K45,0)*K45</f>
+        <f>ROUNDUP(ROUNDUP((C45*$K$65*(1+$K$66)),0)/K45,0)*K45</f>
         <v>6</v>
       </c>
       <c r="P45" s="7">
-        <f t="shared" ref="P45:P64" si="19">O45*M45</f>
+        <f>O45*M45</f>
         <v>32.339999999999996</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="C46">
         <v>4</v>
       </c>
       <c r="D46" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A46)-LEN(SUBSTITUTE(A46,",",""))+1</f>
         <v>4</v>
       </c>
       <c r="J46" s="1"/>
@@ -3523,32 +3530,32 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="N46" s="7">
-        <f t="shared" si="17"/>
+        <f>PRODUCT(M46,C46)</f>
         <v>0.40799999999999997</v>
       </c>
       <c r="O46">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C46*$K$65*(1+$K$66)),0)/K46,0)*K46</f>
         <v>21</v>
       </c>
       <c r="P46" s="7">
-        <f t="shared" si="19"/>
+        <f>O46*M46</f>
         <v>2.1419999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47">
         <v>17</v>
       </c>
       <c r="D47" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A47)-LEN(SUBSTITUTE(A47,",",""))+1</f>
         <v>17</v>
       </c>
       <c r="I47" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="K47" s="9">
         <v>1</v>
@@ -3557,41 +3564,41 @@
         <v>0</v>
       </c>
       <c r="N47" s="7">
-        <f t="shared" si="17"/>
+        <f>PRODUCT(M47,C47)</f>
         <v>0</v>
       </c>
       <c r="O47">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C47*$K$65*(1+$K$66)),0)/K47,0)*K47</f>
         <v>86</v>
       </c>
       <c r="P47" s="7">
-        <f t="shared" si="19"/>
+        <f>O47*M47</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
       <c r="D48" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A48)-LEN(SUBSTITUTE(A48,",",""))+1</f>
         <v>2</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="G48">
         <v>1630424</v>
       </c>
       <c r="H48" s="2"/>
       <c r="J48" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="K48" s="9">
         <v>1</v>
@@ -3600,34 +3607,34 @@
         <v>3.41</v>
       </c>
       <c r="N48" s="7">
-        <f t="shared" si="17"/>
+        <f>PRODUCT(M48,C48)</f>
         <v>6.82</v>
       </c>
       <c r="O48">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C48*$K$65*(1+$K$66)),0)/K48,0)*K48</f>
         <v>11</v>
       </c>
       <c r="P48" s="7">
-        <f t="shared" si="19"/>
+        <f>O48*M48</f>
         <v>37.510000000000005</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A49)-LEN(SUBSTITUTE(A49,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="G49">
         <v>2101366</v>
@@ -3640,34 +3647,34 @@
         <v>0.36199999999999999</v>
       </c>
       <c r="N49" s="7">
-        <f t="shared" si="17"/>
+        <f>PRODUCT(M49,C49)</f>
         <v>0.36199999999999999</v>
       </c>
       <c r="O49">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C49*$K$65*(1+$K$66)),0)/K49,0)*K49</f>
         <v>10</v>
       </c>
       <c r="P49" s="7">
-        <f t="shared" si="19"/>
+        <f>O49*M49</f>
         <v>3.62</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A50)-LEN(SUBSTITUTE(A50,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="G50">
         <v>2510021</v>
@@ -3680,34 +3687,34 @@
         <v>2.85</v>
       </c>
       <c r="N50" s="7">
-        <f t="shared" si="17"/>
+        <f>PRODUCT(M50,C50)</f>
         <v>2.85</v>
       </c>
       <c r="O50">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C50*$K$65*(1+$K$66)),0)/K50,0)*K50</f>
         <v>6</v>
       </c>
       <c r="P50" s="7">
-        <f t="shared" si="19"/>
+        <f>O50*M50</f>
         <v>17.100000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A51)-LEN(SUBSTITUTE(A51,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -3718,34 +3725,34 @@
         <v>2.09</v>
       </c>
       <c r="N51" s="7">
-        <f t="shared" si="17"/>
+        <f>PRODUCT(M51,C51)</f>
         <v>2.09</v>
       </c>
       <c r="O51">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C51*$K$65*(1+$K$66)),0)/K51,0)*K51</f>
         <v>6</v>
       </c>
       <c r="P51" s="7">
-        <f t="shared" si="19"/>
+        <f>O51*M51</f>
         <v>12.54</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A52)-LEN(SUBSTITUTE(A52,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -3760,40 +3767,40 @@
         <v>0.37191000000000002</v>
       </c>
       <c r="N52" s="7">
-        <f t="shared" si="17"/>
+        <f>PRODUCT(M52,C52)</f>
         <v>0.37191000000000002</v>
       </c>
       <c r="O52">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C52*$K$65*(1+$K$66)),0)/K52,0)*K52</f>
         <v>10</v>
       </c>
       <c r="P52" s="7">
-        <f t="shared" si="19"/>
+        <f>O52*M52</f>
         <v>3.7191000000000001</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A53)-LEN(SUBSTITUTE(A53,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="I53" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="K53" s="9">
         <v>1</v>
@@ -3806,41 +3813,41 @@
         <v>7.6614999999999993</v>
       </c>
       <c r="N53" s="7">
-        <f t="shared" si="17"/>
+        <f>PRODUCT(M53,C53)</f>
         <v>7.6614999999999993</v>
       </c>
       <c r="O53">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C53*$K$65*(1+$K$66)),0)/K53,0)*K53</f>
         <v>6</v>
       </c>
       <c r="P53" s="7">
-        <f t="shared" si="19"/>
+        <f>O53*M53</f>
         <v>45.968999999999994</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A54)-LEN(SUBSTITUTE(A54,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="G54">
         <v>1332087</v>
       </c>
       <c r="H54" s="2"/>
       <c r="J54" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="K54" s="9">
         <v>1</v>
@@ -3849,40 +3856,40 @@
         <v>1</v>
       </c>
       <c r="N54" s="7">
-        <f t="shared" si="17"/>
+        <f>PRODUCT(M54,C54)</f>
         <v>1</v>
       </c>
       <c r="O54">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C54*$K$65*(1+$K$66)),0)/K54,0)*K54</f>
         <v>6</v>
       </c>
       <c r="P54" s="7">
-        <f t="shared" si="19"/>
+        <f>O54*M54</f>
         <v>6</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A55)-LEN(SUBSTITUTE(A55,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="G55">
         <v>1085308</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="K55" s="9">
         <v>1</v>
@@ -3891,43 +3898,43 @@
         <v>0.28599999999999998</v>
       </c>
       <c r="N55" s="7">
-        <f t="shared" si="17"/>
+        <f>PRODUCT(M55,C55)</f>
         <v>0.28599999999999998</v>
       </c>
       <c r="O55">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C55*$K$65*(1+$K$66)),0)/K55,0)*K55</f>
         <v>6</v>
       </c>
       <c r="P55" s="7">
-        <f t="shared" si="19"/>
+        <f>O55*M55</f>
         <v>1.7159999999999997</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A56)-LEN(SUBSTITUTE(A56,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="G56">
         <v>1466595</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="K56" s="9">
         <v>5</v>
@@ -3936,41 +3943,41 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N56" s="7">
-        <f t="shared" si="17"/>
+        <f>PRODUCT(M56,C56)</f>
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="O56">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C56*$K$65*(1+$K$66)),0)/K56,0)*K56</f>
         <v>10</v>
       </c>
       <c r="P56" s="7">
-        <f t="shared" si="19"/>
+        <f>O56*M56</f>
         <v>0.44999999999999996</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A57)-LEN(SUBSTITUTE(A57,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G57">
         <v>9387129</v>
       </c>
       <c r="H57" s="2"/>
       <c r="J57" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="K57" s="9">
         <v>1</v>
@@ -3979,82 +3986,82 @@
         <v>1.46</v>
       </c>
       <c r="N57" s="7">
-        <f t="shared" si="17"/>
+        <f>PRODUCT(M57,C57)</f>
         <v>1.46</v>
       </c>
       <c r="O57">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C57*$K$65*(1+$K$66)),0)/K57,0)*K57</f>
         <v>6</v>
       </c>
       <c r="P57" s="7">
-        <f t="shared" si="19"/>
+        <f>O57*M57</f>
         <v>8.76</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A58)-LEN(SUBSTITUTE(A58,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>191</v>
+        <v>233</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>134</v>
+        <v>235</v>
       </c>
       <c r="G58">
-        <v>2103565</v>
+        <v>1593292</v>
       </c>
       <c r="H58" s="2"/>
       <c r="J58" s="1" t="s">
-        <v>95</v>
+        <v>234</v>
       </c>
       <c r="K58" s="9">
         <v>1</v>
       </c>
       <c r="M58" s="6">
-        <v>0.873</v>
+        <v>8.07</v>
       </c>
       <c r="N58" s="7">
-        <f t="shared" si="17"/>
-        <v>0.873</v>
+        <f>PRODUCT(M58,C58)</f>
+        <v>8.07</v>
       </c>
       <c r="O58">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C58*$K$65*(1+$K$66)),0)/K58,0)*K58</f>
         <v>6</v>
       </c>
       <c r="P58" s="7">
-        <f t="shared" si="19"/>
-        <v>5.2379999999999995</v>
+        <f>O58*M58</f>
+        <v>48.42</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A59)-LEN(SUBSTITUTE(A59,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
       <c r="I59" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="K59" s="9">
         <v>1</v>
@@ -4063,40 +4070,40 @@
         <v>26.3</v>
       </c>
       <c r="N59" s="7">
-        <f t="shared" si="17"/>
+        <f>PRODUCT(M59,C59)</f>
         <v>26.3</v>
       </c>
       <c r="O59">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C59*$K$65*(1+$K$66)),0)/K59,0)*K59</f>
         <v>6</v>
       </c>
       <c r="P59" s="7">
-        <f t="shared" si="19"/>
+        <f>O59*M59</f>
         <v>157.80000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A60)-LEN(SUBSTITUTE(A60,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="G60">
         <v>2395902</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="K60" s="9">
         <v>1</v>
@@ -4105,37 +4112,37 @@
         <v>1.5</v>
       </c>
       <c r="N60" s="7">
-        <f t="shared" si="17"/>
+        <f>PRODUCT(M60,C60)</f>
         <v>1.5</v>
       </c>
       <c r="O60">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C60*$K$65*(1+$K$66)),0)/K60,0)*K60</f>
         <v>6</v>
       </c>
       <c r="P60" s="7">
-        <f t="shared" si="19"/>
+        <f>O60*M60</f>
         <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C61">
         <v>4</v>
       </c>
       <c r="D61" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A61)-LEN(SUBSTITUTE(A61,",",""))+1</f>
         <v>4</v>
       </c>
       <c r="E61" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K61" s="8">
         <v>1</v>
@@ -4148,40 +4155,40 @@
         <v>2.4100999999999999</v>
       </c>
       <c r="N61" s="7">
-        <f t="shared" si="17"/>
+        <f>PRODUCT(M61,C61)</f>
         <v>9.6403999999999996</v>
       </c>
       <c r="O61">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C61*$K$65*(1+$K$66)),0)/K61,0)*K61</f>
         <v>21</v>
       </c>
       <c r="P61" s="7">
-        <f t="shared" si="19"/>
+        <f>O61*M61</f>
         <v>50.612099999999998</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
       <c r="D62" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A62)-LEN(SUBSTITUTE(A62,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G62">
         <v>2373743</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="K62" s="9">
         <v>1</v>
@@ -4190,34 +4197,34 @@
         <v>0.68700000000000006</v>
       </c>
       <c r="N62" s="7">
-        <f t="shared" si="17"/>
+        <f>PRODUCT(M62,C62)</f>
         <v>0.68700000000000006</v>
       </c>
       <c r="O62">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C62*$K$65*(1+$K$66)),0)/K62,0)*K62</f>
         <v>6</v>
       </c>
       <c r="P62" s="7">
-        <f t="shared" si="19"/>
+        <f>O62*M62</f>
         <v>4.1219999999999999</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63" s="1">
-        <f t="shared" si="4"/>
+        <f>LEN(A63)-LEN(SUBSTITUTE(A63,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K63" s="8">
         <v>1</v>
@@ -4230,34 +4237,34 @@
         <v>9.0090000000000003E-2</v>
       </c>
       <c r="N63" s="7">
-        <f t="shared" si="17"/>
+        <f>PRODUCT(M63,C63)</f>
         <v>9.0090000000000003E-2</v>
       </c>
       <c r="O63">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C63*$K$65*(1+$K$66)),0)/K63,0)*K63</f>
         <v>6</v>
       </c>
       <c r="P63" s="7">
-        <f t="shared" si="19"/>
+        <f>O63*M63</f>
         <v>0.54054000000000002</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64" s="1">
-        <f t="shared" ref="D64" si="20">LEN(A64)-LEN(SUBSTITUTE(A64,",",""))+1</f>
+        <f>LEN(A64)-LEN(SUBSTITUTE(A64,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K64" s="8">
         <v>1</v>
@@ -4270,43 +4277,43 @@
         <v>0.15400000000000003</v>
       </c>
       <c r="N64" s="7">
-        <f t="shared" si="17"/>
+        <f>PRODUCT(M64,C64)</f>
         <v>0.15400000000000003</v>
       </c>
       <c r="O64">
-        <f t="shared" si="18"/>
+        <f>ROUNDUP(ROUNDUP((C64*$K$65*(1+$K$66)),0)/K64,0)*K64</f>
         <v>6</v>
       </c>
       <c r="P64" s="7">
-        <f t="shared" si="19"/>
+        <f>O64*M64</f>
         <v>0.92400000000000015</v>
       </c>
     </row>
     <row r="65" spans="7:18" x14ac:dyDescent="0.25">
       <c r="J65" s="10" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="K65" s="11">
         <v>5</v>
       </c>
       <c r="M65" s="5" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="N65" s="7">
         <f>SUM(N2:N62)</f>
-        <v>111.4401</v>
+        <v>118.48886999999999</v>
       </c>
       <c r="O65" s="5" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="P65" s="7">
         <f>SUM(P2:P64)</f>
-        <v>656.86777999999993</v>
+        <v>698.57209999999998</v>
       </c>
     </row>
     <row r="66" spans="7:18" x14ac:dyDescent="0.25">
       <c r="J66" s="12" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="K66" s="13">
         <v>1E-3</v>
@@ -4316,13 +4323,13 @@
     </row>
     <row r="67" spans="7:18" x14ac:dyDescent="0.25">
       <c r="J67" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="K67">
         <v>0.77</v>
       </c>
       <c r="R67" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="71" spans="7:18" x14ac:dyDescent="0.25">
@@ -4405,7 +4412,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G81">
         <v>9387129</v>
       </c>
@@ -4413,7 +4420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G82">
         <v>2308433</v>
       </c>
@@ -4421,7 +4428,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G83">
         <v>2356152</v>
       </c>
@@ -4429,7 +4436,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="84" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G84">
         <v>1667519</v>
       </c>
@@ -4437,9 +4444,240 @@
         <v>11</v>
       </c>
     </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="1"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="1"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="1"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="1"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="1"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="1"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="1"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="1"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="1"/>
+      <c r="B139" s="1"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="1"/>
+      <c r="B141" s="1"/>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="1"/>
+      <c r="B142" s="1"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="1"/>
+      <c r="B143" s="1"/>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="1"/>
+      <c r="B144" s="1"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="1"/>
+      <c r="B145" s="1"/>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="1"/>
+      <c r="B147" s="1"/>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="1"/>
+      <c r="B148" s="1"/>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="1"/>
+      <c r="B149" s="1"/>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="1"/>
+      <c r="B150" s="1"/>
+    </row>
   </sheetData>
-  <sortState ref="A2:F60">
-    <sortCondition ref="B1"/>
+  <sortState ref="A2:R67">
+    <sortCondition ref="A2"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="F52" r:id="rId1"/>
@@ -4448,9 +4686,9 @@
     <hyperlink ref="F56" r:id="rId4"/>
     <hyperlink ref="F62" r:id="rId5"/>
     <hyperlink ref="F55" r:id="rId6"/>
-    <hyperlink ref="F19" r:id="rId7"/>
+    <hyperlink ref="F18" r:id="rId7"/>
     <hyperlink ref="F59" r:id="rId8"/>
-    <hyperlink ref="F26" r:id="rId9"/>
+    <hyperlink ref="F27" r:id="rId9"/>
     <hyperlink ref="F60" r:id="rId10"/>
     <hyperlink ref="F54" r:id="rId11"/>
     <hyperlink ref="F58" r:id="rId12"/>
@@ -4458,15 +4696,14 @@
     <hyperlink ref="F48" r:id="rId14"/>
     <hyperlink ref="F57" r:id="rId15"/>
     <hyperlink ref="F53" r:id="rId16"/>
-    <hyperlink ref="F27" r:id="rId17"/>
+    <hyperlink ref="F28" r:id="rId17"/>
     <hyperlink ref="F45" r:id="rId18"/>
-    <hyperlink ref="F25" r:id="rId19"/>
-    <hyperlink ref="F15" r:id="rId20"/>
-    <hyperlink ref="G28" r:id="rId21" tooltip="2449396" display="http://onecall.farnell.com/iqd-frequency-products/lfxtal016178/crystal-32-768khz-6pf-smd/dp/2449396"/>
-    <hyperlink ref="J28" r:id="rId22" tooltip="LFXTAL016178" display="http://onecall.farnell.com/iqd-frequency-products/lfxtal016178/crystal-32-768khz-6pf-smd/dp/2449396"/>
-    <hyperlink ref="G71" r:id="rId23" tooltip="2449396" display="http://onecall.farnell.com/iqd-frequency-products/lfxtal016178/crystal-32-768khz-6pf-smd/dp/2449396"/>
+    <hyperlink ref="F26" r:id="rId19"/>
+    <hyperlink ref="F14" r:id="rId20"/>
+    <hyperlink ref="G71" r:id="rId21" tooltip="2449396" display="http://onecall.farnell.com/iqd-frequency-products/lfxtal016178/crystal-32-768khz-6pf-smd/dp/2449396"/>
+    <hyperlink ref="F24" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="79" fitToHeight="0" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId24"/>
+  <pageSetup paperSize="9" scale="79" fitToHeight="0" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added UART 0-ohms and UART Pi 1 header
</commit_message>
<xml_diff>
--- a/AQN-BOM.xlsx
+++ b/AQN-BOM.xlsx
@@ -675,9 +675,6 @@
     <t>D4, D5, D6, D8, D9, D13, D14, D22</t>
   </si>
   <si>
-    <t>I2C_1, I2C_2, I2C_3, I2C_4, I2C_6, I2C_7, I2C_8, I2C_9, I_UART_HUB_1, LOPY_I2C, LOPY_UART0, LOPY_UART1, PI_RS_485, PI_UART, PI_UART_HUB_2, PI_UART_HUB_3</t>
-  </si>
-  <si>
     <t>L2, L3, L4</t>
   </si>
   <si>
@@ -693,9 +690,6 @@
     <t>R7, R23, R24, R29, R30, R31, R32, R33, R34, R42</t>
   </si>
   <si>
-    <t>R8, R12, R15, R17, R41</t>
-  </si>
-  <si>
     <t>R5, R35, R36</t>
   </si>
   <si>
@@ -760,6 +754,12 @@
   </si>
   <si>
     <t>M20-9990246</t>
+  </si>
+  <si>
+    <t>R1, R3, R8, R12, R15, R17, R41</t>
+  </si>
+  <si>
+    <t>I2C_1, I2C_2, I2C_3, I2C_4, I2C_6, I2C_7, I2C_8, I2C_9, I_UART_HUB_1, LOPY_I2C, LOPY_UART0, LOPY_UART1, PI_RS_485, PI_UART, PI_UART_HUB_1, PI_UART_HUB_2, PI_UART_HUB_3</t>
   </si>
 </sst>
 </file>
@@ -1606,10 +1606,10 @@
   <dimension ref="A1:R150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C93" sqref="C93"/>
+      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,7 +1633,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1695,7 +1695,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <f>LEN(A2)-LEN(SUBSTITUTE(A2,",",""))+1</f>
+        <f t="shared" ref="D2:D33" si="0">LEN(A2)-LEN(SUBSTITUTE(A2,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="K2" s="8">
@@ -1705,19 +1705,19 @@
         <v>0.01</v>
       </c>
       <c r="M2" s="6">
-        <f>L2*$K$67</f>
+        <f t="shared" ref="M2:M13" si="1">L2*$K$67</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N2" s="7">
-        <f>PRODUCT(M2,C2)</f>
+        <f t="shared" ref="N2:N16" si="2">PRODUCT(M2,C2)</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="O2">
-        <f>ROUNDUP(ROUNDUP((C2*$K$65*(1+$K$66)),0)/K2,0)*K2</f>
+        <f t="shared" ref="O2:O16" si="3">ROUNDUP(ROUNDUP((C2*$K$65*(1+$K$66)),0)/K2,0)*K2</f>
         <v>6</v>
       </c>
       <c r="P2" s="7">
-        <f>O2*M2</f>
+        <f t="shared" ref="P2:P16" si="4">O2*M2</f>
         <v>4.6200000000000005E-2</v>
       </c>
     </row>
@@ -1732,7 +1732,7 @@
         <v>25</v>
       </c>
       <c r="D3" s="1">
-        <f>LEN(A3)-LEN(SUBSTITUTE(A3,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="E3" t="s">
@@ -1748,19 +1748,19 @@
         <v>0.01</v>
       </c>
       <c r="M3" s="6">
-        <f>L3*$K$67</f>
+        <f t="shared" si="1"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N3" s="7">
-        <f>PRODUCT(M3,C3)</f>
+        <f t="shared" si="2"/>
         <v>0.1925</v>
       </c>
       <c r="O3">
-        <f>ROUNDUP(ROUNDUP((C3*$K$65*(1+$K$66)),0)/K3,0)*K3</f>
+        <f t="shared" si="3"/>
         <v>126</v>
       </c>
       <c r="P3" s="7">
-        <f>O3*M3</f>
+        <f t="shared" si="4"/>
         <v>0.97020000000000006</v>
       </c>
     </row>
@@ -1775,7 +1775,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="1">
-        <f>LEN(A4)-LEN(SUBSTITUTE(A4,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E4" t="s">
@@ -1791,19 +1791,19 @@
         <v>0.01</v>
       </c>
       <c r="M4" s="6">
-        <f>L4*$K$67</f>
+        <f t="shared" si="1"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N4" s="7">
-        <f>PRODUCT(M4,C4)</f>
+        <f t="shared" si="2"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="O4">
-        <f>ROUNDUP(ROUNDUP((C4*$K$65*(1+$K$66)),0)/K4,0)*K4</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="P4" s="7">
-        <f>O4*M4</f>
+        <f t="shared" si="4"/>
         <v>4.6200000000000005E-2</v>
       </c>
     </row>
@@ -1818,7 +1818,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="1">
-        <f>LEN(A5)-LEN(SUBSTITUTE(A5,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E5" t="s">
@@ -1834,19 +1834,19 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="M5" s="6">
-        <f>L5*$K$67</f>
+        <f t="shared" si="1"/>
         <v>3.696E-2</v>
       </c>
       <c r="N5" s="7">
-        <f>PRODUCT(M5,C5)</f>
+        <f t="shared" si="2"/>
         <v>7.392E-2</v>
       </c>
       <c r="O5">
-        <f>ROUNDUP(ROUNDUP((C5*$K$65*(1+$K$66)),0)/K5,0)*K5</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="P5" s="7">
-        <f>O5*M5</f>
+        <f t="shared" si="4"/>
         <v>0.40655999999999998</v>
       </c>
     </row>
@@ -1861,7 +1861,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="1">
-        <f>LEN(A6)-LEN(SUBSTITUTE(A6,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E6" t="s">
@@ -1877,19 +1877,19 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="M6" s="6">
-        <f>L6*$K$67</f>
+        <f t="shared" si="1"/>
         <v>3.1570000000000001E-2</v>
       </c>
       <c r="N6" s="7">
-        <f>PRODUCT(M6,C6)</f>
+        <f t="shared" si="2"/>
         <v>0.12628</v>
       </c>
       <c r="O6">
-        <f>ROUNDUP(ROUNDUP((C6*$K$65*(1+$K$66)),0)/K6,0)*K6</f>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="P6" s="7">
-        <f>O6*M6</f>
+        <f t="shared" si="4"/>
         <v>0.66297000000000006</v>
       </c>
     </row>
@@ -1904,7 +1904,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="1">
-        <f>LEN(A7)-LEN(SUBSTITUTE(A7,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E7" t="s">
@@ -1920,19 +1920,19 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="M7" s="6">
-        <f>L7*$K$67</f>
+        <f t="shared" si="1"/>
         <v>1.155E-2</v>
       </c>
       <c r="N7" s="7">
-        <f>PRODUCT(M7,C7)</f>
+        <f t="shared" si="2"/>
         <v>1.155E-2</v>
       </c>
       <c r="O7">
-        <f>ROUNDUP(ROUNDUP((C7*$K$65*(1+$K$66)),0)/K7,0)*K7</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="P7" s="7">
-        <f>O7*M7</f>
+        <f t="shared" si="4"/>
         <v>6.93E-2</v>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="1">
-        <f>LEN(A8)-LEN(SUBSTITUTE(A8,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E8" t="s">
@@ -1963,19 +1963,19 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="M8" s="6">
-        <f>L8*$K$67</f>
+        <f t="shared" si="1"/>
         <v>3.1570000000000001E-2</v>
       </c>
       <c r="N8" s="7">
-        <f>PRODUCT(M8,C8)</f>
+        <f t="shared" si="2"/>
         <v>0.12628</v>
       </c>
       <c r="O8">
-        <f>ROUNDUP(ROUNDUP((C8*$K$65*(1+$K$66)),0)/K8,0)*K8</f>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="P8" s="7">
-        <f>O8*M8</f>
+        <f t="shared" si="4"/>
         <v>0.66297000000000006</v>
       </c>
     </row>
@@ -1990,7 +1990,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="1">
-        <f>LEN(A9)-LEN(SUBSTITUTE(A9,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E9" t="s">
@@ -2006,19 +2006,19 @@
         <v>0.104</v>
       </c>
       <c r="M9" s="6">
-        <f>L9*$K$67</f>
+        <f t="shared" si="1"/>
         <v>8.0079999999999998E-2</v>
       </c>
       <c r="N9" s="7">
-        <f>PRODUCT(M9,C9)</f>
+        <f t="shared" si="2"/>
         <v>8.0079999999999998E-2</v>
       </c>
       <c r="O9">
-        <f>ROUNDUP(ROUNDUP((C9*$K$65*(1+$K$66)),0)/K9,0)*K9</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="P9" s="7">
-        <f>O9*M9</f>
+        <f t="shared" si="4"/>
         <v>0.48048000000000002</v>
       </c>
     </row>
@@ -2033,7 +2033,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="1">
-        <f>LEN(A10)-LEN(SUBSTITUTE(A10,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E10" t="s">
@@ -2049,19 +2049,19 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="M10" s="6">
-        <f>L10*$K$67</f>
+        <f t="shared" si="1"/>
         <v>3.696E-2</v>
       </c>
       <c r="N10" s="7">
-        <f>PRODUCT(M10,C10)</f>
+        <f t="shared" si="2"/>
         <v>3.696E-2</v>
       </c>
       <c r="O10">
-        <f>ROUNDUP(ROUNDUP((C10*$K$65*(1+$K$66)),0)/K10,0)*K10</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="P10" s="7">
-        <f>O10*M10</f>
+        <f t="shared" si="4"/>
         <v>0.22176000000000001</v>
       </c>
     </row>
@@ -2076,7 +2076,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="1">
-        <f>LEN(A11)-LEN(SUBSTITUTE(A11,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E11" t="s">
@@ -2092,19 +2092,19 @@
         <v>1.4E-2</v>
       </c>
       <c r="M11" s="6">
-        <f>L11*$K$67</f>
+        <f t="shared" si="1"/>
         <v>1.078E-2</v>
       </c>
       <c r="N11" s="7">
-        <f>PRODUCT(M11,C11)</f>
+        <f t="shared" si="2"/>
         <v>4.3119999999999999E-2</v>
       </c>
       <c r="O11">
-        <f>ROUNDUP(ROUNDUP((C11*$K$65*(1+$K$66)),0)/K11,0)*K11</f>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="P11" s="7">
-        <f>O11*M11</f>
+        <f t="shared" si="4"/>
         <v>0.22638</v>
       </c>
     </row>
@@ -2119,7 +2119,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="1">
-        <f>LEN(A12)-LEN(SUBSTITUTE(A12,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E12" t="s">
@@ -2135,19 +2135,19 @@
         <v>1.4E-2</v>
       </c>
       <c r="M12" s="6">
-        <f>L12*$K$67</f>
+        <f t="shared" si="1"/>
         <v>1.078E-2</v>
       </c>
       <c r="N12" s="7">
-        <f>PRODUCT(M12,C12)</f>
+        <f t="shared" si="2"/>
         <v>8.6239999999999997E-2</v>
       </c>
       <c r="O12">
-        <f>ROUNDUP(ROUNDUP((C12*$K$65*(1+$K$66)),0)/K12,0)*K12</f>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="P12" s="7">
-        <f>O12*M12</f>
+        <f t="shared" si="4"/>
         <v>0.44197999999999998</v>
       </c>
     </row>
@@ -2162,7 +2162,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="1">
-        <f>LEN(A13)-LEN(SUBSTITUTE(A13,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E13" t="s">
@@ -2178,19 +2178,19 @@
         <v>1.4E-2</v>
       </c>
       <c r="M13" s="6">
-        <f>L13*$K$67</f>
+        <f t="shared" si="1"/>
         <v>1.078E-2</v>
       </c>
       <c r="N13" s="7">
-        <f>PRODUCT(M13,C13)</f>
+        <f t="shared" si="2"/>
         <v>5.3899999999999997E-2</v>
       </c>
       <c r="O13">
-        <f>ROUNDUP(ROUNDUP((C13*$K$65*(1+$K$66)),0)/K13,0)*K13</f>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="P13" s="7">
-        <f>O13*M13</f>
+        <f t="shared" si="4"/>
         <v>0.28027999999999997</v>
       </c>
     </row>
@@ -2202,7 +2202,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="1">
-        <f>LEN(A14)-LEN(SUBSTITUTE(A14,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -2222,15 +2222,15 @@
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="N14" s="7">
-        <f>PRODUCT(M14,C14)</f>
+        <f t="shared" si="2"/>
         <v>0.20799999999999999</v>
       </c>
       <c r="O14">
-        <f>ROUNDUP(ROUNDUP((C14*$K$65*(1+$K$66)),0)/K14,0)*K14</f>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="P14" s="7">
-        <f>O14*M14</f>
+        <f t="shared" si="4"/>
         <v>1.0919999999999999</v>
       </c>
     </row>
@@ -2243,7 +2243,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="1">
-        <f>LEN(A15)-LEN(SUBSTITUTE(A15,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G15">
@@ -2260,21 +2260,21 @@
         <v>7.5459999999999999E-2</v>
       </c>
       <c r="N15" s="7">
-        <f>PRODUCT(M15,C15)</f>
+        <f t="shared" si="2"/>
         <v>7.5459999999999999E-2</v>
       </c>
       <c r="O15">
-        <f>ROUNDUP(ROUNDUP((C15*$K$65*(1+$K$66)),0)/K15,0)*K15</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="P15" s="7">
-        <f>O15*M15</f>
+        <f t="shared" si="4"/>
         <v>0.45276</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>99</v>
@@ -2283,7 +2283,7 @@
         <v>35</v>
       </c>
       <c r="D16" s="1">
-        <f>LEN(A16)-LEN(SUBSTITUTE(A16,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="J16" s="1" t="s">
@@ -2300,15 +2300,15 @@
         <v>3.619E-2</v>
       </c>
       <c r="N16" s="7">
-        <f>PRODUCT(M16,C16)</f>
+        <f t="shared" si="2"/>
         <v>1.2666500000000001</v>
       </c>
       <c r="O16">
-        <f>ROUNDUP(ROUNDUP((C16*$K$65*(1+$K$66)),0)/K16,0)*K16</f>
+        <f t="shared" si="3"/>
         <v>176</v>
       </c>
       <c r="P16" s="7">
-        <f>O16*M16</f>
+        <f t="shared" si="4"/>
         <v>6.36944</v>
       </c>
     </row>
@@ -2321,7 +2321,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="1">
-        <f>LEN(A17)-LEN(SUBSTITUTE(A17,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I17" t="s">
@@ -2331,20 +2331,20 @@
       <c r="M17" s="6"/>
       <c r="N17" s="7"/>
       <c r="P17" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>217</v>
+        <v>245</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D18" s="1">
-        <f>LEN(A18)-LEN(SUBSTITUTE(A18,",",""))+1</f>
-        <v>16</v>
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>120</v>
@@ -2360,16 +2360,16 @@
         <v>0.16600000000000001</v>
       </c>
       <c r="N18" s="7">
-        <f>PRODUCT(M18,C18)</f>
-        <v>2.6560000000000001</v>
+        <f t="shared" ref="N18:N64" si="5">PRODUCT(M18,C18)</f>
+        <v>2.8220000000000001</v>
       </c>
       <c r="O18">
-        <f>ROUNDUP(ROUNDUP((C18*$K$65*(1+$K$66)),0)/K18,0)*K18</f>
-        <v>85</v>
+        <f t="shared" ref="O18:O64" si="6">ROUNDUP(ROUNDUP((C18*$K$65*(1+$K$66)),0)/K18,0)*K18</f>
+        <v>90</v>
       </c>
       <c r="P18" s="7">
-        <f>O18*M18</f>
-        <v>14.110000000000001</v>
+        <f t="shared" ref="P18:P64" si="7">O18*M18</f>
+        <v>14.940000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -2383,7 +2383,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="1">
-        <f>LEN(A19)-LEN(SUBSTITUTE(A19,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E19" t="s">
@@ -2403,37 +2403,37 @@
         <v>7.0069999999999993E-2</v>
       </c>
       <c r="N19" s="7">
-        <f>PRODUCT(M19,C19)</f>
+        <f t="shared" si="5"/>
         <v>7.0069999999999993E-2</v>
       </c>
       <c r="O19">
-        <f>ROUNDUP(ROUNDUP((C19*$K$65*(1+$K$66)),0)/K19,0)*K19</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P19" s="7">
-        <f>O19*M19</f>
+        <f t="shared" si="7"/>
         <v>0.42041999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>235</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1">
-        <f>LEN(A20)-LEN(SUBSTITUTE(A20,",",""))+1</f>
-        <v>1</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="J20" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K20" s="8">
         <v>1</v>
@@ -2446,15 +2446,15 @@
         <v>1.617E-2</v>
       </c>
       <c r="N20" s="7">
-        <f>PRODUCT(M20,C20)</f>
+        <f t="shared" si="5"/>
         <v>1.617E-2</v>
       </c>
       <c r="O20">
-        <f>ROUNDUP(ROUNDUP((C20*$K$65*(1+$K$66)),0)/K20,0)*K20</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P20" s="7">
-        <f>O20*M20</f>
+        <f t="shared" si="7"/>
         <v>9.7019999999999995E-2</v>
       </c>
     </row>
@@ -2469,7 +2469,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="1">
-        <f>LEN(A21)-LEN(SUBSTITUTE(A21,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E21" t="s">
@@ -2486,15 +2486,15 @@
         <v>8.3930000000000005E-2</v>
       </c>
       <c r="N21" s="7">
-        <f>PRODUCT(M21,C21)</f>
+        <f t="shared" si="5"/>
         <v>8.3930000000000005E-2</v>
       </c>
       <c r="O21">
-        <f>ROUNDUP(ROUNDUP((C21*$K$65*(1+$K$66)),0)/K21,0)*K21</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P21" s="7">
-        <f>O21*M21</f>
+        <f t="shared" si="7"/>
         <v>0.50358000000000003</v>
       </c>
     </row>
@@ -2509,7 +2509,7 @@
         <v>2</v>
       </c>
       <c r="D22" s="1">
-        <f>LEN(A22)-LEN(SUBSTITUTE(A22,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E22" t="s">
@@ -2529,15 +2529,15 @@
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N22" s="7">
-        <f>PRODUCT(M22,C22)</f>
+        <f t="shared" si="5"/>
         <v>1.54E-2</v>
       </c>
       <c r="O22">
-        <f>ROUNDUP(ROUNDUP((C22*$K$65*(1+$K$66)),0)/K22,0)*K22</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="P22" s="7">
-        <f>O22*M22</f>
+        <f t="shared" si="7"/>
         <v>8.4699999999999998E-2</v>
       </c>
     </row>
@@ -2552,7 +2552,7 @@
         <v>6</v>
       </c>
       <c r="D23" s="1">
-        <f>LEN(A23)-LEN(SUBSTITUTE(A23,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E23" t="s">
@@ -2572,41 +2572,41 @@
         <v>1.9250000000000003E-2</v>
       </c>
       <c r="N23" s="7">
-        <f>PRODUCT(M23,C23)</f>
+        <f t="shared" si="5"/>
         <v>0.11550000000000002</v>
       </c>
       <c r="O23">
-        <f>ROUNDUP(ROUNDUP((C23*$K$65*(1+$K$66)),0)/K23,0)*K23</f>
+        <f t="shared" si="6"/>
         <v>31</v>
       </c>
       <c r="P23" s="7">
-        <f>O23*M23</f>
+        <f t="shared" si="7"/>
         <v>0.59675000000000011</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C24">
         <v>2</v>
       </c>
       <c r="D24" s="1">
-        <f>LEN(A24)-LEN(SUBSTITUTE(A24,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="G24" t="s">
+        <v>242</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="G24" t="s">
-        <v>244</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="K24" s="8">
         <v>10</v>
@@ -2615,21 +2615,21 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="N24" s="7">
-        <f>PRODUCT(M24,C24)</f>
+        <f t="shared" si="5"/>
         <v>0.13</v>
       </c>
       <c r="O24">
-        <f>ROUNDUP(ROUNDUP((C24*$K$65*(1+$K$66)),0)/K24,0)*K24</f>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="P24" s="7">
-        <f>O24*M24</f>
+        <f t="shared" si="7"/>
         <v>1.3</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>59</v>
@@ -2638,7 +2638,7 @@
         <v>3</v>
       </c>
       <c r="D25" s="1">
-        <f>LEN(A25)-LEN(SUBSTITUTE(A25,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E25" t="s">
@@ -2658,15 +2658,15 @@
         <v>1.155E-2</v>
       </c>
       <c r="N25" s="7">
-        <f>PRODUCT(M25,C25)</f>
+        <f t="shared" si="5"/>
         <v>3.465E-2</v>
       </c>
       <c r="O25">
-        <f>ROUNDUP(ROUNDUP((C25*$K$65*(1+$K$66)),0)/K25,0)*K25</f>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="P25" s="7">
-        <f>O25*M25</f>
+        <f t="shared" si="7"/>
         <v>0.18479999999999999</v>
       </c>
     </row>
@@ -2678,7 +2678,7 @@
         <v>2</v>
       </c>
       <c r="D26" s="1">
-        <f>LEN(A26)-LEN(SUBSTITUTE(A26,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F26" s="2" t="s">
@@ -2698,28 +2698,28 @@
         <v>1.41</v>
       </c>
       <c r="N26" s="7">
-        <f>PRODUCT(M26,C26)</f>
+        <f t="shared" si="5"/>
         <v>2.82</v>
       </c>
       <c r="O26">
-        <f>ROUNDUP(ROUNDUP((C26*$K$65*(1+$K$66)),0)/K26,0)*K26</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="P26" s="7">
-        <f>O26*M26</f>
+        <f t="shared" si="7"/>
         <v>15.51</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27">
         <v>9</v>
       </c>
       <c r="D27" s="1">
-        <f>LEN(A27)-LEN(SUBSTITUTE(A27,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F27" s="2" t="s">
@@ -2736,15 +2736,15 @@
         <v>0.23599999999999999</v>
       </c>
       <c r="N27" s="7">
-        <f>PRODUCT(M27,C27)</f>
+        <f t="shared" si="5"/>
         <v>2.1239999999999997</v>
       </c>
       <c r="O27">
-        <f>ROUNDUP(ROUNDUP((C27*$K$65*(1+$K$66)),0)/K27,0)*K27</f>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="P27" s="7">
-        <f>O27*M27</f>
+        <f t="shared" si="7"/>
         <v>11.799999999999999</v>
       </c>
     </row>
@@ -2757,7 +2757,7 @@
         <v>1</v>
       </c>
       <c r="D28" s="1">
-        <f>LEN(A28)-LEN(SUBSTITUTE(A28,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F28" s="2" t="s">
@@ -2775,19 +2775,19 @@
         <v>42.22</v>
       </c>
       <c r="M28" s="6">
-        <f>L28*$K$67</f>
+        <f t="shared" ref="M28:M34" si="8">L28*$K$67</f>
         <v>32.509399999999999</v>
       </c>
       <c r="N28" s="7">
-        <f>PRODUCT(M28,C28)</f>
+        <f t="shared" si="5"/>
         <v>32.509399999999999</v>
       </c>
       <c r="O28">
-        <f>ROUNDUP(ROUNDUP((C28*$K$65*(1+$K$66)),0)/K28,0)*K28</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P28" s="7">
-        <f>O28*M28</f>
+        <f t="shared" si="7"/>
         <v>195.0564</v>
       </c>
     </row>
@@ -2802,7 +2802,7 @@
         <v>2</v>
       </c>
       <c r="D29" s="1">
-        <f>LEN(A29)-LEN(SUBSTITUTE(A29,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E29" t="s">
@@ -2818,19 +2818,19 @@
         <v>0.13600000000000001</v>
       </c>
       <c r="M29" s="6">
-        <f>L29*$K$67</f>
+        <f t="shared" si="8"/>
         <v>0.10472000000000001</v>
       </c>
       <c r="N29" s="7">
-        <f>PRODUCT(M29,C29)</f>
+        <f t="shared" si="5"/>
         <v>0.20944000000000002</v>
       </c>
       <c r="O29">
-        <f>ROUNDUP(ROUNDUP((C29*$K$65*(1+$K$66)),0)/K29,0)*K29</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="P29" s="7">
-        <f>O29*M29</f>
+        <f t="shared" si="7"/>
         <v>1.1519200000000001</v>
       </c>
     </row>
@@ -2845,7 +2845,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="1">
-        <f>LEN(A30)-LEN(SUBSTITUTE(A30,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E30" t="s">
@@ -2861,19 +2861,19 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="M30" s="6">
-        <f>L30*$K$67</f>
+        <f t="shared" si="8"/>
         <v>2.5410000000000002E-2</v>
       </c>
       <c r="N30" s="7">
-        <f>PRODUCT(M30,C30)</f>
+        <f t="shared" si="5"/>
         <v>2.5410000000000002E-2</v>
       </c>
       <c r="O30">
-        <f>ROUNDUP(ROUNDUP((C30*$K$65*(1+$K$66)),0)/K30,0)*K30</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P30" s="7">
-        <f>O30*M30</f>
+        <f t="shared" si="7"/>
         <v>0.15246000000000001</v>
       </c>
     </row>
@@ -2882,13 +2882,13 @@
         <v>191</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31" s="1">
-        <f>LEN(A31)-LEN(SUBSTITUTE(A31,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E31" t="s">
@@ -2902,19 +2902,19 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="M31" s="6">
-        <f>L31*$K$67</f>
+        <f t="shared" si="8"/>
         <v>2.5410000000000002E-2</v>
       </c>
       <c r="N31" s="7">
-        <f>PRODUCT(M31,C31)</f>
+        <f t="shared" si="5"/>
         <v>2.5410000000000002E-2</v>
       </c>
       <c r="O31">
-        <f>ROUNDUP(ROUNDUP((C31*$K$65*(1+$K$66)),0)/K31,0)*K31</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P31" s="7">
-        <f>O31*M31</f>
+        <f t="shared" si="7"/>
         <v>0.15246000000000001</v>
       </c>
     </row>
@@ -2923,13 +2923,13 @@
         <v>199</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
       <c r="D32" s="1">
-        <f>LEN(A32)-LEN(SUBSTITUTE(A32,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E32" t="s">
@@ -2943,19 +2943,19 @@
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="M32" s="6">
-        <f>L32*$K$67</f>
+        <f t="shared" si="8"/>
         <v>8.4700000000000001E-3</v>
       </c>
       <c r="N32" s="7">
-        <f>PRODUCT(M32,C32)</f>
+        <f t="shared" si="5"/>
         <v>1.694E-2</v>
       </c>
       <c r="O32">
-        <f>ROUNDUP(ROUNDUP((C32*$K$65*(1+$K$66)),0)/K32,0)*K32</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="P32" s="7">
-        <f>O32*M32</f>
+        <f t="shared" si="7"/>
         <v>9.3170000000000003E-2</v>
       </c>
     </row>
@@ -2970,7 +2970,7 @@
         <v>6</v>
       </c>
       <c r="D33" s="1">
-        <f>LEN(A33)-LEN(SUBSTITUTE(A33,",",""))+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E33" t="s">
@@ -2986,19 +2986,19 @@
         <v>0.01</v>
       </c>
       <c r="M33" s="6">
-        <f>L33*$K$67</f>
+        <f t="shared" si="8"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N33" s="7">
-        <f>PRODUCT(M33,C33)</f>
+        <f t="shared" si="5"/>
         <v>4.6200000000000005E-2</v>
       </c>
       <c r="O33">
-        <f>ROUNDUP(ROUNDUP((C33*$K$65*(1+$K$66)),0)/K33,0)*K33</f>
+        <f t="shared" si="6"/>
         <v>31</v>
       </c>
       <c r="P33" s="7">
-        <f>O33*M33</f>
+        <f t="shared" si="7"/>
         <v>0.2387</v>
       </c>
     </row>
@@ -3013,7 +3013,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="1">
-        <f>LEN(A34)-LEN(SUBSTITUTE(A34,",",""))+1</f>
+        <f t="shared" ref="D34:D64" si="9">LEN(A34)-LEN(SUBSTITUTE(A34,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="E34" t="s">
@@ -3029,19 +3029,19 @@
         <v>0.01</v>
       </c>
       <c r="M34" s="6">
-        <f>L34*$K$67</f>
+        <f t="shared" si="8"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N34" s="7">
-        <f>PRODUCT(M34,C34)</f>
+        <f t="shared" si="5"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="O34">
-        <f>ROUNDUP(ROUNDUP((C34*$K$65*(1+$K$66)),0)/K34,0)*K34</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P34" s="7">
-        <f>O34*M34</f>
+        <f t="shared" si="7"/>
         <v>4.6200000000000005E-2</v>
       </c>
     </row>
@@ -3054,14 +3054,14 @@
         <v>1</v>
       </c>
       <c r="D35" s="1">
-        <f>LEN(A35)-LEN(SUBSTITUTE(A35,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E35" t="s">
         <v>210</v>
       </c>
       <c r="F35" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G35">
         <v>9238379</v>
@@ -3074,15 +3074,15 @@
         <v>1.35E-2</v>
       </c>
       <c r="N35" s="7">
-        <f>PRODUCT(M35,C35)</f>
+        <f t="shared" si="5"/>
         <v>1.35E-2</v>
       </c>
       <c r="O35">
-        <f>ROUNDUP(ROUNDUP((C35*$K$65*(1+$K$66)),0)/K35,0)*K35</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="P35" s="7">
-        <f>O35*M35</f>
+        <f t="shared" si="7"/>
         <v>0.13500000000000001</v>
       </c>
     </row>
@@ -3097,7 +3097,7 @@
         <v>1</v>
       </c>
       <c r="D36" s="1">
-        <f>LEN(A36)-LEN(SUBSTITUTE(A36,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E36" t="s">
@@ -3113,19 +3113,19 @@
         <v>0.01</v>
       </c>
       <c r="M36" s="6">
-        <f>L36*$K$67</f>
+        <f t="shared" ref="M36:M44" si="10">L36*$K$67</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N36" s="7">
-        <f>PRODUCT(M36,C36)</f>
+        <f t="shared" si="5"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="O36">
-        <f>ROUNDUP(ROUNDUP((C36*$K$65*(1+$K$66)),0)/K36,0)*K36</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P36" s="7">
-        <f>O36*M36</f>
+        <f t="shared" si="7"/>
         <v>4.6200000000000005E-2</v>
       </c>
     </row>
@@ -3140,7 +3140,7 @@
         <v>2</v>
       </c>
       <c r="D37" s="1">
-        <f>LEN(A37)-LEN(SUBSTITUTE(A37,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="E37" t="s">
@@ -3156,19 +3156,19 @@
         <v>0.01</v>
       </c>
       <c r="M37" s="6">
-        <f>L37*$K$67</f>
+        <f t="shared" si="10"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N37" s="7">
-        <f>PRODUCT(M37,C37)</f>
+        <f t="shared" si="5"/>
         <v>1.54E-2</v>
       </c>
       <c r="O37">
-        <f>ROUNDUP(ROUNDUP((C37*$K$65*(1+$K$66)),0)/K37,0)*K37</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="P37" s="7">
-        <f>O37*M37</f>
+        <f t="shared" si="7"/>
         <v>8.4699999999999998E-2</v>
       </c>
     </row>
@@ -3183,7 +3183,7 @@
         <v>2</v>
       </c>
       <c r="D38" s="1">
-        <f>LEN(A38)-LEN(SUBSTITUTE(A38,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="E38" t="s">
@@ -3199,19 +3199,19 @@
         <v>0.01</v>
       </c>
       <c r="M38" s="6">
-        <f>L38*$K$67</f>
+        <f t="shared" si="10"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N38" s="7">
-        <f>PRODUCT(M38,C38)</f>
+        <f t="shared" si="5"/>
         <v>1.54E-2</v>
       </c>
       <c r="O38">
-        <f>ROUNDUP(ROUNDUP((C38*$K$65*(1+$K$66)),0)/K38,0)*K38</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="P38" s="7">
-        <f>O38*M38</f>
+        <f t="shared" si="7"/>
         <v>8.4699999999999998E-2</v>
       </c>
     </row>
@@ -3226,7 +3226,7 @@
         <v>3</v>
       </c>
       <c r="D39" s="1">
-        <f>LEN(A39)-LEN(SUBSTITUTE(A39,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="E39" t="s">
@@ -3242,19 +3242,19 @@
         <v>0.01</v>
       </c>
       <c r="M39" s="6">
-        <f>L39*$K$67</f>
+        <f t="shared" si="10"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N39" s="7">
-        <f>PRODUCT(M39,C39)</f>
+        <f t="shared" si="5"/>
         <v>2.3100000000000002E-2</v>
       </c>
       <c r="O39">
-        <f>ROUNDUP(ROUNDUP((C39*$K$65*(1+$K$66)),0)/K39,0)*K39</f>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="P39" s="7">
-        <f>O39*M39</f>
+        <f t="shared" si="7"/>
         <v>0.1232</v>
       </c>
     </row>
@@ -3263,13 +3263,13 @@
         <v>202</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" s="1">
-        <f>LEN(A40)-LEN(SUBSTITUTE(A40,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J40" s="1"/>
@@ -3280,25 +3280,25 @@
         <v>0.01</v>
       </c>
       <c r="M40" s="6">
-        <f>L40*$K$67</f>
+        <f t="shared" si="10"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N40" s="7">
-        <f>PRODUCT(M40,C40)</f>
+        <f t="shared" si="5"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="O40">
-        <f>ROUNDUP(ROUNDUP((C40*$K$65*(1+$K$66)),0)/K40,0)*K40</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P40" s="7">
-        <f>O40*M40</f>
+        <f t="shared" si="7"/>
         <v>4.6200000000000005E-2</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>37</v>
@@ -3307,7 +3307,7 @@
         <v>3</v>
       </c>
       <c r="D41" s="1">
-        <f>LEN(A41)-LEN(SUBSTITUTE(A41,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="E41" t="s">
@@ -3323,25 +3323,25 @@
         <v>0.01</v>
       </c>
       <c r="M41" s="6">
-        <f>L41*$K$67</f>
+        <f t="shared" si="10"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N41" s="7">
-        <f>PRODUCT(M41,C41)</f>
+        <f t="shared" si="5"/>
         <v>2.3100000000000002E-2</v>
       </c>
       <c r="O41">
-        <f>ROUNDUP(ROUNDUP((C41*$K$65*(1+$K$66)),0)/K41,0)*K41</f>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="P41" s="7">
-        <f>O41*M41</f>
+        <f t="shared" si="7"/>
         <v>0.1232</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>57</v>
@@ -3350,7 +3350,7 @@
         <v>10</v>
       </c>
       <c r="D42" s="1">
-        <f>LEN(A42)-LEN(SUBSTITUTE(A42,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="E42" t="s">
@@ -3366,35 +3366,35 @@
         <v>0.01</v>
       </c>
       <c r="M42" s="6">
-        <f>L42*$K$67</f>
+        <f t="shared" si="10"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N42" s="7">
-        <f>PRODUCT(M42,C42)</f>
+        <f t="shared" si="5"/>
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="O42">
-        <f>ROUNDUP(ROUNDUP((C42*$K$65*(1+$K$66)),0)/K42,0)*K42</f>
+        <f t="shared" si="6"/>
         <v>51</v>
       </c>
       <c r="P42" s="7">
-        <f>O42*M42</f>
+        <f t="shared" si="7"/>
         <v>0.39269999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>223</v>
+        <v>244</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C43">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D43" s="1">
-        <f>LEN(A43)-LEN(SUBSTITUTE(A43,",",""))+1</f>
-        <v>5</v>
+        <f t="shared" si="9"/>
+        <v>7</v>
       </c>
       <c r="E43" t="s">
         <v>4</v>
@@ -3409,20 +3409,20 @@
         <v>0.01</v>
       </c>
       <c r="M43" s="6">
-        <f>L43*$K$67</f>
+        <f t="shared" si="10"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N43" s="7">
-        <f>PRODUCT(M43,C43)</f>
-        <v>3.85E-2</v>
+        <f t="shared" si="5"/>
+        <v>5.3900000000000003E-2</v>
       </c>
       <c r="O43">
-        <f>ROUNDUP(ROUNDUP((C43*$K$65*(1+$K$66)),0)/K43,0)*K43</f>
-        <v>26</v>
+        <f t="shared" si="6"/>
+        <v>36</v>
       </c>
       <c r="P43" s="7">
-        <f>O43*M43</f>
-        <v>0.20020000000000002</v>
+        <f t="shared" si="7"/>
+        <v>0.2772</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -3436,7 +3436,7 @@
         <v>3</v>
       </c>
       <c r="D44" s="1">
-        <f>LEN(A44)-LEN(SUBSTITUTE(A44,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="E44" t="s">
@@ -3452,19 +3452,19 @@
         <v>0.01</v>
       </c>
       <c r="M44" s="6">
-        <f>L44*$K$67</f>
+        <f t="shared" si="10"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="N44" s="7">
-        <f>PRODUCT(M44,C44)</f>
+        <f t="shared" si="5"/>
         <v>2.3100000000000002E-2</v>
       </c>
       <c r="O44">
-        <f>ROUNDUP(ROUNDUP((C44*$K$65*(1+$K$66)),0)/K44,0)*K44</f>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="P44" s="7">
-        <f>O44*M44</f>
+        <f t="shared" si="7"/>
         <v>0.1232</v>
       </c>
     </row>
@@ -3476,7 +3476,7 @@
         <v>1</v>
       </c>
       <c r="D45" s="1">
-        <f>LEN(A45)-LEN(SUBSTITUTE(A45,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="F45" s="2" t="s">
@@ -3496,30 +3496,30 @@
         <v>5.39</v>
       </c>
       <c r="N45" s="7">
-        <f>PRODUCT(M45,C45)</f>
+        <f t="shared" si="5"/>
         <v>5.39</v>
       </c>
       <c r="O45">
-        <f>ROUNDUP(ROUNDUP((C45*$K$65*(1+$K$66)),0)/K45,0)*K45</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P45" s="7">
-        <f>O45*M45</f>
+        <f t="shared" si="7"/>
         <v>32.339999999999996</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C46">
         <v>4</v>
       </c>
       <c r="D46" s="1">
-        <f>LEN(A46)-LEN(SUBSTITUTE(A46,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="J46" s="1"/>
@@ -3530,15 +3530,15 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="N46" s="7">
-        <f>PRODUCT(M46,C46)</f>
+        <f t="shared" si="5"/>
         <v>0.40799999999999997</v>
       </c>
       <c r="O46">
-        <f>ROUNDUP(ROUNDUP((C46*$K$65*(1+$K$66)),0)/K46,0)*K46</f>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="P46" s="7">
-        <f>O46*M46</f>
+        <f t="shared" si="7"/>
         <v>2.1419999999999999</v>
       </c>
     </row>
@@ -3551,7 +3551,7 @@
         <v>17</v>
       </c>
       <c r="D47" s="1">
-        <f>LEN(A47)-LEN(SUBSTITUTE(A47,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="I47" t="s">
@@ -3564,15 +3564,15 @@
         <v>0</v>
       </c>
       <c r="N47" s="7">
-        <f>PRODUCT(M47,C47)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O47">
-        <f>ROUNDUP(ROUNDUP((C47*$K$65*(1+$K$66)),0)/K47,0)*K47</f>
+        <f t="shared" si="6"/>
         <v>86</v>
       </c>
       <c r="P47" s="7">
-        <f>O47*M47</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3587,7 +3587,7 @@
         <v>2</v>
       </c>
       <c r="D48" s="1">
-        <f>LEN(A48)-LEN(SUBSTITUTE(A48,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="F48" s="2" t="s">
@@ -3607,15 +3607,15 @@
         <v>3.41</v>
       </c>
       <c r="N48" s="7">
-        <f>PRODUCT(M48,C48)</f>
+        <f t="shared" si="5"/>
         <v>6.82</v>
       </c>
       <c r="O48">
-        <f>ROUNDUP(ROUNDUP((C48*$K$65*(1+$K$66)),0)/K48,0)*K48</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="P48" s="7">
-        <f>O48*M48</f>
+        <f t="shared" si="7"/>
         <v>37.510000000000005</v>
       </c>
     </row>
@@ -3630,7 +3630,7 @@
         <v>1</v>
       </c>
       <c r="D49" s="1">
-        <f>LEN(A49)-LEN(SUBSTITUTE(A49,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="F49" s="2" t="s">
@@ -3647,15 +3647,15 @@
         <v>0.36199999999999999</v>
       </c>
       <c r="N49" s="7">
-        <f>PRODUCT(M49,C49)</f>
+        <f t="shared" si="5"/>
         <v>0.36199999999999999</v>
       </c>
       <c r="O49">
-        <f>ROUNDUP(ROUNDUP((C49*$K$65*(1+$K$66)),0)/K49,0)*K49</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="P49" s="7">
-        <f>O49*M49</f>
+        <f t="shared" si="7"/>
         <v>3.62</v>
       </c>
     </row>
@@ -3670,7 +3670,7 @@
         <v>1</v>
       </c>
       <c r="D50" s="1">
-        <f>LEN(A50)-LEN(SUBSTITUTE(A50,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="F50" s="2" t="s">
@@ -3687,15 +3687,15 @@
         <v>2.85</v>
       </c>
       <c r="N50" s="7">
-        <f>PRODUCT(M50,C50)</f>
+        <f t="shared" si="5"/>
         <v>2.85</v>
       </c>
       <c r="O50">
-        <f>ROUNDUP(ROUNDUP((C50*$K$65*(1+$K$66)),0)/K50,0)*K50</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P50" s="7">
-        <f>O50*M50</f>
+        <f t="shared" si="7"/>
         <v>17.100000000000001</v>
       </c>
     </row>
@@ -3710,7 +3710,7 @@
         <v>1</v>
       </c>
       <c r="D51" s="1">
-        <f>LEN(A51)-LEN(SUBSTITUTE(A51,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="F51" s="2" t="s">
@@ -3725,15 +3725,15 @@
         <v>2.09</v>
       </c>
       <c r="N51" s="7">
-        <f>PRODUCT(M51,C51)</f>
+        <f t="shared" si="5"/>
         <v>2.09</v>
       </c>
       <c r="O51">
-        <f>ROUNDUP(ROUNDUP((C51*$K$65*(1+$K$66)),0)/K51,0)*K51</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P51" s="7">
-        <f>O51*M51</f>
+        <f t="shared" si="7"/>
         <v>12.54</v>
       </c>
     </row>
@@ -3748,7 +3748,7 @@
         <v>1</v>
       </c>
       <c r="D52" s="1">
-        <f>LEN(A52)-LEN(SUBSTITUTE(A52,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="F52" s="2" t="s">
@@ -3767,15 +3767,15 @@
         <v>0.37191000000000002</v>
       </c>
       <c r="N52" s="7">
-        <f>PRODUCT(M52,C52)</f>
+        <f t="shared" si="5"/>
         <v>0.37191000000000002</v>
       </c>
       <c r="O52">
-        <f>ROUNDUP(ROUNDUP((C52*$K$65*(1+$K$66)),0)/K52,0)*K52</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="P52" s="7">
-        <f>O52*M52</f>
+        <f t="shared" si="7"/>
         <v>3.7191000000000001</v>
       </c>
     </row>
@@ -3788,7 +3788,7 @@
         <v>1</v>
       </c>
       <c r="D53" s="1">
-        <f>LEN(A53)-LEN(SUBSTITUTE(A53,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E53" t="s">
@@ -3813,15 +3813,15 @@
         <v>7.6614999999999993</v>
       </c>
       <c r="N53" s="7">
-        <f>PRODUCT(M53,C53)</f>
+        <f t="shared" si="5"/>
         <v>7.6614999999999993</v>
       </c>
       <c r="O53">
-        <f>ROUNDUP(ROUNDUP((C53*$K$65*(1+$K$66)),0)/K53,0)*K53</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P53" s="7">
-        <f>O53*M53</f>
+        <f t="shared" si="7"/>
         <v>45.968999999999994</v>
       </c>
     </row>
@@ -3836,7 +3836,7 @@
         <v>1</v>
       </c>
       <c r="D54" s="1">
-        <f>LEN(A54)-LEN(SUBSTITUTE(A54,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="F54" s="2" t="s">
@@ -3856,15 +3856,15 @@
         <v>1</v>
       </c>
       <c r="N54" s="7">
-        <f>PRODUCT(M54,C54)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="O54">
-        <f>ROUNDUP(ROUNDUP((C54*$K$65*(1+$K$66)),0)/K54,0)*K54</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P54" s="7">
-        <f>O54*M54</f>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
     </row>
@@ -3879,7 +3879,7 @@
         <v>1</v>
       </c>
       <c r="D55" s="1">
-        <f>LEN(A55)-LEN(SUBSTITUTE(A55,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="F55" s="2" t="s">
@@ -3898,15 +3898,15 @@
         <v>0.28599999999999998</v>
       </c>
       <c r="N55" s="7">
-        <f>PRODUCT(M55,C55)</f>
+        <f t="shared" si="5"/>
         <v>0.28599999999999998</v>
       </c>
       <c r="O55">
-        <f>ROUNDUP(ROUNDUP((C55*$K$65*(1+$K$66)),0)/K55,0)*K55</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P55" s="7">
-        <f>O55*M55</f>
+        <f t="shared" si="7"/>
         <v>1.7159999999999997</v>
       </c>
     </row>
@@ -3921,7 +3921,7 @@
         <v>1</v>
       </c>
       <c r="D56" s="1">
-        <f>LEN(A56)-LEN(SUBSTITUTE(A56,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E56" t="s">
@@ -3943,15 +3943,15 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="N56" s="7">
-        <f>PRODUCT(M56,C56)</f>
+        <f t="shared" si="5"/>
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="O56">
-        <f>ROUNDUP(ROUNDUP((C56*$K$65*(1+$K$66)),0)/K56,0)*K56</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="P56" s="7">
-        <f>O56*M56</f>
+        <f t="shared" si="7"/>
         <v>0.44999999999999996</v>
       </c>
     </row>
@@ -3966,7 +3966,7 @@
         <v>1</v>
       </c>
       <c r="D57" s="1">
-        <f>LEN(A57)-LEN(SUBSTITUTE(A57,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="F57" s="2" t="s">
@@ -3986,15 +3986,15 @@
         <v>1.46</v>
       </c>
       <c r="N57" s="7">
-        <f>PRODUCT(M57,C57)</f>
+        <f t="shared" si="5"/>
         <v>1.46</v>
       </c>
       <c r="O57">
-        <f>ROUNDUP(ROUNDUP((C57*$K$65*(1+$K$66)),0)/K57,0)*K57</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P57" s="7">
-        <f>O57*M57</f>
+        <f t="shared" si="7"/>
         <v>8.76</v>
       </c>
     </row>
@@ -4009,21 +4009,21 @@
         <v>1</v>
       </c>
       <c r="D58" s="1">
-        <f>LEN(A58)-LEN(SUBSTITUTE(A58,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="E58" t="s">
+        <v>231</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="G58">
         <v>1593292</v>
       </c>
       <c r="H58" s="2"/>
       <c r="J58" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="K58" s="9">
         <v>1</v>
@@ -4032,15 +4032,15 @@
         <v>8.07</v>
       </c>
       <c r="N58" s="7">
-        <f>PRODUCT(M58,C58)</f>
+        <f t="shared" si="5"/>
         <v>8.07</v>
       </c>
       <c r="O58">
-        <f>ROUNDUP(ROUNDUP((C58*$K$65*(1+$K$66)),0)/K58,0)*K58</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P58" s="7">
-        <f>O58*M58</f>
+        <f t="shared" si="7"/>
         <v>48.42</v>
       </c>
     </row>
@@ -4052,7 +4052,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="1">
-        <f>LEN(A59)-LEN(SUBSTITUTE(A59,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="F59" s="2" t="s">
@@ -4070,15 +4070,15 @@
         <v>26.3</v>
       </c>
       <c r="N59" s="7">
-        <f>PRODUCT(M59,C59)</f>
+        <f t="shared" si="5"/>
         <v>26.3</v>
       </c>
       <c r="O59">
-        <f>ROUNDUP(ROUNDUP((C59*$K$65*(1+$K$66)),0)/K59,0)*K59</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P59" s="7">
-        <f>O59*M59</f>
+        <f t="shared" si="7"/>
         <v>157.80000000000001</v>
       </c>
     </row>
@@ -4093,7 +4093,7 @@
         <v>1</v>
       </c>
       <c r="D60" s="1">
-        <f>LEN(A60)-LEN(SUBSTITUTE(A60,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="F60" s="2" t="s">
@@ -4112,21 +4112,21 @@
         <v>1.5</v>
       </c>
       <c r="N60" s="7">
-        <f>PRODUCT(M60,C60)</f>
+        <f t="shared" si="5"/>
         <v>1.5</v>
       </c>
       <c r="O60">
-        <f>ROUNDUP(ROUNDUP((C60*$K$65*(1+$K$66)),0)/K60,0)*K60</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P60" s="7">
-        <f>O60*M60</f>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>79</v>
@@ -4135,7 +4135,7 @@
         <v>4</v>
       </c>
       <c r="D61" s="1">
-        <f>LEN(A61)-LEN(SUBSTITUTE(A61,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="E61" t="s">
@@ -4155,15 +4155,15 @@
         <v>2.4100999999999999</v>
       </c>
       <c r="N61" s="7">
-        <f>PRODUCT(M61,C61)</f>
+        <f t="shared" si="5"/>
         <v>9.6403999999999996</v>
       </c>
       <c r="O61">
-        <f>ROUNDUP(ROUNDUP((C61*$K$65*(1+$K$66)),0)/K61,0)*K61</f>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="P61" s="7">
-        <f>O61*M61</f>
+        <f t="shared" si="7"/>
         <v>50.612099999999998</v>
       </c>
     </row>
@@ -4178,7 +4178,7 @@
         <v>1</v>
       </c>
       <c r="D62" s="1">
-        <f>LEN(A62)-LEN(SUBSTITUTE(A62,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="F62" s="3" t="s">
@@ -4197,21 +4197,21 @@
         <v>0.68700000000000006</v>
       </c>
       <c r="N62" s="7">
-        <f>PRODUCT(M62,C62)</f>
+        <f t="shared" si="5"/>
         <v>0.68700000000000006</v>
       </c>
       <c r="O62">
-        <f>ROUNDUP(ROUNDUP((C62*$K$65*(1+$K$66)),0)/K62,0)*K62</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P62" s="7">
-        <f>O62*M62</f>
+        <f t="shared" si="7"/>
         <v>4.1219999999999999</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>111</v>
@@ -4220,7 +4220,7 @@
         <v>1</v>
       </c>
       <c r="D63" s="1">
-        <f>LEN(A63)-LEN(SUBSTITUTE(A63,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J63" s="1" t="s">
@@ -4237,15 +4237,15 @@
         <v>9.0090000000000003E-2</v>
       </c>
       <c r="N63" s="7">
-        <f>PRODUCT(M63,C63)</f>
+        <f t="shared" si="5"/>
         <v>9.0090000000000003E-2</v>
       </c>
       <c r="O63">
-        <f>ROUNDUP(ROUNDUP((C63*$K$65*(1+$K$66)),0)/K63,0)*K63</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P63" s="7">
-        <f>O63*M63</f>
+        <f t="shared" si="7"/>
         <v>0.54054000000000002</v>
       </c>
     </row>
@@ -4260,7 +4260,7 @@
         <v>1</v>
       </c>
       <c r="D64" s="1">
-        <f>LEN(A64)-LEN(SUBSTITUTE(A64,",",""))+1</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="J64" s="1" t="s">
@@ -4277,15 +4277,15 @@
         <v>0.15400000000000003</v>
       </c>
       <c r="N64" s="7">
-        <f>PRODUCT(M64,C64)</f>
+        <f t="shared" si="5"/>
         <v>0.15400000000000003</v>
       </c>
       <c r="O64">
-        <f>ROUNDUP(ROUNDUP((C64*$K$65*(1+$K$66)),0)/K64,0)*K64</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="P64" s="7">
-        <f>O64*M64</f>
+        <f t="shared" si="7"/>
         <v>0.92400000000000015</v>
       </c>
     </row>
@@ -4301,14 +4301,14 @@
       </c>
       <c r="N65" s="7">
         <f>SUM(N2:N62)</f>
-        <v>118.48886999999999</v>
+        <v>118.67026999999999</v>
       </c>
       <c r="O65" s="5" t="s">
         <v>154</v>
       </c>
       <c r="P65" s="7">
         <f>SUM(P2:P64)</f>
-        <v>698.57209999999998</v>
+        <v>699.4790999999999</v>
       </c>
     </row>
     <row r="66" spans="7:18" x14ac:dyDescent="0.25">

</xml_diff>